<commit_message>
Changed chart types in charts sheet to be a combination of a line and bar chart for better readability
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Data\ERC721 Implementation Comparisons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15C94B0-92E4-4F2D-B937-03A75AAC3DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A442F04A-D4A3-4352-9322-20304567733F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="5" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -1220,8 +1220,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1238,23 +1239,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
+              <a:glow rad="63500">
                 <a:schemeClr val="accent1">
                   <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
+                  <a:alpha val="25000"/>
                 </a:schemeClr>
               </a:glow>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'Optimizer | 200 run - Descended'!$P$3:$P$23</c:f>
@@ -1399,13 +1400,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8D4D-4864-AB01-44FA1389F316}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="637921528"/>
+        <c:axId val="637923128"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -1590,7 +1605,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1598,6 +1612,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="637921528"/>
         <c:axId val="637923128"/>
@@ -1955,8 +1970,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1973,23 +1989,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
+              <a:glow rad="63500">
                 <a:schemeClr val="accent1">
                   <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
+                  <a:alpha val="25000"/>
                 </a:schemeClr>
               </a:glow>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$21</c:f>
@@ -2122,13 +2138,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-4D61-4D6C-A35F-22F0B8FEA905}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="587459576"/>
+        <c:axId val="587460536"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -2308,6 +2338,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="587459576"/>
         <c:axId val="587460536"/>
@@ -2670,8 +2701,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2688,23 +2720,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
+              <a:glow rad="63500">
                 <a:schemeClr val="accent1">
                   <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
+                  <a:alpha val="25000"/>
                 </a:schemeClr>
               </a:glow>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'Optimizer | 1000 run - Descend'!$P$3:$P$23</c:f>
@@ -2849,13 +2881,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-D492-4D35-89E6-337FBC1CEFBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="637937208"/>
+        <c:axId val="637935288"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -3047,6 +3093,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="637937208"/>
         <c:axId val="637935288"/>
@@ -7017,8 +7064,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -7035,23 +7083,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
+              <a:glow rad="63500">
                 <a:schemeClr val="accent1">
                   <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
+                  <a:alpha val="25000"/>
                 </a:schemeClr>
               </a:glow>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'Optimizer Disabled - Ascended'!$P$3:$P$23</c:f>
@@ -7196,13 +7244,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-846E-4AB4-AB50-E86F453C6007}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="637928568"/>
+        <c:axId val="637933688"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -7394,6 +7456,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="637928568"/>
         <c:axId val="637933688"/>
@@ -7749,8 +7812,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -7767,23 +7831,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
+              <a:glow rad="63500">
                 <a:schemeClr val="accent1">
                   <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
+                  <a:alpha val="25000"/>
                 </a:schemeClr>
               </a:glow>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'Optimizer Disabled - Descended'!$P$3:$P$23</c:f>
@@ -7928,13 +7992,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-37F4-49D4-A6A4-ABE6CC6D42BC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="587433336"/>
+        <c:axId val="587436536"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -8126,6 +8204,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="587433336"/>
         <c:axId val="587436536"/>
@@ -8483,8 +8562,9 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -8501,23 +8581,23 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
+              <a:glow rad="63500">
                 <a:schemeClr val="accent1">
                   <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
+                  <a:alpha val="25000"/>
                 </a:schemeClr>
               </a:glow>
             </a:effectLst>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
               <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$21</c:f>
@@ -8650,13 +8730,27 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-E5D6-4144-9458-2B5BF39DE2BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="587470456"/>
+        <c:axId val="587471096"/>
+      </c:barChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
@@ -8836,6 +8930,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="587470456"/>
         <c:axId val="587471096"/>
@@ -19204,11 +19299,11 @@
         <v>10</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
+        <f t="shared" ref="Q4:Q21" si="2">C4+D4</f>
         <v>649471</v>
       </c>
       <c r="R4" s="4">
-        <f t="shared" ref="R4:R23" si="3">H4+I4</f>
+        <f t="shared" ref="R4:R21" si="3">H4+I4</f>
         <v>2782683</v>
       </c>
     </row>
@@ -21232,11 +21327,11 @@
         <v>10</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
+        <f t="shared" ref="Q4:Q21" si="2">C4+D4</f>
         <v>649427</v>
       </c>
       <c r="R4" s="4">
-        <f t="shared" ref="R4:R23" si="3">H4+I4</f>
+        <f t="shared" ref="R4:R21" si="3">H4+I4</f>
         <v>2781243</v>
       </c>
     </row>
@@ -22076,7 +22171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
@@ -23128,8 +23223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91734A6-3CBC-46E0-AC2D-961E5CB62031}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update optimizer 200 runs data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34849B30-4E4B-43D3-B3B9-3235E077DBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4BD4AD-283A-41E2-9BF1-C4C4F5E11193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -1155,40 +1155,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -1215,67 +1215,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604353</c:v>
+                  <c:v>604286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1217514</c:v>
+                  <c:v>1209869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1907259</c:v>
+                  <c:v>1876469</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2605904</c:v>
+                  <c:v>2536469</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3171228</c:v>
+                  <c:v>3189869</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3242294</c:v>
+                  <c:v>3254846</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3313449</c:v>
+                  <c:v>3319757</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3384693</c:v>
+                  <c:v>3384602</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3456026</c:v>
+                  <c:v>3449381</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3527448</c:v>
+                  <c:v>3514094</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3598959</c:v>
+                  <c:v>3578741</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3670559</c:v>
+                  <c:v>3643322</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3742248</c:v>
+                  <c:v>3707837</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3814026</c:v>
+                  <c:v>3772286</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3885893</c:v>
+                  <c:v>3836669</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4029894</c:v>
+                  <c:v>3900986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4755239</c:v>
+                  <c:v>4476869</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5489484</c:v>
+                  <c:v>5110469</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6232629</c:v>
+                  <c:v>5737469</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6984674</c:v>
+                  <c:v>6357869</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7728053</c:v>
+                  <c:v>6954345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,40 +1352,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -1412,67 +1412,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2645357</c:v>
+                  <c:v>2645338</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2783210</c:v>
+                  <c:v>2782165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2966875</c:v>
+                  <c:v>2962885</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3182640</c:v>
+                  <c:v>3173805</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3378364</c:v>
+                  <c:v>3414925</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3404274</c:v>
+                  <c:v>3440698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3430505</c:v>
+                  <c:v>3466773</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3457057</c:v>
+                  <c:v>3493150</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3483930</c:v>
+                  <c:v>3519829</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3511124</c:v>
+                  <c:v>3546810</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3538639</c:v>
+                  <c:v>3574093</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3566475</c:v>
+                  <c:v>3601678</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3594632</c:v>
+                  <c:v>3629565</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3623110</c:v>
+                  <c:v>3657754</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3651909</c:v>
+                  <c:v>3686245</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3710470</c:v>
+                  <c:v>3715038</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4022535</c:v>
+                  <c:v>3987765</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4366700</c:v>
+                  <c:v>4319485</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4742965</c:v>
+                  <c:v>4681405</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5151330</c:v>
+                  <c:v>5073525</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5586713</c:v>
+                  <c:v>5491045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4095,10 +4095,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4130,30 +4130,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -4161,66 +4137,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>368032</c:v>
+                  <c:v>367760</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>649471</c:v>
+                  <c:v>640631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1010441</c:v>
+                  <c:v>979161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1422211</c:v>
+                  <c:v>1354891</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1884781</c:v>
+                  <c:v>1767821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2398151</c:v>
+                  <c:v>2217951</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2962321</c:v>
+                  <c:v>2705281</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3577291</c:v>
+                  <c:v>3229811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4243061</c:v>
+                  <c:v>3791541</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4959631</c:v>
+                  <c:v>4390471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5109041</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5184508</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5260483</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5336966</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5413957</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5491456</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5569463</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5647978</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5706926</c:v>
+                  <c:v>5006526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4266,10 +4218,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4301,30 +4253,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -4332,10 +4260,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2645289</c:v>
                 </c:pt>
@@ -4367,30 +4295,6 @@
                   <c:v>5157403</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5243339</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5286793</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5330571</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5374673</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5419099</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5463849</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5508923</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5554321</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>5595243</c:v>
                 </c:pt>
               </c:numCache>
@@ -4822,40 +4726,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -4882,67 +4786,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604353</c:v>
+                  <c:v>604286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1217514</c:v>
+                  <c:v>1209869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1907259</c:v>
+                  <c:v>1876469</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2605904</c:v>
+                  <c:v>2536469</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3171228</c:v>
+                  <c:v>3189869</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3242294</c:v>
+                  <c:v>3254846</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3313449</c:v>
+                  <c:v>3319757</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3384693</c:v>
+                  <c:v>3384602</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3456026</c:v>
+                  <c:v>3449381</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3527448</c:v>
+                  <c:v>3514094</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3598959</c:v>
+                  <c:v>3578741</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3670559</c:v>
+                  <c:v>3643322</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3742248</c:v>
+                  <c:v>3707837</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3814026</c:v>
+                  <c:v>3772286</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3885893</c:v>
+                  <c:v>3836669</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4029894</c:v>
+                  <c:v>3900986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4755239</c:v>
+                  <c:v>4476869</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5489484</c:v>
+                  <c:v>5110469</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6232629</c:v>
+                  <c:v>5737469</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6984674</c:v>
+                  <c:v>6357869</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7728053</c:v>
+                  <c:v>6954345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5005,40 +4909,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -5065,67 +4969,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2645357</c:v>
+                  <c:v>2645338</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2783210</c:v>
+                  <c:v>2782165</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2966875</c:v>
+                  <c:v>2962885</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3182640</c:v>
+                  <c:v>3173805</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3378364</c:v>
+                  <c:v>3414925</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3404274</c:v>
+                  <c:v>3440698</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3430505</c:v>
+                  <c:v>3466773</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3457057</c:v>
+                  <c:v>3493150</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3483930</c:v>
+                  <c:v>3519829</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3511124</c:v>
+                  <c:v>3546810</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3538639</c:v>
+                  <c:v>3574093</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3566475</c:v>
+                  <c:v>3601678</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3594632</c:v>
+                  <c:v>3629565</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3623110</c:v>
+                  <c:v>3657754</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3651909</c:v>
+                  <c:v>3686245</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3710470</c:v>
+                  <c:v>3715038</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4022535</c:v>
+                  <c:v>3987765</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4366700</c:v>
+                  <c:v>4319485</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4742965</c:v>
+                  <c:v>4681405</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5151330</c:v>
+                  <c:v>5073525</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5586713</c:v>
+                  <c:v>5491045</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8360,10 +8264,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -8395,30 +8299,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -8426,66 +8306,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>368032</c:v>
+                  <c:v>367760</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>649471</c:v>
+                  <c:v>640631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1010441</c:v>
+                  <c:v>979161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1422211</c:v>
+                  <c:v>1354891</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1884781</c:v>
+                  <c:v>1767821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2398151</c:v>
+                  <c:v>2217951</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2962321</c:v>
+                  <c:v>2705281</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3577291</c:v>
+                  <c:v>3229811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4243061</c:v>
+                  <c:v>3791541</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4959631</c:v>
+                  <c:v>4390471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5109041</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5184508</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5260483</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5336966</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5413957</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5491456</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5569463</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5647978</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5706926</c:v>
+                  <c:v>5006526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8545,10 +8401,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -8580,30 +8436,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -8611,10 +8443,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$21</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2645289</c:v>
                 </c:pt>
@@ -8646,30 +8478,6 @@
                   <c:v>5157403</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5243339</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5286793</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5330571</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5374673</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5419099</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5463849</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5508923</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5554321</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>5595243</c:v>
                 </c:pt>
               </c:numCache>
@@ -16180,7 +15988,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>19500</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>431100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -17408,8 +17216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1DA2FE-2DBA-48DD-9085-CD8066E7E300}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18458,10 +18266,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F68343B-F0B9-4DF5-8EBB-C222891744B9}">
-  <dimension ref="A2:R23"/>
+  <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18512,11 +18320,11 @@
         <v>281777</v>
       </c>
       <c r="D3" s="4">
-        <v>86255</v>
+        <v>85983</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>368032</v>
+        <v>367760</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -18533,14 +18341,14 @@
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2277257</v>
+        <v>-2277529</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>368032</v>
+        <v>367760</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
@@ -18555,11 +18363,11 @@
         <v>281777</v>
       </c>
       <c r="D4" s="4">
-        <v>367694</v>
+        <v>358854</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E21" si="0">C4+D4</f>
-        <v>649471</v>
+        <f t="shared" ref="E4:E13" si="0">C4+D4</f>
+        <v>640631</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -18575,22 +18383,22 @@
         <v>2782683</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L21" si="1">E4-J4</f>
-        <v>-2133212</v>
+        <f t="shared" ref="L4:L13" si="1">E4-J4</f>
+        <v>-2142052</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>144045</v>
+        <v>135477</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q21" si="2">C4+D4</f>
-        <v>649471</v>
+        <f t="shared" ref="Q4:Q13" si="2">C4+D4</f>
+        <v>640631</v>
       </c>
       <c r="R4" s="4">
-        <f t="shared" ref="R4:R21" si="3">H4+I4</f>
+        <f t="shared" ref="R4:R13" si="3">H4+I4</f>
         <v>2782683</v>
       </c>
     </row>
@@ -18602,11 +18410,11 @@
         <v>281777</v>
       </c>
       <c r="D5" s="4">
-        <v>728664</v>
+        <v>697384</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1010441</v>
+        <v>979161</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -18618,23 +18426,23 @@
         <v>385204</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J20" si="4">H5+I5</f>
+        <f t="shared" ref="J5:J12" si="4">H5+I5</f>
         <v>2966123</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1955682</v>
+        <v>-1986962</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>177530</v>
+        <v>155090</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>1010441</v>
+        <v>979161</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
@@ -18649,11 +18457,11 @@
         <v>281777</v>
       </c>
       <c r="D6" s="4">
-        <v>1140434</v>
+        <v>1073114</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1422211</v>
+        <v>1354891</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -18670,18 +18478,18 @@
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-1759752</v>
+        <v>-1827072</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>195930</v>
+        <v>159890</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>1422211</v>
+        <v>1354891</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
@@ -18696,11 +18504,11 @@
         <v>281777</v>
       </c>
       <c r="D7" s="4">
-        <v>1603004</v>
+        <v>1486044</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1884781</v>
+        <v>1767821</v>
       </c>
       <c r="G7" s="2">
         <v>40</v>
@@ -18717,18 +18525,18 @@
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>-1545422</v>
+        <v>-1662382</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>214330</v>
+        <v>164690</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>1884781</v>
+        <v>1767821</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
@@ -18743,11 +18551,11 @@
         <v>281777</v>
       </c>
       <c r="D8" s="4">
-        <v>2116374</v>
+        <v>1936174</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2398151</v>
+        <v>2217951</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
@@ -18764,18 +18572,18 @@
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-1312692</v>
+        <v>-1492892</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>232730</v>
+        <v>169490</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>2398151</v>
+        <v>2217951</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
@@ -18790,11 +18598,11 @@
         <v>281777</v>
       </c>
       <c r="D9" s="4">
-        <v>2680544</v>
+        <v>2423504</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2962321</v>
+        <v>2705281</v>
       </c>
       <c r="G9" s="2">
         <v>60</v>
@@ -18811,18 +18619,18 @@
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>-1061562</v>
+        <v>-1318602</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>251130</v>
+        <v>174290</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>2962321</v>
+        <v>2705281</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
@@ -18837,11 +18645,11 @@
         <v>281777</v>
       </c>
       <c r="D10" s="4">
-        <v>3295514</v>
+        <v>2948034</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3577291</v>
+        <v>3229811</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
@@ -18858,18 +18666,18 @@
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>-792032</v>
+        <v>-1139512</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>269530</v>
+        <v>179090</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3577291</v>
+        <v>3229811</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
@@ -18884,11 +18692,11 @@
         <v>281777</v>
       </c>
       <c r="D11" s="4">
-        <v>3961284</v>
+        <v>3509764</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>4243061</v>
+        <v>3791541</v>
       </c>
       <c r="G11" s="2">
         <v>80</v>
@@ -18905,18 +18713,18 @@
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>-504102</v>
+        <v>-955622</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>287930</v>
+        <v>183890</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>4243061</v>
+        <v>3791541</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
@@ -18931,11 +18739,11 @@
         <v>281777</v>
       </c>
       <c r="D12" s="4">
-        <v>4677854</v>
+        <v>4108694</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>4959631</v>
+        <v>4390471</v>
       </c>
       <c r="G12" s="2">
         <v>90</v>
@@ -18952,18 +18760,18 @@
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>-197772</v>
+        <v>-766932</v>
       </c>
       <c r="M12" s="5">
         <f>L12-L11</f>
-        <v>306330</v>
+        <v>188690</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>4959631</v>
+        <v>4390471</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
@@ -18972,450 +18780,65 @@
     </row>
     <row r="13" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C13" s="4">
         <v>281777</v>
       </c>
       <c r="D13" s="4">
-        <v>4827264</v>
+        <v>4724749</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>5109041</v>
+        <v>5006526</v>
       </c>
       <c r="G13" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H13" s="4">
         <v>2580919</v>
       </c>
       <c r="I13" s="4">
-        <v>2662420</v>
+        <v>3014324</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="4"/>
-        <v>5243339</v>
+        <f t="shared" ref="J13" si="6">H13+I13</f>
+        <v>5595243</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" ref="L13:L16" si="6">E13-J13</f>
-        <v>-134298</v>
+        <f t="shared" si="1"/>
+        <v>-588717</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" ref="M13:M17" si="7">L13-L12</f>
-        <v>63474</v>
+        <f>L13-L12</f>
+        <v>178215</v>
       </c>
       <c r="P13" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>5109041</v>
+        <v>5006526</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>5243339</v>
+        <v>5595243</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>93</v>
-      </c>
-      <c r="C14" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D14" s="4">
-        <v>4902731</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>5184508</v>
-      </c>
-      <c r="G14" s="2">
-        <v>93</v>
-      </c>
-      <c r="H14" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I14" s="4">
-        <v>2705874</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="4"/>
-        <v>5286793</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="6"/>
-        <v>-102285</v>
-      </c>
-      <c r="M14" s="5">
-        <f t="shared" si="7"/>
-        <v>32013</v>
-      </c>
-      <c r="P14" s="2">
-        <v>93</v>
-      </c>
-      <c r="Q14" s="4">
-        <f t="shared" si="2"/>
-        <v>5184508</v>
-      </c>
-      <c r="R14" s="4">
-        <f t="shared" si="3"/>
-        <v>5286793</v>
-      </c>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
     </row>
     <row r="15" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>94</v>
-      </c>
-      <c r="C15" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D15" s="4">
-        <v>4978706</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>5260483</v>
-      </c>
-      <c r="G15" s="2">
-        <v>94</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2749652</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="4"/>
-        <v>5330571</v>
-      </c>
-      <c r="L15" s="4">
-        <f t="shared" si="6"/>
-        <v>-70088</v>
-      </c>
-      <c r="M15" s="5">
-        <f t="shared" si="7"/>
-        <v>32197</v>
-      </c>
-      <c r="P15" s="2">
-        <v>94</v>
-      </c>
-      <c r="Q15" s="4">
-        <f t="shared" si="2"/>
-        <v>5260483</v>
-      </c>
-      <c r="R15" s="4">
-        <f t="shared" si="3"/>
-        <v>5330571</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>95</v>
-      </c>
-      <c r="C16" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D16" s="4">
-        <v>5055189</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>5336966</v>
-      </c>
-      <c r="G16" s="2">
-        <v>95</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I16" s="4">
-        <v>2793754</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="4"/>
-        <v>5374673</v>
-      </c>
-      <c r="L16" s="4">
-        <f t="shared" si="6"/>
-        <v>-37707</v>
-      </c>
-      <c r="M16" s="5">
-        <f t="shared" si="7"/>
-        <v>32381</v>
-      </c>
-      <c r="P16" s="2">
-        <v>95</v>
-      </c>
-      <c r="Q16" s="4">
-        <f t="shared" si="2"/>
-        <v>5336966</v>
-      </c>
-      <c r="R16" s="4">
-        <f t="shared" si="3"/>
-        <v>5374673</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>96</v>
-      </c>
-      <c r="C17" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D17" s="4">
-        <v>5132180</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>5413957</v>
-      </c>
-      <c r="G17" s="2">
-        <v>96</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I17" s="4">
-        <v>2838180</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="4"/>
-        <v>5419099</v>
-      </c>
-      <c r="L17" s="4">
-        <f t="shared" si="1"/>
-        <v>-5142</v>
-      </c>
-      <c r="M17" s="5">
-        <f t="shared" si="7"/>
-        <v>32565</v>
-      </c>
-      <c r="P17" s="2">
-        <v>96</v>
-      </c>
-      <c r="Q17" s="4">
-        <f t="shared" si="2"/>
-        <v>5413957</v>
-      </c>
-      <c r="R17" s="4">
-        <f t="shared" si="3"/>
-        <v>5419099</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="2">
-        <v>97</v>
-      </c>
-      <c r="C18" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D18" s="4">
-        <v>5209679</v>
-      </c>
-      <c r="E18" s="4">
-        <f t="shared" si="0"/>
-        <v>5491456</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="2">
-        <v>97</v>
-      </c>
-      <c r="H18" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I18" s="4">
-        <v>2882930</v>
-      </c>
-      <c r="J18" s="4">
-        <f t="shared" si="4"/>
-        <v>5463849</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="4">
-        <f t="shared" ref="L18" si="8">E18-J18</f>
-        <v>27607</v>
-      </c>
-      <c r="M18" s="5">
-        <f>L18-L17</f>
-        <v>32749</v>
-      </c>
-      <c r="P18" s="2">
-        <v>97</v>
-      </c>
-      <c r="Q18" s="4">
-        <f t="shared" si="2"/>
-        <v>5491456</v>
-      </c>
-      <c r="R18" s="4">
-        <f t="shared" si="3"/>
-        <v>5463849</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19"/>
-      <c r="B19" s="2">
-        <v>98</v>
-      </c>
-      <c r="C19" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D19" s="4">
-        <v>5287686</v>
-      </c>
-      <c r="E19" s="4">
-        <f t="shared" si="0"/>
-        <v>5569463</v>
-      </c>
-      <c r="F19"/>
-      <c r="G19" s="2">
-        <v>98</v>
-      </c>
-      <c r="H19" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I19" s="4">
-        <v>2928004</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="4"/>
-        <v>5508923</v>
-      </c>
-      <c r="K19"/>
-      <c r="L19" s="4">
-        <f t="shared" ref="L19:L20" si="9">E19-J19</f>
-        <v>60540</v>
-      </c>
-      <c r="M19" s="5">
-        <f t="shared" ref="M19:M20" si="10">L19-L18</f>
-        <v>32933</v>
-      </c>
-      <c r="P19" s="2">
-        <v>98</v>
-      </c>
-      <c r="Q19" s="4">
-        <f t="shared" si="2"/>
-        <v>5569463</v>
-      </c>
-      <c r="R19" s="4">
-        <f t="shared" si="3"/>
-        <v>5508923</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20"/>
-      <c r="B20" s="2">
-        <v>99</v>
-      </c>
-      <c r="C20" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D20" s="4">
-        <v>5366201</v>
-      </c>
-      <c r="E20" s="4">
-        <f t="shared" si="0"/>
-        <v>5647978</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20" s="2">
-        <v>99</v>
-      </c>
-      <c r="H20" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I20" s="4">
-        <v>2973402</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" si="4"/>
-        <v>5554321</v>
-      </c>
-      <c r="K20"/>
-      <c r="L20" s="4">
-        <f t="shared" si="9"/>
-        <v>93657</v>
-      </c>
-      <c r="M20" s="5">
-        <f t="shared" si="10"/>
-        <v>33117</v>
-      </c>
-      <c r="P20" s="2">
-        <v>99</v>
-      </c>
-      <c r="Q20" s="4">
-        <f t="shared" si="2"/>
-        <v>5647978</v>
-      </c>
-      <c r="R20" s="4">
-        <f t="shared" si="3"/>
-        <v>5554321</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <v>100</v>
-      </c>
-      <c r="C21" s="4">
-        <v>281777</v>
-      </c>
-      <c r="D21" s="4">
-        <v>5425149</v>
-      </c>
-      <c r="E21" s="4">
-        <f t="shared" si="0"/>
-        <v>5706926</v>
-      </c>
-      <c r="G21" s="2">
-        <v>100</v>
-      </c>
-      <c r="H21" s="4">
-        <v>2580919</v>
-      </c>
-      <c r="I21" s="4">
-        <v>3014324</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" ref="J21" si="11">H21+I21</f>
-        <v>5595243</v>
-      </c>
-      <c r="L21" s="4">
-        <f t="shared" si="1"/>
-        <v>111683</v>
-      </c>
-      <c r="M21" s="5">
-        <f>L21-L12</f>
-        <v>309455</v>
-      </c>
-      <c r="P21" s="2">
-        <v>100</v>
-      </c>
-      <c r="Q21" s="4">
-        <f t="shared" si="2"/>
-        <v>5706926</v>
-      </c>
-      <c r="R21" s="4">
-        <f t="shared" si="3"/>
-        <v>5595243</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-    </row>
-    <row r="23" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L3:L21">
+  <conditionalFormatting sqref="L3:L13">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -19437,7 +18860,7 @@
   <dimension ref="A2:R23"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19488,11 +18911,11 @@
         <v>281777</v>
       </c>
       <c r="D3" s="4">
-        <v>322576</v>
+        <v>322509</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>604353</v>
+        <v>604286</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -19501,26 +18924,26 @@
         <v>2580919</v>
       </c>
       <c r="I3" s="4">
-        <v>64438</v>
+        <v>64419</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2645357</v>
+        <v>2645338</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2041004</v>
+        <v>-2041052</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>604353</v>
+        <v>604286</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2645357</v>
+        <v>2645338</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19531,11 +18954,11 @@
         <v>281777</v>
       </c>
       <c r="D4" s="4">
-        <v>935737</v>
+        <v>928092</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E23" si="0">C4+D4</f>
-        <v>1217514</v>
+        <v>1209869</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -19544,30 +18967,30 @@
         <v>2580919</v>
       </c>
       <c r="I4" s="4">
-        <v>202291</v>
+        <v>201246</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2783210</v>
+        <v>2782165</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>-1565696</v>
+        <v>-1572296</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>475308</v>
+        <v>468756</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
-        <v>1217514</v>
+        <v>1209869</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>2783210</v>
+        <v>2782165</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19578,11 +19001,11 @@
         <v>281777</v>
       </c>
       <c r="D5" s="4">
-        <v>1625482</v>
+        <v>1594692</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1907259</v>
+        <v>1876469</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -19591,30 +19014,30 @@
         <v>2580919</v>
       </c>
       <c r="I5" s="4">
-        <v>385956</v>
+        <v>381966</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J23" si="4">H5+I5</f>
-        <v>2966875</v>
+        <f>H5+I5</f>
+        <v>2962885</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1059616</v>
+        <v>-1086416</v>
       </c>
       <c r="M5" s="5">
-        <f t="shared" ref="M5:M23" si="5">L5-L4</f>
-        <v>506080</v>
+        <f t="shared" ref="M5:M23" si="4">L5-L4</f>
+        <v>485880</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>1907259</v>
+        <v>1876469</v>
       </c>
       <c r="R5" s="4">
-        <f t="shared" si="3"/>
-        <v>2966875</v>
+        <f>H5+I5</f>
+        <v>2962885</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19625,11 +19048,11 @@
         <v>281777</v>
       </c>
       <c r="D6" s="4">
-        <v>2324127</v>
+        <v>2254692</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2605904</v>
+        <v>2536469</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -19638,597 +19061,597 @@
         <v>2580919</v>
       </c>
       <c r="I6" s="4">
-        <v>601721</v>
+        <v>592886</v>
       </c>
       <c r="J6" s="4">
-        <f t="shared" si="4"/>
-        <v>3182640</v>
+        <f t="shared" ref="J6:J23" si="5">H6+I6</f>
+        <v>3173805</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-576736</v>
+        <v>-637336</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>482880</v>
+        <v>449080</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>2605904</v>
+        <v>2536469</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3182640</v>
+        <v>3173805</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4">
         <v>281777</v>
       </c>
       <c r="D7" s="4">
-        <v>2889451</v>
+        <v>2908092</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>3171228</v>
+        <v>3189869</v>
       </c>
       <c r="G7" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H7" s="4">
         <v>2580919</v>
       </c>
       <c r="I7" s="4">
-        <v>797445</v>
+        <v>834006</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="4"/>
-        <v>3378364</v>
+        <f t="shared" si="5"/>
+        <v>3414925</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7:L17" si="6">E7-J7</f>
-        <v>-207136</v>
+        <f t="shared" ref="L7:L8" si="6">E7-J7</f>
+        <v>-225056</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" ref="M7:M18" si="7">L7-L6</f>
-        <v>369600</v>
+        <f>L7-L6</f>
+        <v>412280</v>
       </c>
       <c r="P7" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>3171228</v>
+        <v>3189869</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
-        <v>3378364</v>
+        <v>3414925</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4">
         <v>281777</v>
       </c>
       <c r="D8" s="4">
-        <v>2960517</v>
+        <v>2973069</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3242294</v>
+        <v>3254846</v>
       </c>
       <c r="G8" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H8" s="4">
         <v>2580919</v>
       </c>
       <c r="I8" s="4">
-        <v>823355</v>
+        <v>859779</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="4"/>
-        <v>3404274</v>
+        <f t="shared" si="5"/>
+        <v>3440698</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="6"/>
-        <v>-161980</v>
+        <v>-185852</v>
       </c>
       <c r="M8" s="5">
-        <f t="shared" si="7"/>
-        <v>45156</v>
+        <f>L8-L7</f>
+        <v>39204</v>
       </c>
       <c r="P8" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>3242294</v>
+        <v>3254846</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>3404274</v>
+        <v>3440698</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4">
         <v>281777</v>
       </c>
       <c r="D9" s="4">
-        <v>3031672</v>
+        <v>3037980</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3313449</v>
+        <v>3319757</v>
       </c>
       <c r="G9" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H9" s="4">
         <v>2580919</v>
       </c>
       <c r="I9" s="4">
-        <v>849586</v>
+        <v>885854</v>
       </c>
       <c r="J9" s="4">
-        <f t="shared" si="4"/>
-        <v>3430505</v>
+        <f t="shared" si="5"/>
+        <v>3466773</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="6"/>
-        <v>-117056</v>
+        <f t="shared" ref="L7:L15" si="7">E9-J9</f>
+        <v>-147016</v>
       </c>
       <c r="M9" s="5">
-        <f t="shared" si="7"/>
-        <v>44924</v>
+        <f t="shared" ref="M8:M15" si="8">L9-L8</f>
+        <v>38836</v>
       </c>
       <c r="P9" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>3313449</v>
+        <v>3319757</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>3430505</v>
+        <v>3466773</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4">
         <v>281777</v>
       </c>
       <c r="D10" s="4">
-        <v>3102916</v>
+        <v>3102825</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3384693</v>
+        <v>3384602</v>
       </c>
       <c r="G10" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H10" s="4">
         <v>2580919</v>
       </c>
       <c r="I10" s="4">
-        <v>876138</v>
+        <v>912231</v>
       </c>
       <c r="J10" s="4">
-        <f t="shared" si="4"/>
-        <v>3457057</v>
+        <f t="shared" si="5"/>
+        <v>3493150</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="6"/>
-        <v>-72364</v>
+        <f t="shared" si="7"/>
+        <v>-108548</v>
       </c>
       <c r="M10" s="5">
-        <f t="shared" si="7"/>
-        <v>44692</v>
+        <f t="shared" si="8"/>
+        <v>38468</v>
       </c>
       <c r="P10" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3384693</v>
+        <v>3384602</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>3457057</v>
+        <v>3493150</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
         <v>281777</v>
       </c>
       <c r="D11" s="4">
-        <v>3174249</v>
+        <v>3167604</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3456026</v>
+        <v>3449381</v>
       </c>
       <c r="G11" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H11" s="4">
         <v>2580919</v>
       </c>
       <c r="I11" s="4">
-        <v>903011</v>
+        <v>938910</v>
       </c>
       <c r="J11" s="4">
-        <f t="shared" si="4"/>
-        <v>3483930</v>
+        <f t="shared" si="5"/>
+        <v>3519829</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="6"/>
-        <v>-27904</v>
+        <f t="shared" si="7"/>
+        <v>-70448</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" si="7"/>
-        <v>44460</v>
+        <f t="shared" si="8"/>
+        <v>38100</v>
       </c>
       <c r="P11" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3456026</v>
+        <v>3449381</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>3483930</v>
+        <v>3519829</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
       <c r="B12" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4">
         <v>281777</v>
       </c>
       <c r="D12" s="4">
-        <v>3245671</v>
+        <v>3232317</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3527448</v>
-      </c>
-      <c r="F12" s="6"/>
+        <v>3514094</v>
+      </c>
       <c r="G12" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H12" s="4">
         <v>2580919</v>
       </c>
       <c r="I12" s="4">
-        <v>930205</v>
+        <v>965891</v>
       </c>
       <c r="J12" s="4">
-        <f t="shared" si="4"/>
-        <v>3511124</v>
-      </c>
-      <c r="K12" s="6"/>
+        <f t="shared" si="5"/>
+        <v>3546810</v>
+      </c>
       <c r="L12" s="4">
-        <f t="shared" si="6"/>
-        <v>16324</v>
+        <f t="shared" si="7"/>
+        <v>-32716</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" si="7"/>
-        <v>44228</v>
+        <f t="shared" si="8"/>
+        <v>37732</v>
       </c>
       <c r="P12" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>3527448</v>
+        <v>3514094</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>3511124</v>
+        <v>3546810</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
       <c r="B13" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4">
         <v>281777</v>
       </c>
       <c r="D13" s="4">
-        <v>3317182</v>
+        <v>3296964</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>3598959</v>
-      </c>
+        <v>3578741</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="G13" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H13" s="4">
         <v>2580919</v>
       </c>
       <c r="I13" s="4">
-        <v>957720</v>
+        <v>993174</v>
       </c>
       <c r="J13" s="4">
-        <f t="shared" si="4"/>
-        <v>3538639</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>3574093</v>
+      </c>
+      <c r="K13" s="6"/>
       <c r="L13" s="4">
-        <f t="shared" si="6"/>
-        <v>60320</v>
+        <f t="shared" si="7"/>
+        <v>4648</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" si="7"/>
-        <v>43996</v>
+        <f t="shared" si="8"/>
+        <v>37364</v>
       </c>
       <c r="P13" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>3598959</v>
+        <v>3578741</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>3538639</v>
+        <v>3574093</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4">
         <v>281777</v>
       </c>
       <c r="D14" s="4">
-        <v>3388782</v>
+        <v>3361545</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3670559</v>
+        <v>3643322</v>
       </c>
       <c r="G14" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H14" s="4">
         <v>2580919</v>
       </c>
       <c r="I14" s="4">
-        <v>985556</v>
+        <v>1020759</v>
       </c>
       <c r="J14" s="4">
-        <f t="shared" si="4"/>
-        <v>3566475</v>
+        <f t="shared" si="5"/>
+        <v>3601678</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" si="6"/>
-        <v>104084</v>
+        <f t="shared" si="7"/>
+        <v>41644</v>
       </c>
       <c r="M14" s="5">
-        <f t="shared" si="7"/>
-        <v>43764</v>
+        <f t="shared" si="8"/>
+        <v>36996</v>
       </c>
       <c r="P14" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>3670559</v>
+        <v>3643322</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>3566475</v>
+        <v>3601678</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4">
         <v>281777</v>
       </c>
       <c r="D15" s="4">
-        <v>3460471</v>
+        <v>3426060</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>3742248</v>
+        <v>3707837</v>
       </c>
       <c r="G15" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H15" s="4">
         <v>2580919</v>
       </c>
       <c r="I15" s="4">
-        <v>1013713</v>
+        <v>1048646</v>
       </c>
       <c r="J15" s="4">
-        <f t="shared" si="4"/>
-        <v>3594632</v>
+        <f t="shared" si="5"/>
+        <v>3629565</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" si="6"/>
-        <v>147616</v>
+        <f t="shared" si="7"/>
+        <v>78272</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" si="7"/>
-        <v>43532</v>
+        <f t="shared" si="8"/>
+        <v>36628</v>
       </c>
       <c r="P15" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>3742248</v>
+        <v>3707837</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>3594632</v>
+        <v>3629565</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" s="4">
         <v>281777</v>
       </c>
       <c r="D16" s="4">
-        <v>3532249</v>
+        <v>3490509</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>3814026</v>
+        <v>3772286</v>
       </c>
       <c r="G16" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H16" s="4">
         <v>2580919</v>
       </c>
       <c r="I16" s="4">
-        <v>1042191</v>
+        <v>1076835</v>
       </c>
       <c r="J16" s="4">
-        <f t="shared" si="4"/>
-        <v>3623110</v>
+        <f t="shared" si="5"/>
+        <v>3657754</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="6"/>
-        <v>190916</v>
+        <f t="shared" ref="L16:L17" si="9">E16-J16</f>
+        <v>114532</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" si="7"/>
-        <v>43300</v>
+        <f t="shared" ref="M16:M17" si="10">L16-L15</f>
+        <v>36260</v>
       </c>
       <c r="P16" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="Q16" s="4">
-        <f t="shared" si="2"/>
-        <v>3814026</v>
+        <f t="shared" ref="Q16" si="11">C16+D16</f>
+        <v>3772286</v>
       </c>
       <c r="R16" s="4">
-        <f t="shared" si="3"/>
-        <v>3623110</v>
+        <f t="shared" ref="R16" si="12">H16+I16</f>
+        <v>3657754</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C17" s="4">
         <v>281777</v>
       </c>
       <c r="D17" s="4">
-        <v>3604116</v>
+        <v>3554892</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>3885893</v>
+        <v>3836669</v>
       </c>
       <c r="G17" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H17" s="4">
         <v>2580919</v>
       </c>
       <c r="I17" s="4">
-        <v>1070990</v>
+        <v>1105326</v>
       </c>
       <c r="J17" s="4">
-        <f t="shared" si="4"/>
-        <v>3651909</v>
+        <f t="shared" si="5"/>
+        <v>3686245</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" si="6"/>
-        <v>233984</v>
+        <f t="shared" si="9"/>
+        <v>150424</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" si="7"/>
-        <v>43068</v>
+        <f t="shared" si="10"/>
+        <v>35892</v>
       </c>
       <c r="P17" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q17" s="4">
         <f t="shared" si="2"/>
-        <v>3885893</v>
+        <v>3836669</v>
       </c>
       <c r="R17" s="4">
         <f t="shared" si="3"/>
-        <v>3651909</v>
+        <v>3686245</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="4">
         <v>281777</v>
       </c>
       <c r="D18" s="4">
-        <v>3748117</v>
+        <v>3619209</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>4029894</v>
+        <v>3900986</v>
       </c>
       <c r="G18" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H18" s="4">
         <v>2580919</v>
       </c>
       <c r="I18" s="4">
-        <v>1129551</v>
+        <v>1134119</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" si="4"/>
-        <v>3710470</v>
+        <f t="shared" si="5"/>
+        <v>3715038</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="1"/>
-        <v>319424</v>
+        <f t="shared" ref="L18:L19" si="13">E18-J18</f>
+        <v>185948</v>
       </c>
       <c r="M18" s="5">
-        <f t="shared" si="7"/>
-        <v>85440</v>
+        <f t="shared" ref="M18:M19" si="14">L18-L17</f>
+        <v>35524</v>
       </c>
       <c r="P18" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="2"/>
-        <v>4029894</v>
+        <f t="shared" ref="Q18" si="15">C18+D18</f>
+        <v>3900986</v>
       </c>
       <c r="R18" s="4">
-        <f t="shared" si="3"/>
-        <v>3710470</v>
+        <f t="shared" ref="R18" si="16">H18+I18</f>
+        <v>3715038</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20239,11 +19662,11 @@
         <v>281777</v>
       </c>
       <c r="D19" s="4">
-        <v>4473462</v>
+        <v>4195092</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>4755239</v>
+        <v>4476869</v>
       </c>
       <c r="G19" s="2">
         <v>60</v>
@@ -20252,30 +19675,30 @@
         <v>2580919</v>
       </c>
       <c r="I19" s="4">
-        <v>1441616</v>
+        <v>1406846</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="4"/>
-        <v>4022535</v>
+        <f t="shared" si="5"/>
+        <v>3987765</v>
       </c>
       <c r="L19" s="4">
-        <f t="shared" si="1"/>
-        <v>732704</v>
+        <f t="shared" si="13"/>
+        <v>489104</v>
       </c>
       <c r="M19" s="5">
-        <f t="shared" si="5"/>
-        <v>413280</v>
+        <f t="shared" si="14"/>
+        <v>303156</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="2"/>
-        <v>4755239</v>
+        <v>4476869</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>4022535</v>
+        <v>3987765</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20286,11 +19709,11 @@
         <v>281777</v>
       </c>
       <c r="D20" s="4">
-        <v>5207707</v>
+        <v>4828692</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>5489484</v>
+        <v>5110469</v>
       </c>
       <c r="G20" s="2">
         <v>70</v>
@@ -20299,30 +19722,30 @@
         <v>2580919</v>
       </c>
       <c r="I20" s="4">
-        <v>1785781</v>
+        <v>1738566</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="4"/>
-        <v>4366700</v>
+        <f t="shared" si="5"/>
+        <v>4319485</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>1122784</v>
+        <v>790984</v>
       </c>
       <c r="M20" s="5">
-        <f t="shared" si="5"/>
-        <v>390080</v>
+        <f t="shared" si="4"/>
+        <v>301880</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="2"/>
-        <v>5489484</v>
+        <v>5110469</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>4366700</v>
+        <v>4319485</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20333,11 +19756,11 @@
         <v>281777</v>
       </c>
       <c r="D21" s="4">
-        <v>5950852</v>
+        <v>5455692</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>6232629</v>
+        <v>5737469</v>
       </c>
       <c r="G21" s="2">
         <v>80</v>
@@ -20346,30 +19769,30 @@
         <v>2580919</v>
       </c>
       <c r="I21" s="4">
-        <v>2162046</v>
+        <v>2100486</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="4"/>
-        <v>4742965</v>
+        <f>H21+I21</f>
+        <v>4681405</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>1489664</v>
+        <v>1056064</v>
       </c>
       <c r="M21" s="5">
-        <f t="shared" si="5"/>
-        <v>366880</v>
+        <f t="shared" si="4"/>
+        <v>265080</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="2"/>
-        <v>6232629</v>
+        <v>5737469</v>
       </c>
       <c r="R21" s="4">
-        <f t="shared" si="3"/>
-        <v>4742965</v>
+        <f>H21+I21</f>
+        <v>4681405</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20380,11 +19803,11 @@
         <v>281777</v>
       </c>
       <c r="D22" s="4">
-        <v>6702897</v>
+        <v>6076092</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>6984674</v>
+        <v>6357869</v>
       </c>
       <c r="G22" s="2">
         <v>90</v>
@@ -20393,30 +19816,30 @@
         <v>2580919</v>
       </c>
       <c r="I22" s="4">
-        <v>2570411</v>
+        <v>2492606</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="4"/>
-        <v>5151330</v>
+        <f t="shared" si="5"/>
+        <v>5073525</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>1833344</v>
+        <v>1284344</v>
       </c>
       <c r="M22" s="5">
-        <f t="shared" si="5"/>
-        <v>343680</v>
+        <f t="shared" si="4"/>
+        <v>228280</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="2"/>
-        <v>6984674</v>
+        <v>6357869</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>5151330</v>
+        <v>5073525</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20427,11 +19850,11 @@
         <v>281777</v>
       </c>
       <c r="D23" s="4">
-        <v>7446276</v>
+        <v>6672568</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>7728053</v>
+        <v>6954345</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
@@ -20440,30 +19863,30 @@
         <v>2580919</v>
       </c>
       <c r="I23" s="4">
-        <v>3005794</v>
+        <v>2910126</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="4"/>
-        <v>5586713</v>
+        <f t="shared" si="5"/>
+        <v>5491045</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>2141340</v>
+        <v>1463300</v>
       </c>
       <c r="M23" s="5">
-        <f t="shared" si="5"/>
-        <v>307996</v>
+        <f t="shared" si="4"/>
+        <v>178956</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="2"/>
-        <v>7728053</v>
+        <v>6954345</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>5586713</v>
+        <v>5491045</v>
       </c>
     </row>
   </sheetData>
@@ -22510,8 +21933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91734A6-3CBC-46E0-AC2D-961E5CB62031}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update optimizer 1000 runs data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4BD4AD-283A-41E2-9BF1-C4C4F5E11193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41134B3A-C186-45DA-9E91-93B4E218670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
@@ -1888,10 +1888,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1923,30 +1923,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1954,66 +1930,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>367988</c:v>
+                  <c:v>367760</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>649427</c:v>
+                  <c:v>640631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1010397</c:v>
+                  <c:v>979161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1422167</c:v>
+                  <c:v>1354891</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1884737</c:v>
+                  <c:v>1767821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2398107</c:v>
+                  <c:v>2217951</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2962277</c:v>
+                  <c:v>2705281</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3577247</c:v>
+                  <c:v>3229811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4243017</c:v>
+                  <c:v>3791541</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4959587</c:v>
+                  <c:v>4390471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5108997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5184464</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5260439</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5336922</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5413913</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5491412</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5569419</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5647934</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5706882</c:v>
+                  <c:v>5006526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2073,10 +2025,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2108,30 +2060,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -2139,10 +2067,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2644065</c:v>
                 </c:pt>
@@ -2174,30 +2102,6 @@
                   <c:v>5154043</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5239931</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5283361</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5327115</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5371193</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5415595</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5460321</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5505371</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5550745</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>5591643</c:v>
                 </c:pt>
               </c:numCache>
@@ -2636,40 +2540,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -2696,67 +2600,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604265</c:v>
+                  <c:v>604286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1217426</c:v>
+                  <c:v>1209869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1907171</c:v>
+                  <c:v>1876469</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2605816</c:v>
+                  <c:v>2536469</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3100163</c:v>
+                  <c:v>3189869</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3171140</c:v>
+                  <c:v>3254846</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3242206</c:v>
+                  <c:v>3319757</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3313361</c:v>
+                  <c:v>3384602</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3455938</c:v>
+                  <c:v>3449381</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3527360</c:v>
+                  <c:v>3514094</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3598871</c:v>
+                  <c:v>3578741</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3670471</c:v>
+                  <c:v>3643322</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3742160</c:v>
+                  <c:v>3707837</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3813938</c:v>
+                  <c:v>3772286</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3885805</c:v>
+                  <c:v>3836669</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4029806</c:v>
+                  <c:v>3900986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4755151</c:v>
+                  <c:v>4476869</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5489396</c:v>
+                  <c:v>5110469</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6232541</c:v>
+                  <c:v>5737469</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6984586</c:v>
+                  <c:v>6357869</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7727965</c:v>
+                  <c:v>6954345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2833,40 +2737,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -2893,67 +2797,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2644133</c:v>
+                  <c:v>2644114</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2781770</c:v>
+                  <c:v>2780725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2965195</c:v>
+                  <c:v>2961205</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3180720</c:v>
+                  <c:v>3171885</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3350687</c:v>
+                  <c:v>3412765</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3376252</c:v>
+                  <c:v>3438514</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3402138</c:v>
+                  <c:v>3464565</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3428345</c:v>
+                  <c:v>3490918</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3481722</c:v>
+                  <c:v>3517573</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3508892</c:v>
+                  <c:v>3544530</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3536383</c:v>
+                  <c:v>3571789</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3564195</c:v>
+                  <c:v>3599350</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3592328</c:v>
+                  <c:v>3627213</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3620782</c:v>
+                  <c:v>3655378</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3649557</c:v>
+                  <c:v>3683845</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3708070</c:v>
+                  <c:v>3712614</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4019895</c:v>
+                  <c:v>3985125</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4363820</c:v>
+                  <c:v>4316605</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4739845</c:v>
+                  <c:v>4678285</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5147970</c:v>
+                  <c:v>5070165</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5583113</c:v>
+                  <c:v>5487445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5443,10 +5347,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5478,30 +5382,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -5509,66 +5389,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>367988</c:v>
+                  <c:v>367760</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>649427</c:v>
+                  <c:v>640631</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1010397</c:v>
+                  <c:v>979161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1422167</c:v>
+                  <c:v>1354891</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1884737</c:v>
+                  <c:v>1767821</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2398107</c:v>
+                  <c:v>2217951</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2962277</c:v>
+                  <c:v>2705281</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3577247</c:v>
+                  <c:v>3229811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4243017</c:v>
+                  <c:v>3791541</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4959587</c:v>
+                  <c:v>4390471</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5108997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5184464</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5260439</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5336922</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5413913</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5491412</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5569419</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5647934</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5706882</c:v>
+                  <c:v>5006526</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5614,10 +5470,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5649,30 +5505,6 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>92</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>96</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>98</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>99</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -5680,10 +5512,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$21</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$13</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2644065</c:v>
                 </c:pt>
@@ -5715,30 +5547,6 @@
                   <c:v>5154043</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5239931</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5283361</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5327115</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>5371193</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5415595</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5460321</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5505371</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5550745</c:v>
-                </c:pt>
-                <c:pt idx="18">
                   <c:v>5591643</c:v>
                 </c:pt>
               </c:numCache>
@@ -6175,40 +5983,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -6235,67 +6043,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604265</c:v>
+                  <c:v>604286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1217426</c:v>
+                  <c:v>1209869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1907171</c:v>
+                  <c:v>1876469</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2605816</c:v>
+                  <c:v>2536469</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3100163</c:v>
+                  <c:v>3189869</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3171140</c:v>
+                  <c:v>3254846</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3242206</c:v>
+                  <c:v>3319757</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3313361</c:v>
+                  <c:v>3384602</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3455938</c:v>
+                  <c:v>3449381</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3527360</c:v>
+                  <c:v>3514094</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3598871</c:v>
+                  <c:v>3578741</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3670471</c:v>
+                  <c:v>3643322</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3742160</c:v>
+                  <c:v>3707837</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3813938</c:v>
+                  <c:v>3772286</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3885805</c:v>
+                  <c:v>3836669</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4029806</c:v>
+                  <c:v>3900986</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4755151</c:v>
+                  <c:v>4476869</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5489396</c:v>
+                  <c:v>5110469</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6232541</c:v>
+                  <c:v>5737469</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6984586</c:v>
+                  <c:v>6357869</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7727965</c:v>
+                  <c:v>6954345</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6358,40 +6166,40 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>45</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>47</c:v>
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>48</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>50</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>60</c:v>
@@ -6418,67 +6226,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2644133</c:v>
+                  <c:v>2644114</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2781770</c:v>
+                  <c:v>2780725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2965195</c:v>
+                  <c:v>2961205</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3180720</c:v>
+                  <c:v>3171885</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3350687</c:v>
+                  <c:v>3412765</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3376252</c:v>
+                  <c:v>3438514</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3402138</c:v>
+                  <c:v>3464565</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3428345</c:v>
+                  <c:v>3490918</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3481722</c:v>
+                  <c:v>3517573</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3508892</c:v>
+                  <c:v>3544530</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3536383</c:v>
+                  <c:v>3571789</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3564195</c:v>
+                  <c:v>3599350</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3592328</c:v>
+                  <c:v>3627213</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3620782</c:v>
+                  <c:v>3655378</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3649557</c:v>
+                  <c:v>3683845</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3708070</c:v>
+                  <c:v>3712614</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4019895</c:v>
+                  <c:v>3985125</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4363820</c:v>
+                  <c:v>4316605</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4739845</c:v>
+                  <c:v>4678285</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5147970</c:v>
+                  <c:v>5070165</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5583113</c:v>
+                  <c:v>5487445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16066,16 +15874,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1362075</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>19500</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>431100</xdr:rowOff>
+      <xdr:colOff>450</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -18859,7 +18667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06EBE3-BB9C-4874-A95E-FF2651C40304}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
@@ -19909,10 +19717,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871ADF-8F0F-453C-9415-AC73938A5FD8}">
-  <dimension ref="A2:R23"/>
+  <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19960,14 +19768,14 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D3" s="4">
-        <v>86255</v>
+        <v>85983</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>367988</v>
+        <v>367760</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -19984,14 +19792,14 @@
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2276077</v>
+        <v>-2276305</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>367988</v>
+        <v>367760</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
@@ -20003,14 +19811,14 @@
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D4" s="4">
-        <v>367694</v>
+        <v>358854</v>
       </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E21" si="0">C4+D4</f>
-        <v>649427</v>
+        <f t="shared" ref="E4:E13" si="0">C4+D4</f>
+        <v>640631</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -20026,22 +19834,22 @@
         <v>2781243</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L21" si="1">E4-J4</f>
-        <v>-2131816</v>
+        <f t="shared" ref="L4:L13" si="1">E4-J4</f>
+        <v>-2140612</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>144261</v>
+        <v>135693</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q21" si="2">C4+D4</f>
-        <v>649427</v>
+        <f t="shared" ref="Q4:Q13" si="2">C4+D4</f>
+        <v>640631</v>
       </c>
       <c r="R4" s="4">
-        <f t="shared" ref="R4:R21" si="3">H4+I4</f>
+        <f t="shared" ref="R4:R13" si="3">H4+I4</f>
         <v>2781243</v>
       </c>
     </row>
@@ -20050,14 +19858,14 @@
         <v>20</v>
       </c>
       <c r="C5" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D5" s="4">
-        <v>728664</v>
+        <v>697384</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1010397</v>
+        <v>979161</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -20069,23 +19877,23 @@
         <v>384724</v>
       </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J21" si="4">H5+I5</f>
+        <f t="shared" ref="J5:J13" si="4">H5+I5</f>
         <v>2964443</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1954046</v>
+        <v>-1985282</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>177770</v>
+        <v>155330</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>1010397</v>
+        <v>979161</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
@@ -20097,14 +19905,14 @@
         <v>30</v>
       </c>
       <c r="C6" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D6" s="4">
-        <v>1140434</v>
+        <v>1073114</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1422167</v>
+        <v>1354891</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -20121,18 +19929,18 @@
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-1757876</v>
+        <v>-1825152</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>196170</v>
+        <v>160130</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>1422167</v>
+        <v>1354891</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
@@ -20144,14 +19952,14 @@
         <v>40</v>
       </c>
       <c r="C7" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D7" s="4">
-        <v>1603004</v>
+        <v>1486044</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1884737</v>
+        <v>1767821</v>
       </c>
       <c r="G7" s="2">
         <v>40</v>
@@ -20168,18 +19976,18 @@
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>-1543306</v>
+        <v>-1660222</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>214570</v>
+        <v>164930</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>1884737</v>
+        <v>1767821</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
@@ -20191,14 +19999,14 @@
         <v>50</v>
       </c>
       <c r="C8" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D8" s="4">
-        <v>2116374</v>
+        <v>1936174</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2398107</v>
+        <v>2217951</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
@@ -20215,18 +20023,18 @@
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-1310336</v>
+        <v>-1490492</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>232970</v>
+        <v>169730</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>2398107</v>
+        <v>2217951</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
@@ -20238,14 +20046,14 @@
         <v>60</v>
       </c>
       <c r="C9" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D9" s="4">
-        <v>2680544</v>
+        <v>2423504</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2962277</v>
+        <v>2705281</v>
       </c>
       <c r="G9" s="2">
         <v>60</v>
@@ -20262,18 +20070,18 @@
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>-1058966</v>
+        <v>-1315962</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>251370</v>
+        <v>174530</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>2962277</v>
+        <v>2705281</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
@@ -20285,14 +20093,14 @@
         <v>70</v>
       </c>
       <c r="C10" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D10" s="4">
-        <v>3295514</v>
+        <v>2948034</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3577247</v>
+        <v>3229811</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
@@ -20309,18 +20117,18 @@
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>-789196</v>
+        <v>-1136632</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>269770</v>
+        <v>179330</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3577247</v>
+        <v>3229811</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
@@ -20332,14 +20140,14 @@
         <v>80</v>
       </c>
       <c r="C11" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D11" s="4">
-        <v>3961284</v>
+        <v>3509764</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>4243017</v>
+        <v>3791541</v>
       </c>
       <c r="G11" s="2">
         <v>80</v>
@@ -20356,18 +20164,18 @@
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>-501026</v>
+        <v>-952502</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>288170</v>
+        <v>184130</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>4243017</v>
+        <v>3791541</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
@@ -20379,14 +20187,14 @@
         <v>90</v>
       </c>
       <c r="C12" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D12" s="4">
-        <v>4677854</v>
+        <v>4108694</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>4959587</v>
+        <v>4390471</v>
       </c>
       <c r="G12" s="2">
         <v>90</v>
@@ -20403,18 +20211,18 @@
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>-194456</v>
+        <v>-763572</v>
       </c>
       <c r="M12" s="5">
         <f>L12-L11</f>
-        <v>306570</v>
+        <v>188930</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>4959587</v>
+        <v>4390471</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
@@ -20423,444 +20231,65 @@
     </row>
     <row r="13" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C13" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D13" s="4">
-        <v>4827264</v>
+        <v>4724749</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>5108997</v>
+        <v>5006526</v>
       </c>
       <c r="G13" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="H13" s="4">
         <v>2579719</v>
       </c>
       <c r="I13" s="4">
-        <v>2660212</v>
+        <v>3011924</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>5239931</v>
+        <v>5591643</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" ref="L13:L16" si="6">E13-J13</f>
-        <v>-130934</v>
+        <f t="shared" si="1"/>
+        <v>-585117</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" ref="M13:M16" si="7">L13-L12</f>
-        <v>63522</v>
+        <f>L13-L12</f>
+        <v>178455</v>
       </c>
       <c r="P13" s="2">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>5108997</v>
+        <v>5006526</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>5239931</v>
+        <v>5591643</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
-        <v>93</v>
-      </c>
-      <c r="C14" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D14" s="4">
-        <v>4902731</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>5184464</v>
-      </c>
-      <c r="G14" s="2">
-        <v>93</v>
-      </c>
-      <c r="H14" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I14" s="4">
-        <v>2703642</v>
-      </c>
-      <c r="J14" s="4">
-        <f t="shared" si="4"/>
-        <v>5283361</v>
-      </c>
-      <c r="L14" s="4">
-        <f t="shared" si="6"/>
-        <v>-98897</v>
-      </c>
-      <c r="M14" s="5">
-        <f t="shared" si="7"/>
-        <v>32037</v>
-      </c>
-      <c r="P14" s="2">
-        <v>93</v>
-      </c>
-      <c r="Q14" s="4">
-        <f t="shared" si="2"/>
-        <v>5184464</v>
-      </c>
-      <c r="R14" s="4">
-        <f t="shared" si="3"/>
-        <v>5283361</v>
-      </c>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
     </row>
     <row r="15" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
-        <v>94</v>
-      </c>
-      <c r="C15" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D15" s="4">
-        <v>4978706</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>5260439</v>
-      </c>
-      <c r="G15" s="2">
-        <v>94</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2747396</v>
-      </c>
-      <c r="J15" s="4">
-        <f t="shared" si="4"/>
-        <v>5327115</v>
-      </c>
-      <c r="L15" s="4">
-        <f t="shared" si="6"/>
-        <v>-66676</v>
-      </c>
-      <c r="M15" s="5">
-        <f t="shared" si="7"/>
-        <v>32221</v>
-      </c>
-      <c r="P15" s="2">
-        <v>94</v>
-      </c>
-      <c r="Q15" s="4">
-        <f t="shared" si="2"/>
-        <v>5260439</v>
-      </c>
-      <c r="R15" s="4">
-        <f t="shared" si="3"/>
-        <v>5327115</v>
-      </c>
-    </row>
-    <row r="16" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
-        <v>95</v>
-      </c>
-      <c r="C16" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D16" s="4">
-        <v>5055189</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>5336922</v>
-      </c>
-      <c r="G16" s="2">
-        <v>95</v>
-      </c>
-      <c r="H16" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I16" s="4">
-        <v>2791474</v>
-      </c>
-      <c r="J16" s="4">
-        <f t="shared" si="4"/>
-        <v>5371193</v>
-      </c>
-      <c r="L16" s="4">
-        <f t="shared" si="6"/>
-        <v>-34271</v>
-      </c>
-      <c r="M16" s="5">
-        <f t="shared" si="7"/>
-        <v>32405</v>
-      </c>
-      <c r="P16" s="2">
-        <v>95</v>
-      </c>
-      <c r="Q16" s="4">
-        <f t="shared" si="2"/>
-        <v>5336922</v>
-      </c>
-      <c r="R16" s="4">
-        <f t="shared" si="3"/>
-        <v>5371193</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
-        <v>96</v>
-      </c>
-      <c r="C17" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D17" s="4">
-        <v>5132180</v>
-      </c>
-      <c r="E17" s="4">
-        <f t="shared" si="0"/>
-        <v>5413913</v>
-      </c>
-      <c r="G17" s="2">
-        <v>96</v>
-      </c>
-      <c r="H17" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I17" s="4">
-        <v>2835876</v>
-      </c>
-      <c r="J17" s="4">
-        <f t="shared" si="4"/>
-        <v>5415595</v>
-      </c>
-      <c r="L17" s="4">
-        <f t="shared" ref="L17" si="8">E17-J17</f>
-        <v>-1682</v>
-      </c>
-      <c r="M17" s="5">
-        <f>L17-L12</f>
-        <v>192774</v>
-      </c>
-      <c r="P17" s="2">
-        <v>96</v>
-      </c>
-      <c r="Q17" s="4">
-        <f t="shared" si="2"/>
-        <v>5413913</v>
-      </c>
-      <c r="R17" s="4">
-        <f t="shared" si="3"/>
-        <v>5415595</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="2">
-        <v>97</v>
-      </c>
-      <c r="C18" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D18" s="4">
-        <v>5209679</v>
-      </c>
-      <c r="E18" s="4">
-        <f t="shared" si="0"/>
-        <v>5491412</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="2">
-        <v>97</v>
-      </c>
-      <c r="H18" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I18" s="4">
-        <v>2880602</v>
-      </c>
-      <c r="J18" s="4">
-        <f t="shared" si="4"/>
-        <v>5460321</v>
-      </c>
-      <c r="K18" s="6"/>
-      <c r="L18" s="4">
-        <f t="shared" ref="L18" si="9">E18-J18</f>
-        <v>31091</v>
-      </c>
-      <c r="M18" s="5">
-        <f>L18-L12</f>
-        <v>225547</v>
-      </c>
-      <c r="P18" s="2">
-        <v>97</v>
-      </c>
-      <c r="Q18" s="4">
-        <f t="shared" si="2"/>
-        <v>5491412</v>
-      </c>
-      <c r="R18" s="4">
-        <f t="shared" si="3"/>
-        <v>5460321</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
-        <v>98</v>
-      </c>
-      <c r="C19" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D19" s="4">
-        <v>5287686</v>
-      </c>
-      <c r="E19" s="4">
-        <f t="shared" si="0"/>
-        <v>5569419</v>
-      </c>
-      <c r="G19" s="2">
-        <v>98</v>
-      </c>
-      <c r="H19" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I19" s="4">
-        <v>2925652</v>
-      </c>
-      <c r="J19" s="4">
-        <f t="shared" si="4"/>
-        <v>5505371</v>
-      </c>
-      <c r="L19" s="4">
-        <f t="shared" ref="L19" si="10">E19-J19</f>
-        <v>64048</v>
-      </c>
-      <c r="M19" s="5">
-        <f>L19-L12</f>
-        <v>258504</v>
-      </c>
-      <c r="P19" s="2">
-        <v>98</v>
-      </c>
-      <c r="Q19" s="4">
-        <f t="shared" si="2"/>
-        <v>5569419</v>
-      </c>
-      <c r="R19" s="4">
-        <f t="shared" si="3"/>
-        <v>5505371</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
-        <v>99</v>
-      </c>
-      <c r="C20" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D20" s="4">
-        <v>5366201</v>
-      </c>
-      <c r="E20" s="4">
-        <f t="shared" si="0"/>
-        <v>5647934</v>
-      </c>
-      <c r="G20" s="2">
-        <v>99</v>
-      </c>
-      <c r="H20" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I20" s="4">
-        <v>2971026</v>
-      </c>
-      <c r="J20" s="4">
-        <f t="shared" si="4"/>
-        <v>5550745</v>
-      </c>
-      <c r="L20" s="4">
-        <f t="shared" ref="L20" si="11">E20-J20</f>
-        <v>97189</v>
-      </c>
-      <c r="M20" s="5">
-        <f>L20-L12</f>
-        <v>291645</v>
-      </c>
-      <c r="P20" s="2">
-        <v>99</v>
-      </c>
-      <c r="Q20" s="4">
-        <f t="shared" si="2"/>
-        <v>5647934</v>
-      </c>
-      <c r="R20" s="4">
-        <f t="shared" si="3"/>
-        <v>5550745</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
-        <v>100</v>
-      </c>
-      <c r="C21" s="4">
-        <v>281733</v>
-      </c>
-      <c r="D21" s="4">
-        <v>5425149</v>
-      </c>
-      <c r="E21" s="4">
-        <f t="shared" si="0"/>
-        <v>5706882</v>
-      </c>
-      <c r="G21" s="2">
-        <v>100</v>
-      </c>
-      <c r="H21" s="4">
-        <v>2579719</v>
-      </c>
-      <c r="I21" s="4">
-        <v>3011924</v>
-      </c>
-      <c r="J21" s="4">
-        <f t="shared" si="4"/>
-        <v>5591643</v>
-      </c>
-      <c r="L21" s="4">
-        <f t="shared" si="1"/>
-        <v>115239</v>
-      </c>
-      <c r="M21" s="5">
-        <f>L21-L12</f>
-        <v>309695</v>
-      </c>
-      <c r="P21" s="2">
-        <v>100</v>
-      </c>
-      <c r="Q21" s="4">
-        <f t="shared" si="2"/>
-        <v>5706882</v>
-      </c>
-      <c r="R21" s="4">
-        <f t="shared" si="3"/>
-        <v>5591643</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-    </row>
-    <row r="23" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
-      <c r="R23"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L3:L21">
+  <conditionalFormatting sqref="L3:L13">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -20881,8 +20310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20930,14 +20359,14 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D3" s="4">
-        <v>322532</v>
+        <v>322509</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>604265</v>
+        <v>604286</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -20946,26 +20375,26 @@
         <v>2579719</v>
       </c>
       <c r="I3" s="4">
-        <v>64414</v>
+        <v>64395</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2644133</v>
+        <v>2644114</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2039868</v>
+        <v>-2039828</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>604265</v>
+        <v>604286</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2644133</v>
+        <v>2644114</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20973,14 +20402,14 @@
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D4" s="4">
-        <v>935693</v>
+        <v>928092</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E23" si="0">C4+D4</f>
-        <v>1217426</v>
+        <v>1209869</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -20989,30 +20418,30 @@
         <v>2579719</v>
       </c>
       <c r="I4" s="4">
-        <v>202051</v>
+        <v>201006</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2781770</v>
+        <v>2780725</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>-1564344</v>
+        <v>-1570856</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>475524</v>
+        <v>468972</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
-        <v>1217426</v>
+        <v>1209869</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>2781770</v>
+        <v>2780725</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21020,14 +20449,14 @@
         <v>20</v>
       </c>
       <c r="C5" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D5" s="4">
-        <v>1625438</v>
+        <v>1594692</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1907171</v>
+        <v>1876469</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -21036,30 +20465,30 @@
         <v>2579719</v>
       </c>
       <c r="I5" s="4">
-        <v>385476</v>
+        <v>381486</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J23" si="4">H5+I5</f>
-        <v>2965195</v>
+        <v>2961205</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1058024</v>
+        <v>-1084736</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="5">L5-L4</f>
-        <v>506320</v>
+        <v>486120</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>1907171</v>
+        <v>1876469</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>2965195</v>
+        <v>2961205</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21067,14 +20496,14 @@
         <v>30</v>
       </c>
       <c r="C6" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D6" s="4">
-        <v>2324083</v>
+        <v>2254692</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2605816</v>
+        <v>2536469</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -21083,597 +20512,597 @@
         <v>2579719</v>
       </c>
       <c r="I6" s="4">
-        <v>601001</v>
+        <v>592166</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>3180720</v>
+        <v>3171885</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-574904</v>
+        <v>-635416</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>483120</v>
+        <v>449320</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>2605816</v>
+        <v>2536469</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3180720</v>
+        <v>3171885</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C7" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D7" s="4">
-        <v>2818430</v>
+        <v>2908092</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>3100163</v>
+        <v>3189869</v>
       </c>
       <c r="G7" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H7" s="4">
         <v>2579719</v>
       </c>
       <c r="I7" s="4">
-        <v>770968</v>
+        <v>833046</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>3350687</v>
+        <v>3412765</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7:L9" si="6">E7-J7</f>
-        <v>-250524</v>
+        <f>E7-J7</f>
+        <v>-222896</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" ref="M7:M10" si="7">L7-L6</f>
-        <v>324380</v>
+        <f>L7-L6</f>
+        <v>412520</v>
       </c>
       <c r="P7" s="2">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>3100163</v>
+        <v>3189869</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
-        <v>3350687</v>
+        <v>3412765</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D8" s="4">
-        <v>2889407</v>
+        <v>2973069</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3171140</v>
+        <v>3254846</v>
       </c>
       <c r="G8" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="H8" s="4">
         <v>2579719</v>
       </c>
       <c r="I8" s="4">
-        <v>796533</v>
+        <v>858795</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>3376252</v>
+        <v>3438514</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="6"/>
-        <v>-205112</v>
+        <f>E8-J8</f>
+        <v>-183668</v>
       </c>
       <c r="M8" s="5">
-        <f t="shared" si="7"/>
-        <v>45412</v>
+        <f>L8-L7</f>
+        <v>39228</v>
       </c>
       <c r="P8" s="2">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="2"/>
-        <v>3171140</v>
+        <f t="shared" ref="Q8" si="6">C8+D8</f>
+        <v>3254846</v>
       </c>
       <c r="R8" s="4">
-        <f t="shared" si="3"/>
-        <v>3376252</v>
+        <f t="shared" ref="R8" si="7">H8+I8</f>
+        <v>3438514</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C9" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D9" s="4">
-        <v>2960473</v>
+        <v>3037980</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3242206</v>
+        <v>3319757</v>
       </c>
       <c r="G9" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="H9" s="4">
         <v>2579719</v>
       </c>
       <c r="I9" s="4">
-        <v>822419</v>
+        <v>884846</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>3402138</v>
+        <v>3464565</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="6"/>
-        <v>-159932</v>
+        <f t="shared" ref="L9" si="8">E9-J9</f>
+        <v>-144808</v>
       </c>
       <c r="M9" s="5">
-        <f t="shared" si="7"/>
-        <v>45180</v>
+        <f>L9-L8</f>
+        <v>38860</v>
       </c>
       <c r="P9" s="2">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>3242206</v>
+        <v>3319757</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>3402138</v>
+        <v>3464565</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D10" s="4">
-        <v>3031628</v>
+        <v>3102825</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3313361</v>
+        <v>3384602</v>
       </c>
       <c r="G10" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H10" s="4">
         <v>2579719</v>
       </c>
       <c r="I10" s="4">
-        <v>848626</v>
+        <v>911199</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>3428345</v>
+        <v>3490918</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="1"/>
-        <v>-114984</v>
+        <f t="shared" ref="L10" si="9">E10-J10</f>
+        <v>-106316</v>
       </c>
       <c r="M10" s="5">
-        <f t="shared" si="7"/>
-        <v>44948</v>
+        <f t="shared" ref="M10:M14" si="10">L10-L9</f>
+        <v>38492</v>
       </c>
       <c r="P10" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3313361</v>
+        <v>3384602</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>3428345</v>
+        <v>3490918</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C11" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D11" s="4">
-        <v>3174205</v>
+        <v>3167604</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3455938</v>
+        <v>3449381</v>
       </c>
       <c r="G11" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H11" s="4">
         <v>2579719</v>
       </c>
       <c r="I11" s="4">
-        <v>902003</v>
+        <v>937854</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>3481722</v>
+        <v>3517573</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" ref="L11" si="8">E11-J11</f>
-        <v>-25784</v>
+        <f t="shared" ref="L11" si="11">E11-J11</f>
+        <v>-68192</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" ref="M11" si="9">L11-L10</f>
-        <v>89200</v>
+        <f t="shared" si="10"/>
+        <v>38124</v>
       </c>
       <c r="P11" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3455938</v>
+        <v>3449381</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>3481722</v>
+        <v>3517573</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
       <c r="B12" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C12" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D12" s="4">
-        <v>3245627</v>
+        <v>3232317</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3527360</v>
-      </c>
-      <c r="F12" s="6"/>
+        <v>3514094</v>
+      </c>
       <c r="G12" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H12" s="4">
         <v>2579719</v>
       </c>
       <c r="I12" s="4">
-        <v>929173</v>
+        <v>964811</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>3508892</v>
-      </c>
-      <c r="K12" s="6"/>
+        <v>3544530</v>
+      </c>
       <c r="L12" s="4">
-        <f t="shared" ref="L12" si="10">E12-J12</f>
-        <v>18468</v>
+        <f t="shared" ref="L12" si="12">E12-J12</f>
+        <v>-30436</v>
       </c>
       <c r="M12" s="5">
-        <f>L12-L10</f>
-        <v>133452</v>
+        <f t="shared" si="10"/>
+        <v>37756</v>
       </c>
       <c r="P12" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>3527360</v>
+        <v>3514094</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>3508892</v>
+        <v>3544530</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
       <c r="B13" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D13" s="4">
-        <v>3317138</v>
+        <v>3296964</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>3598871</v>
-      </c>
+        <v>3578741</v>
+      </c>
+      <c r="F13" s="6"/>
       <c r="G13" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H13" s="4">
         <v>2579719</v>
       </c>
       <c r="I13" s="4">
-        <v>956664</v>
+        <v>992070</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>3536383</v>
-      </c>
+        <v>3571789</v>
+      </c>
+      <c r="K13" s="6"/>
       <c r="L13" s="4">
-        <f t="shared" ref="L13" si="11">E13-J13</f>
-        <v>62488</v>
+        <f t="shared" ref="L13:L15" si="13">E13-J13</f>
+        <v>6952</v>
       </c>
       <c r="M13" s="5">
-        <f>L13-L10</f>
-        <v>177472</v>
+        <f t="shared" si="10"/>
+        <v>37388</v>
       </c>
       <c r="P13" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>3598871</v>
+        <v>3578741</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>3536383</v>
+        <v>3571789</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D14" s="4">
-        <v>3388738</v>
+        <v>3361545</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3670471</v>
+        <v>3643322</v>
       </c>
       <c r="G14" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H14" s="4">
         <v>2579719</v>
       </c>
       <c r="I14" s="4">
-        <v>984476</v>
+        <v>1019631</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="4"/>
-        <v>3564195</v>
+        <v>3599350</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" ref="L14" si="12">E14-J14</f>
-        <v>106276</v>
+        <f t="shared" si="13"/>
+        <v>43972</v>
       </c>
       <c r="M14" s="5">
-        <f>L14-L10</f>
-        <v>221260</v>
+        <f t="shared" si="10"/>
+        <v>37020</v>
       </c>
       <c r="P14" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>3670471</v>
+        <v>3643322</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>3564195</v>
+        <v>3599350</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D15" s="4">
-        <v>3460427</v>
+        <v>3426060</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>3742160</v>
+        <v>3707837</v>
       </c>
       <c r="G15" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H15" s="4">
         <v>2579719</v>
       </c>
       <c r="I15" s="4">
-        <v>1012609</v>
+        <v>1047494</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="4"/>
-        <v>3592328</v>
+        <v>3627213</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" ref="L15:L17" si="13">E15-J15</f>
-        <v>149832</v>
+        <f t="shared" si="13"/>
+        <v>80624</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" ref="M15:M17" si="14">L15-L11</f>
-        <v>175616</v>
+        <f t="shared" ref="M15" si="14">L15-L11</f>
+        <v>148816</v>
       </c>
       <c r="P15" s="2">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>3742160</v>
+        <v>3707837</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>3592328</v>
+        <v>3627213</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C16" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D16" s="4">
-        <v>3532205</v>
+        <v>3490509</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>3813938</v>
+        <v>3772286</v>
       </c>
       <c r="G16" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H16" s="4">
         <v>2579719</v>
       </c>
       <c r="I16" s="4">
-        <v>1041063</v>
+        <v>1075659</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="4"/>
-        <v>3620782</v>
+        <v>3655378</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="13"/>
-        <v>193156</v>
+        <f t="shared" ref="L16:L17" si="15">E16-J16</f>
+        <v>116908</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" si="14"/>
-        <v>174688</v>
+        <f t="shared" ref="M16:M17" si="16">L16-L12</f>
+        <v>147344</v>
       </c>
       <c r="P16" s="2">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="Q16" s="4">
-        <f t="shared" si="2"/>
-        <v>3813938</v>
+        <f t="shared" ref="Q16:Q18" si="17">C16+D16</f>
+        <v>3772286</v>
       </c>
       <c r="R16" s="4">
-        <f t="shared" si="3"/>
-        <v>3620782</v>
+        <f t="shared" ref="R16:R18" si="18">H16+I16</f>
+        <v>3655378</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C17" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D17" s="4">
-        <v>3604072</v>
+        <v>3554892</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>3885805</v>
+        <v>3836669</v>
       </c>
       <c r="G17" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H17" s="4">
         <v>2579719</v>
       </c>
       <c r="I17" s="4">
-        <v>1069838</v>
+        <v>1104126</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="4"/>
-        <v>3649557</v>
+        <v>3683845</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" si="13"/>
-        <v>236248</v>
+        <f t="shared" si="15"/>
+        <v>152824</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" si="14"/>
-        <v>173760</v>
+        <f t="shared" si="16"/>
+        <v>145872</v>
       </c>
       <c r="P17" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" si="2"/>
-        <v>3885805</v>
+        <f t="shared" si="17"/>
+        <v>3836669</v>
       </c>
       <c r="R17" s="4">
-        <f t="shared" si="3"/>
-        <v>3649557</v>
+        <f t="shared" si="18"/>
+        <v>3683845</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C18" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D18" s="4">
-        <v>3748073</v>
+        <v>3619209</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>4029806</v>
+        <v>3900986</v>
       </c>
       <c r="G18" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H18" s="4">
         <v>2579719</v>
       </c>
       <c r="I18" s="4">
-        <v>1128351</v>
+        <v>1132895</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="4"/>
-        <v>3708070</v>
+        <v>3712614</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="1"/>
-        <v>321736</v>
+        <f t="shared" ref="L18:L19" si="19">E18-J18</f>
+        <v>188372</v>
       </c>
       <c r="M18" s="5">
-        <f>L18-L10</f>
-        <v>436720</v>
+        <f t="shared" ref="M18:M19" si="20">L18-L14</f>
+        <v>144400</v>
       </c>
       <c r="P18" s="2">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="2"/>
-        <v>4029806</v>
+        <f t="shared" si="17"/>
+        <v>3900986</v>
       </c>
       <c r="R18" s="4">
-        <f t="shared" si="3"/>
-        <v>3708070</v>
+        <f t="shared" si="18"/>
+        <v>3712614</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21681,14 +21110,14 @@
         <v>60</v>
       </c>
       <c r="C19" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D19" s="4">
-        <v>4473418</v>
+        <v>4195092</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>4755151</v>
+        <v>4476869</v>
       </c>
       <c r="G19" s="2">
         <v>60</v>
@@ -21697,30 +21126,30 @@
         <v>2579719</v>
       </c>
       <c r="I19" s="4">
-        <v>1440176</v>
+        <v>1405406</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="4"/>
-        <v>4019895</v>
+        <v>3985125</v>
       </c>
       <c r="L19" s="4">
-        <f t="shared" si="1"/>
-        <v>735256</v>
+        <f t="shared" si="19"/>
+        <v>491744</v>
       </c>
       <c r="M19" s="5">
-        <f t="shared" si="5"/>
-        <v>413520</v>
+        <f t="shared" si="20"/>
+        <v>411120</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="2"/>
-        <v>4755151</v>
+        <v>4476869</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>4019895</v>
+        <v>3985125</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21728,14 +21157,14 @@
         <v>70</v>
       </c>
       <c r="C20" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D20" s="4">
-        <v>5207663</v>
+        <v>4828692</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>5489396</v>
+        <v>5110469</v>
       </c>
       <c r="G20" s="2">
         <v>70</v>
@@ -21744,30 +21173,30 @@
         <v>2579719</v>
       </c>
       <c r="I20" s="4">
-        <v>1784101</v>
+        <v>1736886</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="4"/>
-        <v>4363820</v>
+        <v>4316605</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>1125576</v>
+        <v>793864</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="5"/>
-        <v>390320</v>
+        <v>302120</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="2"/>
-        <v>5489396</v>
+        <v>5110469</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>4363820</v>
+        <v>4316605</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21775,14 +21204,14 @@
         <v>80</v>
       </c>
       <c r="C21" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D21" s="4">
-        <v>5950808</v>
+        <v>5455692</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>6232541</v>
+        <v>5737469</v>
       </c>
       <c r="G21" s="2">
         <v>80</v>
@@ -21791,30 +21220,30 @@
         <v>2579719</v>
       </c>
       <c r="I21" s="4">
-        <v>2160126</v>
+        <v>2098566</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="4"/>
-        <v>4739845</v>
+        <v>4678285</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>1492696</v>
+        <v>1059184</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>367120</v>
+        <v>265320</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="2"/>
-        <v>6232541</v>
+        <v>5737469</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="3"/>
-        <v>4739845</v>
+        <v>4678285</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21822,14 +21251,14 @@
         <v>90</v>
       </c>
       <c r="C22" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D22" s="4">
-        <v>6702853</v>
+        <v>6076092</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>6984586</v>
+        <v>6357869</v>
       </c>
       <c r="G22" s="2">
         <v>90</v>
@@ -21838,30 +21267,30 @@
         <v>2579719</v>
       </c>
       <c r="I22" s="4">
-        <v>2568251</v>
+        <v>2490446</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="4"/>
-        <v>5147970</v>
+        <v>5070165</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>1836616</v>
+        <v>1287704</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="5"/>
-        <v>343920</v>
+        <v>228520</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="2"/>
-        <v>6984586</v>
+        <v>6357869</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>5147970</v>
+        <v>5070165</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21869,14 +21298,14 @@
         <v>100</v>
       </c>
       <c r="C23" s="4">
-        <v>281733</v>
+        <v>281777</v>
       </c>
       <c r="D23" s="4">
-        <v>7446232</v>
+        <v>6672568</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>7727965</v>
+        <v>6954345</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
@@ -21885,30 +21314,30 @@
         <v>2579719</v>
       </c>
       <c r="I23" s="4">
-        <v>3003394</v>
+        <v>2907726</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="4"/>
-        <v>5583113</v>
+        <v>5487445</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>2144852</v>
+        <v>1466900</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="5"/>
-        <v>308236</v>
+        <v>179196</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="2"/>
-        <v>7727965</v>
+        <v>6954345</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>5583113</v>
+        <v>5487445</v>
       </c>
     </row>
   </sheetData>
@@ -21933,8 +21362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91734A6-3CBC-46E0-AC2D-961E5CB62031}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update optimizer disabled data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41134B3A-C186-45DA-9E91-93B4E218670B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB4E27D-6D25-480E-8677-C6E311717560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -688,37 +688,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2696138</c:v>
+                  <c:v>2698111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2843135</c:v>
+                  <c:v>2827630</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3044560</c:v>
+                  <c:v>3013150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3286085</c:v>
+                  <c:v>3242470</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3567710</c:v>
+                  <c:v>3515590</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3889435</c:v>
+                  <c:v>3832510</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4251260</c:v>
+                  <c:v>4193230</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4653185</c:v>
+                  <c:v>4597750</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5095210</c:v>
+                  <c:v>5046070</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5577335</c:v>
+                  <c:v>5538190</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6094760</c:v>
+                  <c:v>6069310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2102,7 +2102,7 @@
                   <c:v>5154043</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5591643</c:v>
+                  <c:v>5385993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3282,37 +3282,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -3354,37 +3354,37 @@
                   <c:v>2843293</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3148647</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>3224913</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3301150</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3377358</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3453537</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3529687</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>3605808</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>3681900</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>3757963</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3833997</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>3910002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3985978</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>4365423</c:v>
@@ -3465,37 +3465,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -3525,67 +3525,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2696333</c:v>
+                  <c:v>2698306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2845067</c:v>
+                  <c:v>2829562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3048422</c:v>
+                  <c:v>3017012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3291877</c:v>
+                  <c:v>3248262</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3428642</c:v>
+                  <c:v>3353026</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3457198</c:v>
+                  <c:v>3380312</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3486155</c:v>
+                  <c:v>3408036</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3515513</c:v>
+                  <c:v>3436198</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3545272</c:v>
+                  <c:v>3464798</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3575432</c:v>
+                  <c:v>3493836</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3605993</c:v>
+                  <c:v>3523312</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3636955</c:v>
+                  <c:v>3553226</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3668318</c:v>
+                  <c:v>3583578</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3700082</c:v>
+                  <c:v>3614368</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3732247</c:v>
+                  <c:v>3645596</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3899087</c:v>
+                  <c:v>3842162</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4262842</c:v>
+                  <c:v>4204812</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4666697</c:v>
+                  <c:v>4611262</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5110652</c:v>
+                  <c:v>5061512</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5594707</c:v>
+                  <c:v>5555562</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6114062</c:v>
+                  <c:v>6088612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5547,7 +5547,7 @@
                   <c:v>5154043</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5591643</c:v>
+                  <c:v>5385993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6878,37 +6878,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2696138</c:v>
+                  <c:v>2698111</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2843135</c:v>
+                  <c:v>2827630</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3044560</c:v>
+                  <c:v>3013150</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3286085</c:v>
+                  <c:v>3242470</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3567710</c:v>
+                  <c:v>3515590</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3889435</c:v>
+                  <c:v>3832510</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4251260</c:v>
+                  <c:v>4193230</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4653185</c:v>
+                  <c:v>4597750</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5095210</c:v>
+                  <c:v>5046070</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5577335</c:v>
+                  <c:v>5538190</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6094760</c:v>
+                  <c:v>6069310</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7339,37 +7339,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -7411,37 +7411,37 @@
                   <c:v>2843293</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>3148647</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>3224913</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>3301150</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>3377358</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>3453537</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>3529687</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>3605808</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>3681900</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>3757963</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>3833997</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>3910002</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3985978</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>4365423</c:v>
@@ -7536,37 +7536,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>35</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>36</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>37</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="8">
                   <c:v>38</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="10">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="12">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="13">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="14">
                   <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -7596,67 +7596,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2696333</c:v>
+                  <c:v>2698306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2845067</c:v>
+                  <c:v>2829562</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3048422</c:v>
+                  <c:v>3017012</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3291877</c:v>
+                  <c:v>3248262</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3428642</c:v>
+                  <c:v>3353026</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3457198</c:v>
+                  <c:v>3380312</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3486155</c:v>
+                  <c:v>3408036</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3515513</c:v>
+                  <c:v>3436198</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3545272</c:v>
+                  <c:v>3464798</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3575432</c:v>
+                  <c:v>3493836</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3605993</c:v>
+                  <c:v>3523312</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3636955</c:v>
+                  <c:v>3553226</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3668318</c:v>
+                  <c:v>3583578</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3700082</c:v>
+                  <c:v>3614368</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3732247</c:v>
+                  <c:v>3645596</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3899087</c:v>
+                  <c:v>3842162</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4262842</c:v>
+                  <c:v>4204812</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4666697</c:v>
+                  <c:v>4611262</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5110652</c:v>
+                  <c:v>5061512</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5594707</c:v>
+                  <c:v>5555562</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6114062</c:v>
+                  <c:v>6088612</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15710,7 +15710,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>19500</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>431100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -16446,7 +16446,7 @@
   <dimension ref="B2:R13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16507,18 +16507,18 @@
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I3" s="4">
-        <v>65348</v>
+        <v>63221</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2696138</v>
+        <v>2698111</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2325881</v>
+        <v>-2327854</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
@@ -16529,7 +16529,7 @@
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2696138</v>
+        <v>2698111</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16550,22 +16550,22 @@
         <v>10</v>
       </c>
       <c r="H4" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I4" s="4">
-        <v>212345</v>
+        <v>192740</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2843135</v>
+        <v>2827630</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L13" si="1">E4-J4</f>
-        <v>-2188001</v>
+        <v>-2172496</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>137880</v>
+        <v>155358</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
@@ -16576,7 +16576,7 @@
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R13" si="3">H4+I4</f>
-        <v>2843135</v>
+        <v>2827630</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16597,22 +16597,22 @@
         <v>20</v>
       </c>
       <c r="H5" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I5" s="4">
-        <v>413770</v>
+        <v>378260</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J12" si="4">H5+I5</f>
-        <v>3044560</v>
+        <v>3013150</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-2027771</v>
+        <v>-1996361</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>160230</v>
+        <v>176135</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
@@ -16623,7 +16623,7 @@
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>3044560</v>
+        <v>3013150</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16644,22 +16644,22 @@
         <v>30</v>
       </c>
       <c r="H6" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I6" s="4">
-        <v>655295</v>
+        <v>607580</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>3286085</v>
+        <v>3242470</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-1860141</v>
+        <v>-1816526</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>167630</v>
+        <v>179835</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
@@ -16670,7 +16670,7 @@
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3286085</v>
+        <v>3242470</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16691,22 +16691,22 @@
         <v>40</v>
       </c>
       <c r="H7" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I7" s="4">
-        <v>936920</v>
+        <v>880700</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>3567710</v>
+        <v>3515590</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>-1685111</v>
+        <v>-1632991</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>175030</v>
+        <v>183535</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
@@ -16717,7 +16717,7 @@
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
-        <v>3567710</v>
+        <v>3515590</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16738,22 +16738,22 @@
         <v>50</v>
       </c>
       <c r="H8" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I8" s="4">
-        <v>1258645</v>
+        <v>1197620</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>3889435</v>
+        <v>3832510</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-1502681</v>
+        <v>-1445756</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>182430</v>
+        <v>187235</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
@@ -16764,7 +16764,7 @@
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>3889435</v>
+        <v>3832510</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16785,22 +16785,22 @@
         <v>60</v>
       </c>
       <c r="H9" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I9" s="4">
-        <v>1620470</v>
+        <v>1558340</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>4251260</v>
+        <v>4193230</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>-1312851</v>
+        <v>-1254821</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>189830</v>
+        <v>190935</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
@@ -16811,7 +16811,7 @@
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>4251260</v>
+        <v>4193230</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16832,22 +16832,22 @@
         <v>70</v>
       </c>
       <c r="H10" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I10" s="4">
-        <v>2022395</v>
+        <v>1962860</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>4653185</v>
+        <v>4597750</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>-1115621</v>
+        <v>-1060186</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>197230</v>
+        <v>194635</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
@@ -16858,7 +16858,7 @@
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>4653185</v>
+        <v>4597750</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16879,22 +16879,22 @@
         <v>80</v>
       </c>
       <c r="H11" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I11" s="4">
-        <v>2464420</v>
+        <v>2411180</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>5095210</v>
+        <v>5046070</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>-910991</v>
+        <v>-861851</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>204630</v>
+        <v>198335</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
@@ -16905,7 +16905,7 @@
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>5095210</v>
+        <v>5046070</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16926,22 +16926,22 @@
         <v>90</v>
       </c>
       <c r="H12" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I12" s="4">
-        <v>2946545</v>
+        <v>2903300</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>5577335</v>
+        <v>5538190</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>-698961</v>
+        <v>-659816</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" ref="M12:M13" si="6">L12-L11</f>
-        <v>212030</v>
+        <v>202035</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
@@ -16952,7 +16952,7 @@
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>5577335</v>
+        <v>5538190</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16973,22 +16973,22 @@
         <v>100</v>
       </c>
       <c r="H13" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I13" s="4">
-        <v>3463970</v>
+        <v>3434420</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" ref="J13" si="8">H13+I13</f>
-        <v>6094760</v>
+        <v>6069310</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>-494823</v>
+        <v>-469373</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="6"/>
-        <v>204138</v>
+        <v>190443</v>
       </c>
       <c r="P13" s="2">
         <v>100</v>
@@ -16999,18 +16999,18 @@
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>6094760</v>
+        <v>6069310</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L3:L13">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17025,7 +17025,7 @@
   <dimension ref="A2:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17086,18 +17086,18 @@
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I3" s="4">
-        <v>65543</v>
+        <v>63416</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2696333</v>
+        <v>2698306</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2080733</v>
+        <v>-2082706</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
@@ -17108,7 +17108,7 @@
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2696333</v>
+        <v>2698306</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17129,22 +17129,22 @@
         <v>10</v>
       </c>
       <c r="H4" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I4" s="4">
-        <v>214277</v>
+        <v>194672</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2845067</v>
+        <v>2829562</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>-1535504</v>
+        <v>-1519999</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>545229</v>
+        <v>562707</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
@@ -17155,7 +17155,7 @@
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>2845067</v>
+        <v>2829562</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17176,22 +17176,22 @@
         <v>20</v>
       </c>
       <c r="H5" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I5" s="4">
-        <v>417632</v>
+        <v>382122</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J17" si="4">H5+I5</f>
-        <v>3048422</v>
+        <v>3017012</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-970544</v>
+        <v>-939134</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="5">L5-L4</f>
-        <v>564960</v>
+        <v>580865</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
@@ -17202,7 +17202,7 @@
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>3048422</v>
+        <v>3017012</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17223,22 +17223,22 @@
         <v>30</v>
       </c>
       <c r="H6" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I6" s="4">
-        <v>661087</v>
+        <v>613372</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>3291877</v>
+        <v>3248262</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-448584</v>
+        <v>-404969</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>521960</v>
+        <v>534165</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
@@ -17249,527 +17249,527 @@
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3291877</v>
+        <v>3248262</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="4">
         <v>283159</v>
       </c>
       <c r="D7" s="4">
-        <v>2941754</v>
+        <v>2865488</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>3224913</v>
+        <v>3148647</v>
       </c>
       <c r="G7" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I7" s="4">
-        <v>797852</v>
+        <v>718136</v>
       </c>
       <c r="J7" s="4">
-        <f t="shared" si="4"/>
-        <v>3428642</v>
+        <f t="shared" ref="J7:J8" si="6">H7+I7</f>
+        <v>3353026</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7:L11" si="6">E7-J7</f>
-        <v>-203729</v>
+        <f t="shared" ref="L7:L8" si="7">E7-J7</f>
+        <v>-204379</v>
       </c>
       <c r="M7" s="5">
-        <f>L7-L6</f>
-        <v>244855</v>
+        <f t="shared" ref="M7:M8" si="8">L7-L6</f>
+        <v>200590</v>
       </c>
       <c r="P7" s="2">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" si="2"/>
-        <v>3224913</v>
+        <f t="shared" ref="Q7:Q8" si="9">C7+D7</f>
+        <v>3148647</v>
       </c>
       <c r="R7" s="4">
-        <f t="shared" si="3"/>
-        <v>3428642</v>
+        <f t="shared" ref="R7:R8" si="10">H7+I7</f>
+        <v>3353026</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4">
         <v>283159</v>
       </c>
       <c r="D8" s="4">
-        <v>3017991</v>
+        <v>2941754</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3301150</v>
+        <v>3224913</v>
       </c>
       <c r="G8" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I8" s="4">
-        <v>826408</v>
+        <v>745422</v>
       </c>
       <c r="J8" s="4">
-        <f t="shared" si="4"/>
-        <v>3457198</v>
+        <f t="shared" si="6"/>
+        <v>3380312</v>
       </c>
       <c r="L8" s="4">
-        <f t="shared" si="6"/>
-        <v>-156048</v>
+        <f t="shared" si="7"/>
+        <v>-155399</v>
       </c>
       <c r="M8" s="5">
-        <f>L8-L7</f>
-        <v>47681</v>
+        <f t="shared" si="8"/>
+        <v>48980</v>
       </c>
       <c r="P8" s="2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="2"/>
-        <v>3301150</v>
+        <f t="shared" si="9"/>
+        <v>3224913</v>
       </c>
       <c r="R8" s="4">
-        <f t="shared" si="3"/>
-        <v>3457198</v>
+        <f t="shared" si="10"/>
+        <v>3380312</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4">
         <v>283159</v>
       </c>
       <c r="D9" s="4">
-        <v>3094199</v>
+        <v>3017991</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3377358</v>
+        <v>3301150</v>
       </c>
       <c r="G9" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I9" s="4">
-        <v>855365</v>
+        <v>773146</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>3486155</v>
+        <v>3408036</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" si="6"/>
-        <v>-108797</v>
+        <f t="shared" ref="L9:L12" si="11">E9-J9</f>
+        <v>-106886</v>
       </c>
       <c r="M9" s="5">
-        <f t="shared" ref="M8:M12" si="7">L9-L8</f>
-        <v>47251</v>
+        <f>L9-L8</f>
+        <v>48513</v>
       </c>
       <c r="P9" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>3377358</v>
+        <v>3301150</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>3486155</v>
+        <v>3408036</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4">
         <v>283159</v>
       </c>
       <c r="D10" s="4">
-        <v>3170378</v>
+        <v>3094199</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3453537</v>
+        <v>3377358</v>
       </c>
       <c r="G10" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H10" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I10" s="4">
-        <v>884723</v>
+        <v>801308</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>3515513</v>
+        <v>3436198</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" si="6"/>
-        <v>-61976</v>
+        <f t="shared" si="11"/>
+        <v>-58840</v>
       </c>
       <c r="M10" s="5">
-        <f t="shared" si="7"/>
-        <v>46821</v>
+        <f t="shared" ref="M10:M13" si="12">L10-L9</f>
+        <v>48046</v>
       </c>
       <c r="P10" s="2">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3453537</v>
+        <v>3377358</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>3515513</v>
+        <v>3436198</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="4">
         <v>283159</v>
       </c>
       <c r="D11" s="4">
-        <v>3246528</v>
+        <v>3170378</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3529687</v>
+        <v>3453537</v>
       </c>
       <c r="G11" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H11" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I11" s="4">
-        <v>914482</v>
+        <v>829908</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>3545272</v>
+        <v>3464798</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="6"/>
-        <v>-15585</v>
+        <f t="shared" si="11"/>
+        <v>-11261</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" si="7"/>
-        <v>46391</v>
+        <f t="shared" si="12"/>
+        <v>47579</v>
       </c>
       <c r="P11" s="2">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3529687</v>
+        <v>3453537</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>3545272</v>
+        <v>3464798</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="4">
         <v>283159</v>
       </c>
       <c r="D12" s="4">
-        <v>3322649</v>
+        <v>3246528</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3605808</v>
+        <v>3529687</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H12" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I12" s="4">
-        <v>944642</v>
+        <v>858946</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>3575432</v>
+        <v>3493836</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="4">
-        <f t="shared" si="1"/>
-        <v>30376</v>
+        <f t="shared" si="11"/>
+        <v>35851</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" si="7"/>
-        <v>45961</v>
+        <f t="shared" si="12"/>
+        <v>47112</v>
       </c>
       <c r="P12" s="2">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>3605808</v>
+        <v>3529687</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>3575432</v>
+        <v>3493836</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="4">
         <v>283159</v>
       </c>
       <c r="D13" s="4">
-        <v>3398741</v>
+        <v>3322649</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>3681900</v>
+        <v>3605808</v>
       </c>
       <c r="G13" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H13" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I13" s="4">
-        <v>975203</v>
+        <v>888422</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>3605993</v>
+        <v>3523312</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>75907</v>
+        <v>82496</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" si="5"/>
-        <v>45531</v>
+        <f t="shared" si="12"/>
+        <v>46645</v>
       </c>
       <c r="P13" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>3681900</v>
+        <v>3605808</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>3605993</v>
+        <v>3523312</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="4">
         <v>283159</v>
       </c>
       <c r="D14" s="4">
-        <v>3474804</v>
+        <v>3398741</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3757963</v>
+        <v>3681900</v>
       </c>
       <c r="G14" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H14" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I14" s="4">
-        <v>1006165</v>
+        <v>918336</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="4"/>
-        <v>3636955</v>
+        <v>3553226</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="1"/>
-        <v>121008</v>
+        <v>128674</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="5"/>
-        <v>45101</v>
+        <v>46178</v>
       </c>
       <c r="P14" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>3757963</v>
+        <v>3681900</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>3636955</v>
+        <v>3553226</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="4">
         <v>283159</v>
       </c>
       <c r="D15" s="4">
-        <v>3550838</v>
+        <v>3474804</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>3833997</v>
+        <v>3757963</v>
       </c>
       <c r="G15" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H15" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I15" s="4">
-        <v>1037528</v>
+        <v>948688</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="4"/>
-        <v>3668318</v>
+        <v>3583578</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>165679</v>
+        <v>174385</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="5"/>
-        <v>44671</v>
+        <v>45711</v>
       </c>
       <c r="P15" s="2">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>3833997</v>
+        <v>3757963</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>3668318</v>
+        <v>3583578</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4">
         <v>283159</v>
       </c>
       <c r="D16" s="4">
-        <v>3626843</v>
+        <v>3550838</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>3910002</v>
+        <v>3833997</v>
       </c>
       <c r="G16" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H16" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I16" s="4">
-        <v>1069292</v>
+        <v>979478</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="4"/>
-        <v>3700082</v>
+        <v>3614368</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="1"/>
-        <v>209920</v>
+        <v>219629</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" si="5"/>
-        <v>44241</v>
+        <f>L16-L15</f>
+        <v>45244</v>
       </c>
       <c r="P16" s="2">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q16" s="4">
         <f t="shared" si="2"/>
-        <v>3910002</v>
+        <v>3833997</v>
       </c>
       <c r="R16" s="4">
         <f t="shared" si="3"/>
-        <v>3700082</v>
+        <v>3614368</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="4">
         <v>283159</v>
       </c>
       <c r="D17" s="4">
-        <v>3702819</v>
+        <v>3626843</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>3985978</v>
+        <v>3910002</v>
       </c>
       <c r="G17" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H17" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I17" s="4">
-        <v>1101457</v>
+        <v>1010706</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="4"/>
-        <v>3732247</v>
+        <v>3645596</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" si="1"/>
-        <v>253731</v>
+        <f t="shared" ref="L17:L18" si="13">E17-J17</f>
+        <v>264406</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" si="5"/>
-        <v>43811</v>
+        <f t="shared" ref="M17:M18" si="14">L17-L16</f>
+        <v>44777</v>
       </c>
       <c r="P17" s="2">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" ref="Q17" si="8">C17+D17</f>
-        <v>3985978</v>
+        <f t="shared" ref="Q17" si="15">C17+D17</f>
+        <v>3910002</v>
       </c>
       <c r="R17" s="4">
-        <f t="shared" ref="R17" si="9">H17+I17</f>
-        <v>3732247</v>
+        <f t="shared" ref="R17" si="16">H17+I17</f>
+        <v>3645596</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17790,22 +17790,22 @@
         <v>50</v>
       </c>
       <c r="H18" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I18" s="4">
-        <v>1268297</v>
+        <v>1207272</v>
       </c>
       <c r="J18" s="4">
-        <f t="shared" ref="J18:J23" si="10">H18+I18</f>
-        <v>3899087</v>
+        <f t="shared" ref="J18:J23" si="17">H18+I18</f>
+        <v>3842162</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="1"/>
-        <v>466336</v>
+        <f t="shared" si="13"/>
+        <v>523261</v>
       </c>
       <c r="M18" s="5">
-        <f t="shared" si="5"/>
-        <v>212605</v>
+        <f t="shared" si="14"/>
+        <v>258855</v>
       </c>
       <c r="P18" s="2">
         <v>50</v>
@@ -17816,7 +17816,7 @@
       </c>
       <c r="R18" s="4">
         <f t="shared" si="3"/>
-        <v>3899087</v>
+        <v>3842162</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17837,22 +17837,22 @@
         <v>60</v>
       </c>
       <c r="H19" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I19" s="4">
-        <v>1632052</v>
+        <v>1569922</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" si="10"/>
-        <v>4262842</v>
+        <f t="shared" si="17"/>
+        <v>4204812</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="1"/>
-        <v>859296</v>
+        <v>917326</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="5"/>
-        <v>392960</v>
+        <v>394065</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
@@ -17863,7 +17863,7 @@
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>4262842</v>
+        <v>4204812</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17884,22 +17884,22 @@
         <v>70</v>
       </c>
       <c r="H20" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I20" s="4">
-        <v>2035907</v>
+        <v>1976372</v>
       </c>
       <c r="J20" s="4">
-        <f t="shared" si="10"/>
-        <v>4666697</v>
+        <f t="shared" si="17"/>
+        <v>4611262</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>1209256</v>
+        <v>1264691</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="5"/>
-        <v>349960</v>
+        <v>347365</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
@@ -17910,7 +17910,7 @@
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>4666697</v>
+        <v>4611262</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17931,22 +17931,22 @@
         <v>80</v>
       </c>
       <c r="H21" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I21" s="4">
-        <v>2479862</v>
+        <v>2426622</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="10"/>
-        <v>5110652</v>
+        <f t="shared" si="17"/>
+        <v>5061512</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>1516216</v>
+        <v>1565356</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>306960</v>
+        <v>300665</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
@@ -17957,7 +17957,7 @@
       </c>
       <c r="R21" s="4">
         <f t="shared" si="3"/>
-        <v>5110652</v>
+        <v>5061512</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17978,22 +17978,22 @@
         <v>90</v>
       </c>
       <c r="H22" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I22" s="4">
-        <v>2963917</v>
+        <v>2920672</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="10"/>
-        <v>5594707</v>
+        <f t="shared" si="17"/>
+        <v>5555562</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>1780176</v>
+        <v>1819321</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="5"/>
-        <v>263960</v>
+        <v>253965</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
@@ -18004,7 +18004,7 @@
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>5594707</v>
+        <v>5555562</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18025,22 +18025,22 @@
         <v>100</v>
       </c>
       <c r="H23" s="4">
-        <v>2630790</v>
+        <v>2634890</v>
       </c>
       <c r="I23" s="4">
-        <v>3483272</v>
+        <v>3453722</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="10"/>
-        <v>6114062</v>
+        <f t="shared" si="17"/>
+        <v>6088612</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>1988636</v>
+        <v>2014086</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="5"/>
-        <v>208460</v>
+        <v>194765</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
@@ -18051,7 +18051,7 @@
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>6114062</v>
+        <v>6088612</v>
       </c>
     </row>
   </sheetData>
@@ -18076,8 +18076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F68343B-F0B9-4DF5-8EBB-C222891744B9}">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U15" sqref="U15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19017,11 +19017,11 @@
         <v>3466773</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" ref="L7:L15" si="7">E9-J9</f>
+        <f t="shared" ref="L9:L15" si="7">E9-J9</f>
         <v>-147016</v>
       </c>
       <c r="M9" s="5">
-        <f t="shared" ref="M8:M15" si="8">L9-L8</f>
+        <f t="shared" ref="M9:M15" si="8">L9-L8</f>
         <v>38836</v>
       </c>
       <c r="P9" s="2">
@@ -19719,8 +19719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871ADF-8F0F-453C-9415-AC73938A5FD8}">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20247,22 +20247,22 @@
         <v>100</v>
       </c>
       <c r="H13" s="4">
-        <v>2579719</v>
+        <v>2596719</v>
       </c>
       <c r="I13" s="4">
-        <v>3011924</v>
+        <v>2789274</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>5591643</v>
+        <v>5385993</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>-585117</v>
+        <v>-379467</v>
       </c>
       <c r="M13" s="5">
         <f>L13-L12</f>
-        <v>178455</v>
+        <v>384105</v>
       </c>
       <c r="P13" s="2">
         <v>100</v>
@@ -20273,7 +20273,7 @@
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>5591643</v>
+        <v>5385993</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20283,20 +20283,20 @@
       <c r="R14"/>
     </row>
     <row r="15" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L3:L13">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21362,7 +21362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91734A6-3CBC-46E0-AC2D-961E5CB62031}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update Break even ERC721A and ERC721F.xlsx
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E57FBCD-DF86-4492-B8D5-A4A8B91E7A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F267F16-05C2-4F7B-A71F-9738C4A388BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -20310,7 +20310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
@@ -21362,8 +21362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91734A6-3CBC-46E0-AC2D-961E5CB62031}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correction optimizer 1000 runs data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F267F16-05C2-4F7B-A71F-9738C4A388BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABCA39B-0FCB-4CCA-8A3A-684FC666B63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="5" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -2072,37 +2072,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2661431</c:v>
+                  <c:v>2652887</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2779880</c:v>
+                  <c:v>2771228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2941985</c:v>
+                  <c:v>2933213</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3136190</c:v>
+                  <c:v>3127298</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3362495</c:v>
+                  <c:v>3353483</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3620900</c:v>
+                  <c:v>3611768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3911405</c:v>
+                  <c:v>3902153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4234010</c:v>
+                  <c:v>4224638</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4588715</c:v>
+                  <c:v>4579223</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4975520</c:v>
+                  <c:v>4965908</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5389625</c:v>
+                  <c:v>5379893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2797,67 +2797,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2661458</c:v>
+                  <c:v>2652936</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2779340</c:v>
+                  <c:v>2770710</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2938725</c:v>
+                  <c:v>2929975</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3128010</c:v>
+                  <c:v>3119140</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3323931</c:v>
+                  <c:v>3314953</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3347195</c:v>
+                  <c:v>3338205</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3370758</c:v>
+                  <c:v>3361756</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3394620</c:v>
+                  <c:v>3385606</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3418781</c:v>
+                  <c:v>3409755</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3443241</c:v>
+                  <c:v>3434203</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3468000</c:v>
+                  <c:v>3458950</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3493058</c:v>
+                  <c:v>3483996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3518415</c:v>
+                  <c:v>3509341</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3544071</c:v>
+                  <c:v>3534985</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3570026</c:v>
+                  <c:v>3560928</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3596280</c:v>
+                  <c:v>3587170</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3875265</c:v>
+                  <c:v>3866035</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4184150</c:v>
+                  <c:v>4174800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4522935</c:v>
+                  <c:v>4513465</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4891620</c:v>
+                  <c:v>4882030</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5285405</c:v>
+                  <c:v>5275695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5517,37 +5517,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>2661431</c:v>
+                  <c:v>2652887</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2779880</c:v>
+                  <c:v>2771228</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2941985</c:v>
+                  <c:v>2933213</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3136190</c:v>
+                  <c:v>3127298</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3362495</c:v>
+                  <c:v>3353483</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3620900</c:v>
+                  <c:v>3611768</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3911405</c:v>
+                  <c:v>3902153</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4234010</c:v>
+                  <c:v>4224638</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4588715</c:v>
+                  <c:v>4579223</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4975520</c:v>
+                  <c:v>4965908</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5389625</c:v>
+                  <c:v>5379893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6226,67 +6226,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2661458</c:v>
+                  <c:v>2652936</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2779340</c:v>
+                  <c:v>2770710</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2938725</c:v>
+                  <c:v>2929975</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3128010</c:v>
+                  <c:v>3119140</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3323931</c:v>
+                  <c:v>3314953</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3347195</c:v>
+                  <c:v>3338205</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3370758</c:v>
+                  <c:v>3361756</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3394620</c:v>
+                  <c:v>3385606</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3418781</c:v>
+                  <c:v>3409755</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3443241</c:v>
+                  <c:v>3434203</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3468000</c:v>
+                  <c:v>3458950</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3493058</c:v>
+                  <c:v>3483996</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3518415</c:v>
+                  <c:v>3509341</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3544071</c:v>
+                  <c:v>3534985</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3570026</c:v>
+                  <c:v>3560928</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3596280</c:v>
+                  <c:v>3587170</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3875265</c:v>
+                  <c:v>3866035</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4184150</c:v>
+                  <c:v>4174800</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4522935</c:v>
+                  <c:v>4513465</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4891620</c:v>
+                  <c:v>4882030</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5285405</c:v>
+                  <c:v>5275695</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19720,7 +19720,7 @@
   <dimension ref="B2:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19781,18 +19781,18 @@
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I3" s="4">
-        <v>62346</v>
+        <v>62268</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2661431</v>
+        <v>2652887</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2293671</v>
+        <v>-2285127</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
@@ -19803,7 +19803,7 @@
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2661431</v>
+        <v>2652887</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19824,22 +19824,22 @@
         <v>10</v>
       </c>
       <c r="H4" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I4" s="4">
-        <v>180795</v>
+        <v>180609</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2779880</v>
+        <v>2771228</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L13" si="1">E4-J4</f>
-        <v>-2139249</v>
+        <v>-2130597</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>154422</v>
+        <v>154530</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
@@ -19850,7 +19850,7 @@
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R13" si="3">H4+I4</f>
-        <v>2779880</v>
+        <v>2771228</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19871,22 +19871,22 @@
         <v>20</v>
       </c>
       <c r="H5" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I5" s="4">
-        <v>342900</v>
+        <v>342594</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J13" si="4">H5+I5</f>
-        <v>2941985</v>
+        <v>2933213</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1962824</v>
+        <v>-1954052</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>176425</v>
+        <v>176545</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
@@ -19897,7 +19897,7 @@
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>2941985</v>
+        <v>2933213</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19918,22 +19918,22 @@
         <v>30</v>
       </c>
       <c r="H6" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I6" s="4">
-        <v>537105</v>
+        <v>536679</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>3136190</v>
+        <v>3127298</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-1781299</v>
+        <v>-1772407</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>181525</v>
+        <v>181645</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
@@ -19944,7 +19944,7 @@
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3136190</v>
+        <v>3127298</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19965,22 +19965,22 @@
         <v>40</v>
       </c>
       <c r="H7" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I7" s="4">
-        <v>763410</v>
+        <v>762864</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>3362495</v>
+        <v>3353483</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>-1594674</v>
+        <v>-1585662</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>186625</v>
+        <v>186745</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
@@ -19991,7 +19991,7 @@
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
-        <v>3362495</v>
+        <v>3353483</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20012,22 +20012,22 @@
         <v>50</v>
       </c>
       <c r="H8" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I8" s="4">
-        <v>1021815</v>
+        <v>1021149</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>3620900</v>
+        <v>3611768</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-1402949</v>
+        <v>-1393817</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>191725</v>
+        <v>191845</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
@@ -20038,7 +20038,7 @@
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>3620900</v>
+        <v>3611768</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20059,22 +20059,22 @@
         <v>60</v>
       </c>
       <c r="H9" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I9" s="4">
-        <v>1312320</v>
+        <v>1311534</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>3911405</v>
+        <v>3902153</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>-1206124</v>
+        <v>-1196872</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>196825</v>
+        <v>196945</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
@@ -20085,7 +20085,7 @@
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>3911405</v>
+        <v>3902153</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20106,22 +20106,22 @@
         <v>70</v>
       </c>
       <c r="H10" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I10" s="4">
-        <v>1634925</v>
+        <v>1634019</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>4234010</v>
+        <v>4224638</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>-1004199</v>
+        <v>-994827</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>201925</v>
+        <v>202045</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
@@ -20132,7 +20132,7 @@
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>4234010</v>
+        <v>4224638</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20153,22 +20153,22 @@
         <v>80</v>
       </c>
       <c r="H11" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I11" s="4">
-        <v>1989630</v>
+        <v>1988604</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>4588715</v>
+        <v>4579223</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>-797174</v>
+        <v>-787682</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>207025</v>
+        <v>207145</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
@@ -20179,7 +20179,7 @@
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>4588715</v>
+        <v>4579223</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20200,22 +20200,22 @@
         <v>90</v>
       </c>
       <c r="H12" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I12" s="4">
-        <v>2376435</v>
+        <v>2375289</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>4975520</v>
+        <v>4965908</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>-585049</v>
+        <v>-575437</v>
       </c>
       <c r="M12" s="5">
         <f>L12-L11</f>
-        <v>212125</v>
+        <v>212245</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
@@ -20226,7 +20226,7 @@
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>4975520</v>
+        <v>4965908</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20247,22 +20247,22 @@
         <v>100</v>
       </c>
       <c r="H13" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I13" s="4">
-        <v>2790540</v>
+        <v>2789274</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>5389625</v>
+        <v>5379893</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>-383099</v>
+        <v>-373367</v>
       </c>
       <c r="M13" s="5">
         <f>L13-L12</f>
-        <v>201950</v>
+        <v>202070</v>
       </c>
       <c r="P13" s="2">
         <v>100</v>
@@ -20273,7 +20273,7 @@
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>5389625</v>
+        <v>5379893</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20310,8 +20310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20372,18 +20372,18 @@
         <v>1</v>
       </c>
       <c r="H3" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I3" s="4">
-        <v>62373</v>
+        <v>62317</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2661458</v>
+        <v>2652936</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2057172</v>
+        <v>-2048650</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
@@ -20394,7 +20394,7 @@
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2661458</v>
+        <v>2652936</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20415,22 +20415,22 @@
         <v>10</v>
       </c>
       <c r="H4" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I4" s="4">
-        <v>180255</v>
+        <v>180091</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2779340</v>
+        <v>2770710</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>-1569471</v>
+        <v>-1560841</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>487701</v>
+        <v>487809</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
@@ -20441,7 +20441,7 @@
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>2779340</v>
+        <v>2770710</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20462,22 +20462,22 @@
         <v>20</v>
       </c>
       <c r="H5" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I5" s="4">
-        <v>339640</v>
+        <v>339356</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J23" si="4">H5+I5</f>
-        <v>2938725</v>
+        <v>2929975</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1062256</v>
+        <v>-1053506</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="5">L5-L4</f>
-        <v>507215</v>
+        <v>507335</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
@@ -20488,7 +20488,7 @@
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>2938725</v>
+        <v>2929975</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20509,22 +20509,22 @@
         <v>30</v>
       </c>
       <c r="H6" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I6" s="4">
-        <v>528925</v>
+        <v>528521</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>3128010</v>
+        <v>3119140</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-591541</v>
+        <v>-582671</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>470715</v>
+        <v>470835</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
@@ -20535,7 +20535,7 @@
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3128010</v>
+        <v>3119140</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20556,22 +20556,22 @@
         <v>39</v>
       </c>
       <c r="H7" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I7" s="4">
-        <v>724846</v>
+        <v>724334</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>3323931</v>
+        <v>3314953</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" ref="L7:L8" si="6">E7-J7</f>
-        <v>-199193</v>
+        <v>-190215</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" ref="M7:M8" si="7">L7-L6</f>
-        <v>392348</v>
+        <v>392456</v>
       </c>
       <c r="P7" s="2">
         <v>31</v>
@@ -20582,7 +20582,7 @@
       </c>
       <c r="R7" s="4">
         <f t="shared" ref="R7" si="9">H7+I7</f>
-        <v>3323931</v>
+        <v>3314953</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20603,22 +20603,22 @@
         <v>40</v>
       </c>
       <c r="H8" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I8" s="4">
-        <v>748110</v>
+        <v>747586</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>3347195</v>
+        <v>3338205</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="6"/>
-        <v>-157326</v>
+        <v>-148336</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="7"/>
-        <v>41867</v>
+        <v>41879</v>
       </c>
       <c r="P8" s="2">
         <v>40</v>
@@ -20629,7 +20629,7 @@
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>3347195</v>
+        <v>3338205</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20650,22 +20650,22 @@
         <v>41</v>
       </c>
       <c r="H9" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I9" s="4">
-        <v>771673</v>
+        <v>771137</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>3370758</v>
+        <v>3361756</v>
       </c>
       <c r="L9" s="4">
         <f>E9-J9</f>
-        <v>-115912</v>
+        <v>-106910</v>
       </c>
       <c r="M9" s="5">
         <f>L9-L8</f>
-        <v>41414</v>
+        <v>41426</v>
       </c>
       <c r="P9" s="2">
         <v>41</v>
@@ -20676,7 +20676,7 @@
       </c>
       <c r="R9" s="4">
         <f t="shared" ref="R9" si="11">H9+I9</f>
-        <v>3370758</v>
+        <v>3361756</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20697,22 +20697,22 @@
         <v>42</v>
       </c>
       <c r="H10" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I10" s="4">
-        <v>795535</v>
+        <v>794987</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>3394620</v>
+        <v>3385606</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" ref="L10" si="12">E10-J10</f>
-        <v>-74863</v>
+        <v>-65849</v>
       </c>
       <c r="M10" s="5">
         <f>L10-L9</f>
-        <v>41049</v>
+        <v>41061</v>
       </c>
       <c r="P10" s="2">
         <v>42</v>
@@ -20723,7 +20723,7 @@
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>3394620</v>
+        <v>3385606</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20744,22 +20744,22 @@
         <v>43</v>
       </c>
       <c r="H11" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I11" s="4">
-        <v>819696</v>
+        <v>819136</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>3418781</v>
+        <v>3409755</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" ref="L11" si="13">E11-J11</f>
-        <v>-34179</v>
+        <v>-25153</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" ref="M11:M15" si="14">L11-L10</f>
-        <v>40684</v>
+        <v>40696</v>
       </c>
       <c r="P11" s="2">
         <v>43</v>
@@ -20770,7 +20770,7 @@
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>3418781</v>
+        <v>3409755</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20793,23 +20793,23 @@
         <v>44</v>
       </c>
       <c r="H12" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I12" s="4">
-        <v>844156</v>
+        <v>843584</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>3443241</v>
+        <v>3434203</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="4">
         <f t="shared" ref="L12" si="15">E12-J12</f>
-        <v>6140</v>
+        <v>15178</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="14"/>
-        <v>40319</v>
+        <v>40331</v>
       </c>
       <c r="P12" s="2">
         <v>44</v>
@@ -20820,7 +20820,7 @@
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>3443241</v>
+        <v>3434203</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20841,22 +20841,22 @@
         <v>45</v>
       </c>
       <c r="H13" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I13" s="4">
-        <v>868915</v>
+        <v>868331</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>3468000</v>
+        <v>3458950</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" ref="L13" si="16">E13-J13</f>
-        <v>46094</v>
+        <v>55144</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="14"/>
-        <v>39954</v>
+        <v>39966</v>
       </c>
       <c r="P13" s="2">
         <v>45</v>
@@ -20867,7 +20867,7 @@
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>3468000</v>
+        <v>3458950</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20888,22 +20888,22 @@
         <v>46</v>
       </c>
       <c r="H14" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I14" s="4">
-        <v>893973</v>
+        <v>893377</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="4"/>
-        <v>3493058</v>
+        <v>3483996</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" ref="L14:L16" si="17">E14-J14</f>
-        <v>85683</v>
+        <v>94745</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="14"/>
-        <v>39589</v>
+        <v>39601</v>
       </c>
       <c r="P14" s="2">
         <v>46</v>
@@ -20914,7 +20914,7 @@
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>3493058</v>
+        <v>3483996</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20935,22 +20935,22 @@
         <v>47</v>
       </c>
       <c r="H15" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I15" s="4">
-        <v>919330</v>
+        <v>918722</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="4"/>
-        <v>3518415</v>
+        <v>3509341</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="17"/>
-        <v>124907</v>
+        <v>133981</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="14"/>
-        <v>39224</v>
+        <v>39236</v>
       </c>
       <c r="P15" s="2">
         <v>47</v>
@@ -20961,7 +20961,7 @@
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>3518415</v>
+        <v>3509341</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20982,22 +20982,22 @@
         <v>48</v>
       </c>
       <c r="H16" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I16" s="4">
-        <v>944986</v>
+        <v>944366</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="4"/>
-        <v>3544071</v>
+        <v>3534985</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="17"/>
-        <v>163766</v>
+        <v>172852</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" ref="M16" si="18">L16-L12</f>
-        <v>157626</v>
+        <v>157674</v>
       </c>
       <c r="P16" s="2">
         <v>48</v>
@@ -21008,7 +21008,7 @@
       </c>
       <c r="R16" s="4">
         <f t="shared" si="3"/>
-        <v>3544071</v>
+        <v>3534985</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21029,22 +21029,22 @@
         <v>49</v>
       </c>
       <c r="H17" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I17" s="4">
-        <v>970941</v>
+        <v>970309</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="4"/>
-        <v>3570026</v>
+        <v>3560928</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" ref="L17:L18" si="19">E17-J17</f>
-        <v>202260</v>
+        <v>211358</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" ref="M17:M18" si="20">L17-L13</f>
-        <v>156166</v>
+        <v>156214</v>
       </c>
       <c r="P17" s="2">
         <v>49</v>
@@ -21055,7 +21055,7 @@
       </c>
       <c r="R17" s="4">
         <f t="shared" ref="R17:R18" si="22">H17+I17</f>
-        <v>3570026</v>
+        <v>3560928</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21076,22 +21076,22 @@
         <v>50</v>
       </c>
       <c r="H18" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I18" s="4">
-        <v>997195</v>
+        <v>996551</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="4"/>
-        <v>3596280</v>
+        <v>3587170</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="19"/>
-        <v>240389</v>
+        <v>249499</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="20"/>
-        <v>154706</v>
+        <v>154754</v>
       </c>
       <c r="P18" s="2">
         <v>50</v>
@@ -21102,7 +21102,7 @@
       </c>
       <c r="R18" s="4">
         <f t="shared" si="22"/>
-        <v>3596280</v>
+        <v>3587170</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21123,22 +21123,22 @@
         <v>60</v>
       </c>
       <c r="H19" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I19" s="4">
-        <v>1276180</v>
+        <v>1275416</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="4"/>
-        <v>3875265</v>
+        <v>3866035</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" ref="L19" si="23">E19-J19</f>
-        <v>601604</v>
+        <v>610834</v>
       </c>
       <c r="M19" s="5">
         <f>L19-L16</f>
-        <v>437838</v>
+        <v>437982</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
@@ -21149,7 +21149,7 @@
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>3875265</v>
+        <v>3866035</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21170,22 +21170,22 @@
         <v>70</v>
       </c>
       <c r="H20" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I20" s="4">
-        <v>1585065</v>
+        <v>1584181</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="4"/>
-        <v>4184150</v>
+        <v>4174800</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>926319</v>
+        <v>935669</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="5"/>
-        <v>324715</v>
+        <v>324835</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
@@ -21196,7 +21196,7 @@
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>4184150</v>
+        <v>4174800</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21217,22 +21217,22 @@
         <v>80</v>
       </c>
       <c r="H21" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I21" s="4">
-        <v>1923850</v>
+        <v>1922846</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="4"/>
-        <v>4522935</v>
+        <v>4513465</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>1214534</v>
+        <v>1224004</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>288215</v>
+        <v>288335</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
@@ -21243,7 +21243,7 @@
       </c>
       <c r="R21" s="4">
         <f t="shared" si="3"/>
-        <v>4522935</v>
+        <v>4513465</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21264,22 +21264,22 @@
         <v>90</v>
       </c>
       <c r="H22" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I22" s="4">
-        <v>2292535</v>
+        <v>2291411</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="4"/>
-        <v>4891620</v>
+        <v>4882030</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>1466249</v>
+        <v>1475839</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="5"/>
-        <v>251715</v>
+        <v>251835</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
@@ -21290,7 +21290,7 @@
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>4891620</v>
+        <v>4882030</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21311,22 +21311,22 @@
         <v>100</v>
       </c>
       <c r="H23" s="4">
-        <v>2599085</v>
+        <v>2590619</v>
       </c>
       <c r="I23" s="4">
-        <v>2686320</v>
+        <v>2685076</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="4"/>
-        <v>5285405</v>
+        <v>5275695</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>1668940</v>
+        <v>1678650</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="5"/>
-        <v>202691</v>
+        <v>202811</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
@@ -21337,7 +21337,7 @@
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>5285405</v>
+        <v>5275695</v>
       </c>
     </row>
   </sheetData>
@@ -21362,7 +21362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91734A6-3CBC-46E0-AC2D-961E5CB62031}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update non-optimizer ascended data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABCA39B-0FCB-4CCA-8A3A-684FC666B63A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D939769D-0389-4A3D-B0D5-AE35252CAE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="5" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -565,37 +565,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>370257</c:v>
+                  <c:v>368151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>655134</c:v>
+                  <c:v>652074</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1016789</c:v>
+                  <c:v>1012669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1425944</c:v>
+                  <c:v>1420764</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1882599</c:v>
+                  <c:v>1876359</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2386754</c:v>
+                  <c:v>2379454</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2938409</c:v>
+                  <c:v>2930049</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3537564</c:v>
+                  <c:v>3528144</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4184219</c:v>
+                  <c:v>4173739</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4878374</c:v>
+                  <c:v>4866834</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5599937</c:v>
+                  <c:v>5587337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6741,37 +6741,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>370257</c:v>
+                  <c:v>368151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>655134</c:v>
+                  <c:v>652074</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1016789</c:v>
+                  <c:v>1012669</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1425944</c:v>
+                  <c:v>1420764</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1882599</c:v>
+                  <c:v>1876359</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2386754</c:v>
+                  <c:v>2379454</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2938409</c:v>
+                  <c:v>2930049</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3537564</c:v>
+                  <c:v>3528144</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4184219</c:v>
+                  <c:v>4173739</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4878374</c:v>
+                  <c:v>4866834</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5599937</c:v>
+                  <c:v>5587337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16445,8 +16445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B24426-E0C0-44FB-A9C0-0B3FA4280E8F}">
   <dimension ref="B2:R13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -16497,11 +16497,11 @@
         <v>283159</v>
       </c>
       <c r="D3" s="4">
-        <v>87098</v>
+        <v>84992</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>370257</v>
+        <v>368151</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -16518,14 +16518,14 @@
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2327854</v>
+        <v>-2329960</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>370257</v>
+        <v>368151</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
@@ -16540,11 +16540,11 @@
         <v>283159</v>
       </c>
       <c r="D4" s="4">
-        <v>371975</v>
+        <v>368915</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E12" si="0">C4+D4</f>
-        <v>655134</v>
+        <v>652074</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -16561,18 +16561,18 @@
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L13" si="1">E4-J4</f>
-        <v>-2172496</v>
+        <v>-2175556</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>155358</v>
+        <v>154404</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q13" si="2">C4+D4</f>
-        <v>655134</v>
+        <v>652074</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R13" si="3">H4+I4</f>
@@ -16587,11 +16587,11 @@
         <v>283159</v>
       </c>
       <c r="D5" s="4">
-        <v>733630</v>
+        <v>729510</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1016789</v>
+        <v>1012669</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -16608,18 +16608,18 @@
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1996361</v>
+        <v>-2000481</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>176135</v>
+        <v>175075</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>1016789</v>
+        <v>1012669</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
@@ -16634,11 +16634,11 @@
         <v>283159</v>
       </c>
       <c r="D6" s="4">
-        <v>1142785</v>
+        <v>1137605</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1425944</v>
+        <v>1420764</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -16655,18 +16655,18 @@
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-1816526</v>
+        <v>-1821706</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>179835</v>
+        <v>178775</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>1425944</v>
+        <v>1420764</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
@@ -16681,11 +16681,11 @@
         <v>283159</v>
       </c>
       <c r="D7" s="4">
-        <v>1599440</v>
+        <v>1593200</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1882599</v>
+        <v>1876359</v>
       </c>
       <c r="G7" s="2">
         <v>40</v>
@@ -16702,18 +16702,18 @@
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>-1632991</v>
+        <v>-1639231</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>183535</v>
+        <v>182475</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>1882599</v>
+        <v>1876359</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
@@ -16728,11 +16728,11 @@
         <v>283159</v>
       </c>
       <c r="D8" s="4">
-        <v>2103595</v>
+        <v>2096295</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2386754</v>
+        <v>2379454</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
@@ -16749,18 +16749,18 @@
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-1445756</v>
+        <v>-1453056</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>187235</v>
+        <v>186175</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>2386754</v>
+        <v>2379454</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
@@ -16775,11 +16775,11 @@
         <v>283159</v>
       </c>
       <c r="D9" s="4">
-        <v>2655250</v>
+        <v>2646890</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2938409</v>
+        <v>2930049</v>
       </c>
       <c r="G9" s="2">
         <v>60</v>
@@ -16796,18 +16796,18 @@
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>-1254821</v>
+        <v>-1263181</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>190935</v>
+        <v>189875</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>2938409</v>
+        <v>2930049</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
@@ -16822,11 +16822,11 @@
         <v>283159</v>
       </c>
       <c r="D10" s="4">
-        <v>3254405</v>
+        <v>3244985</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3537564</v>
+        <v>3528144</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
@@ -16843,18 +16843,18 @@
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>-1060186</v>
+        <v>-1069606</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>194635</v>
+        <v>193575</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3537564</v>
+        <v>3528144</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
@@ -16869,11 +16869,11 @@
         <v>283159</v>
       </c>
       <c r="D11" s="4">
-        <v>3901060</v>
+        <v>3890580</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>4184219</v>
+        <v>4173739</v>
       </c>
       <c r="G11" s="2">
         <v>80</v>
@@ -16890,18 +16890,18 @@
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>-861851</v>
+        <v>-872331</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>198335</v>
+        <v>197275</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>4184219</v>
+        <v>4173739</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
@@ -16916,11 +16916,11 @@
         <v>283159</v>
       </c>
       <c r="D12" s="4">
-        <v>4595215</v>
+        <v>4583675</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>4878374</v>
+        <v>4866834</v>
       </c>
       <c r="G12" s="2">
         <v>90</v>
@@ -16937,18 +16937,18 @@
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>-659816</v>
+        <v>-671356</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" ref="M12:M13" si="6">L12-L11</f>
-        <v>202035</v>
+        <v>200975</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>4878374</v>
+        <v>4866834</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
@@ -16963,11 +16963,11 @@
         <v>283159</v>
       </c>
       <c r="D13" s="4">
-        <v>5316778</v>
+        <v>5304178</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" ref="E13" si="7">C13+D13</f>
-        <v>5599937</v>
+        <v>5587337</v>
       </c>
       <c r="G13" s="2">
         <v>100</v>
@@ -16984,18 +16984,18 @@
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>-469373</v>
+        <v>-481973</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="6"/>
-        <v>190443</v>
+        <v>189383</v>
       </c>
       <c r="P13" s="2">
         <v>100</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>5599937</v>
+        <v>5587337</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
@@ -20310,7 +20310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update non-optimizer descended data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D939769D-0389-4A3D-B0D5-AE35252CAE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791F02CE-2878-4B62-8727-92DC6905A08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -3342,67 +3342,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>615600</c:v>
+                  <c:v>613312</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1309563</c:v>
+                  <c:v>1304683</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2077878</c:v>
+                  <c:v>2070118</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2843293</c:v>
+                  <c:v>2832653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3148647</c:v>
+                  <c:v>3136855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3224913</c:v>
+                  <c:v>3212833</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3301150</c:v>
+                  <c:v>3288782</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3377358</c:v>
+                  <c:v>3364702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3453537</c:v>
+                  <c:v>3440593</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3529687</c:v>
+                  <c:v>3516455</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3605808</c:v>
+                  <c:v>3592288</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3681900</c:v>
+                  <c:v>3668092</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3757963</c:v>
+                  <c:v>3743867</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3833997</c:v>
+                  <c:v>3819613</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3910002</c:v>
+                  <c:v>3895330</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4365423</c:v>
+                  <c:v>4349023</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5122138</c:v>
+                  <c:v>5102858</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5875953</c:v>
+                  <c:v>5853793</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6626868</c:v>
+                  <c:v>6601828</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7374883</c:v>
+                  <c:v>7346963</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8102698</c:v>
+                  <c:v>8071898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3525,67 +3525,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2698306</c:v>
+                  <c:v>2698124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2829562</c:v>
+                  <c:v>2827742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3017012</c:v>
+                  <c:v>3013372</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3248262</c:v>
+                  <c:v>3242802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3353026</c:v>
+                  <c:v>3346838</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3380312</c:v>
+                  <c:v>3373942</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3408036</c:v>
+                  <c:v>3401484</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3436198</c:v>
+                  <c:v>3429464</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3464798</c:v>
+                  <c:v>3457882</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3493836</c:v>
+                  <c:v>3486738</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3523312</c:v>
+                  <c:v>3516032</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3553226</c:v>
+                  <c:v>3545764</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3583578</c:v>
+                  <c:v>3575934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3614368</c:v>
+                  <c:v>3606542</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3645596</c:v>
+                  <c:v>3637588</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3842162</c:v>
+                  <c:v>3833062</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4204812</c:v>
+                  <c:v>4193892</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4611262</c:v>
+                  <c:v>4598522</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5061512</c:v>
+                  <c:v>5046952</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5555562</c:v>
+                  <c:v>5539182</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6088612</c:v>
+                  <c:v>6070412</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7399,67 +7399,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>615600</c:v>
+                  <c:v>613312</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1309563</c:v>
+                  <c:v>1304683</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2077878</c:v>
+                  <c:v>2070118</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2843293</c:v>
+                  <c:v>2832653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3148647</c:v>
+                  <c:v>3136855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3224913</c:v>
+                  <c:v>3212833</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3301150</c:v>
+                  <c:v>3288782</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3377358</c:v>
+                  <c:v>3364702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3453537</c:v>
+                  <c:v>3440593</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3529687</c:v>
+                  <c:v>3516455</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3605808</c:v>
+                  <c:v>3592288</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3681900</c:v>
+                  <c:v>3668092</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3757963</c:v>
+                  <c:v>3743867</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3833997</c:v>
+                  <c:v>3819613</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3910002</c:v>
+                  <c:v>3895330</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4365423</c:v>
+                  <c:v>4349023</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5122138</c:v>
+                  <c:v>5102858</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5875953</c:v>
+                  <c:v>5853793</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6626868</c:v>
+                  <c:v>6601828</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7374883</c:v>
+                  <c:v>7346963</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8102698</c:v>
+                  <c:v>8071898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7596,67 +7596,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2698306</c:v>
+                  <c:v>2698124</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2829562</c:v>
+                  <c:v>2827742</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3017012</c:v>
+                  <c:v>3013372</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3248262</c:v>
+                  <c:v>3242802</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3353026</c:v>
+                  <c:v>3346838</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3380312</c:v>
+                  <c:v>3373942</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3408036</c:v>
+                  <c:v>3401484</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3436198</c:v>
+                  <c:v>3429464</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3464798</c:v>
+                  <c:v>3457882</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3493836</c:v>
+                  <c:v>3486738</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3523312</c:v>
+                  <c:v>3516032</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3553226</c:v>
+                  <c:v>3545764</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3583578</c:v>
+                  <c:v>3575934</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3614368</c:v>
+                  <c:v>3606542</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3645596</c:v>
+                  <c:v>3637588</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3842162</c:v>
+                  <c:v>3833062</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4204812</c:v>
+                  <c:v>4193892</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4611262</c:v>
+                  <c:v>4598522</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5061512</c:v>
+                  <c:v>5046952</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5555562</c:v>
+                  <c:v>5539182</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6088612</c:v>
+                  <c:v>6070412</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16445,7 +16445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6B24426-E0C0-44FB-A9C0-0B3FA4280E8F}">
   <dimension ref="B2:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -17024,8 +17024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1DA2FE-2DBA-48DD-9085-CD8066E7E300}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17076,11 +17076,11 @@
         <v>283159</v>
       </c>
       <c r="D3" s="4">
-        <v>332441</v>
+        <v>330153</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>615600</v>
+        <v>613312</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -17089,26 +17089,26 @@
         <v>2634890</v>
       </c>
       <c r="I3" s="4">
-        <v>63416</v>
+        <v>63234</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2698306</v>
+        <v>2698124</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2082706</v>
+        <v>-2084812</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>615600</v>
+        <v>613312</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2698306</v>
+        <v>2698124</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17119,11 +17119,11 @@
         <v>283159</v>
       </c>
       <c r="D4" s="4">
-        <v>1026404</v>
+        <v>1021524</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E23" si="0">C4+D4</f>
-        <v>1309563</v>
+        <v>1304683</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -17132,30 +17132,30 @@
         <v>2634890</v>
       </c>
       <c r="I4" s="4">
-        <v>194672</v>
+        <v>192852</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2829562</v>
+        <v>2827742</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>-1519999</v>
+        <v>-1523059</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>562707</v>
+        <v>561753</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
-        <v>1309563</v>
+        <v>1304683</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>2829562</v>
+        <v>2827742</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17166,11 +17166,11 @@
         <v>283159</v>
       </c>
       <c r="D5" s="4">
-        <v>1794719</v>
+        <v>1786959</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>2077878</v>
+        <v>2070118</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -17179,30 +17179,30 @@
         <v>2634890</v>
       </c>
       <c r="I5" s="4">
-        <v>382122</v>
+        <v>378482</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J17" si="4">H5+I5</f>
-        <v>3017012</v>
+        <v>3013372</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-939134</v>
+        <v>-943254</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="5">L5-L4</f>
-        <v>580865</v>
+        <v>579805</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>2077878</v>
+        <v>2070118</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>3017012</v>
+        <v>3013372</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17213,11 +17213,11 @@
         <v>283159</v>
       </c>
       <c r="D6" s="4">
-        <v>2560134</v>
+        <v>2549494</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2843293</v>
+        <v>2832653</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -17226,30 +17226,30 @@
         <v>2634890</v>
       </c>
       <c r="I6" s="4">
-        <v>613372</v>
+        <v>607912</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>3248262</v>
+        <v>3242802</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-404969</v>
+        <v>-410149</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>534165</v>
+        <v>533105</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>2843293</v>
+        <v>2832653</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3248262</v>
+        <v>3242802</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17260,11 +17260,11 @@
         <v>283159</v>
       </c>
       <c r="D7" s="4">
-        <v>2865488</v>
+        <v>2853696</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>3148647</v>
+        <v>3136855</v>
       </c>
       <c r="G7" s="2">
         <v>34</v>
@@ -17273,30 +17273,30 @@
         <v>2634890</v>
       </c>
       <c r="I7" s="4">
-        <v>718136</v>
+        <v>711948</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" ref="J7:J8" si="6">H7+I7</f>
-        <v>3353026</v>
+        <v>3346838</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" ref="L7:L8" si="7">E7-J7</f>
-        <v>-204379</v>
+        <v>-209983</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" ref="M7:M8" si="8">L7-L6</f>
-        <v>200590</v>
+        <v>200166</v>
       </c>
       <c r="P7" s="2">
         <v>34</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" ref="Q7:Q8" si="9">C7+D7</f>
-        <v>3148647</v>
+        <v>3136855</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" ref="R7:R8" si="10">H7+I7</f>
-        <v>3353026</v>
+        <v>3346838</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17307,11 +17307,11 @@
         <v>283159</v>
       </c>
       <c r="D8" s="4">
-        <v>2941754</v>
+        <v>2929674</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3224913</v>
+        <v>3212833</v>
       </c>
       <c r="G8" s="2">
         <v>35</v>
@@ -17320,30 +17320,30 @@
         <v>2634890</v>
       </c>
       <c r="I8" s="4">
-        <v>745422</v>
+        <v>739052</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="6"/>
-        <v>3380312</v>
+        <v>3373942</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="7"/>
-        <v>-155399</v>
+        <v>-161109</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="8"/>
-        <v>48980</v>
+        <v>48874</v>
       </c>
       <c r="P8" s="2">
         <v>35</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="9"/>
-        <v>3224913</v>
+        <v>3212833</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="10"/>
-        <v>3380312</v>
+        <v>3373942</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17354,11 +17354,11 @@
         <v>283159</v>
       </c>
       <c r="D9" s="4">
-        <v>3017991</v>
+        <v>3005623</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3301150</v>
+        <v>3288782</v>
       </c>
       <c r="G9" s="2">
         <v>36</v>
@@ -17367,30 +17367,30 @@
         <v>2634890</v>
       </c>
       <c r="I9" s="4">
-        <v>773146</v>
+        <v>766594</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>3408036</v>
+        <v>3401484</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" ref="L9:L12" si="11">E9-J9</f>
-        <v>-106886</v>
+        <v>-112702</v>
       </c>
       <c r="M9" s="5">
         <f>L9-L8</f>
-        <v>48513</v>
+        <v>48407</v>
       </c>
       <c r="P9" s="2">
         <v>36</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>3301150</v>
+        <v>3288782</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>3408036</v>
+        <v>3401484</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17401,11 +17401,11 @@
         <v>283159</v>
       </c>
       <c r="D10" s="4">
-        <v>3094199</v>
+        <v>3081543</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3377358</v>
+        <v>3364702</v>
       </c>
       <c r="G10" s="2">
         <v>37</v>
@@ -17414,30 +17414,30 @@
         <v>2634890</v>
       </c>
       <c r="I10" s="4">
-        <v>801308</v>
+        <v>794574</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>3436198</v>
+        <v>3429464</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="11"/>
-        <v>-58840</v>
+        <v>-64762</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" ref="M10:M13" si="12">L10-L9</f>
-        <v>48046</v>
+        <v>47940</v>
       </c>
       <c r="P10" s="2">
         <v>37</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3377358</v>
+        <v>3364702</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>3436198</v>
+        <v>3429464</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17448,11 +17448,11 @@
         <v>283159</v>
       </c>
       <c r="D11" s="4">
-        <v>3170378</v>
+        <v>3157434</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3453537</v>
+        <v>3440593</v>
       </c>
       <c r="G11" s="2">
         <v>38</v>
@@ -17461,30 +17461,30 @@
         <v>2634890</v>
       </c>
       <c r="I11" s="4">
-        <v>829908</v>
+        <v>822992</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>3464798</v>
+        <v>3457882</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="11"/>
-        <v>-11261</v>
+        <v>-17289</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="12"/>
-        <v>47579</v>
+        <v>47473</v>
       </c>
       <c r="P11" s="2">
         <v>38</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3453537</v>
+        <v>3440593</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>3464798</v>
+        <v>3457882</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17496,11 +17496,11 @@
         <v>283159</v>
       </c>
       <c r="D12" s="4">
-        <v>3246528</v>
+        <v>3233296</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3529687</v>
+        <v>3516455</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2">
@@ -17510,31 +17510,31 @@
         <v>2634890</v>
       </c>
       <c r="I12" s="4">
-        <v>858946</v>
+        <v>851848</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>3493836</v>
+        <v>3486738</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="4">
         <f t="shared" si="11"/>
-        <v>35851</v>
+        <v>29717</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="12"/>
-        <v>47112</v>
+        <v>47006</v>
       </c>
       <c r="P12" s="2">
         <v>39</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>3529687</v>
+        <v>3516455</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>3493836</v>
+        <v>3486738</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17545,11 +17545,11 @@
         <v>283159</v>
       </c>
       <c r="D13" s="4">
-        <v>3322649</v>
+        <v>3309129</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>3605808</v>
+        <v>3592288</v>
       </c>
       <c r="G13" s="2">
         <v>40</v>
@@ -17558,30 +17558,30 @@
         <v>2634890</v>
       </c>
       <c r="I13" s="4">
-        <v>888422</v>
+        <v>881142</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>3523312</v>
+        <v>3516032</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>82496</v>
+        <v>76256</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="12"/>
-        <v>46645</v>
+        <v>46539</v>
       </c>
       <c r="P13" s="2">
         <v>40</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>3605808</v>
+        <v>3592288</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>3523312</v>
+        <v>3516032</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17592,11 +17592,11 @@
         <v>283159</v>
       </c>
       <c r="D14" s="4">
-        <v>3398741</v>
+        <v>3384933</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3681900</v>
+        <v>3668092</v>
       </c>
       <c r="G14" s="2">
         <v>41</v>
@@ -17605,30 +17605,30 @@
         <v>2634890</v>
       </c>
       <c r="I14" s="4">
-        <v>918336</v>
+        <v>910874</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="4"/>
-        <v>3553226</v>
+        <v>3545764</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="1"/>
-        <v>128674</v>
+        <v>122328</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="5"/>
-        <v>46178</v>
+        <v>46072</v>
       </c>
       <c r="P14" s="2">
         <v>41</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>3681900</v>
+        <v>3668092</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>3553226</v>
+        <v>3545764</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17639,11 +17639,11 @@
         <v>283159</v>
       </c>
       <c r="D15" s="4">
-        <v>3474804</v>
+        <v>3460708</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>3757963</v>
+        <v>3743867</v>
       </c>
       <c r="G15" s="2">
         <v>42</v>
@@ -17652,30 +17652,30 @@
         <v>2634890</v>
       </c>
       <c r="I15" s="4">
-        <v>948688</v>
+        <v>941044</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="4"/>
-        <v>3583578</v>
+        <v>3575934</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="1"/>
-        <v>174385</v>
+        <v>167933</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="5"/>
-        <v>45711</v>
+        <v>45605</v>
       </c>
       <c r="P15" s="2">
         <v>42</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>3757963</v>
+        <v>3743867</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>3583578</v>
+        <v>3575934</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17686,11 +17686,11 @@
         <v>283159</v>
       </c>
       <c r="D16" s="4">
-        <v>3550838</v>
+        <v>3536454</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>3833997</v>
+        <v>3819613</v>
       </c>
       <c r="G16" s="2">
         <v>43</v>
@@ -17699,30 +17699,30 @@
         <v>2634890</v>
       </c>
       <c r="I16" s="4">
-        <v>979478</v>
+        <v>971652</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="4"/>
-        <v>3614368</v>
+        <v>3606542</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="1"/>
-        <v>219629</v>
+        <v>213071</v>
       </c>
       <c r="M16" s="5">
         <f>L16-L15</f>
-        <v>45244</v>
+        <v>45138</v>
       </c>
       <c r="P16" s="2">
         <v>43</v>
       </c>
       <c r="Q16" s="4">
         <f t="shared" si="2"/>
-        <v>3833997</v>
+        <v>3819613</v>
       </c>
       <c r="R16" s="4">
         <f t="shared" si="3"/>
-        <v>3614368</v>
+        <v>3606542</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17733,11 +17733,11 @@
         <v>283159</v>
       </c>
       <c r="D17" s="4">
-        <v>3626843</v>
+        <v>3612171</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>3910002</v>
+        <v>3895330</v>
       </c>
       <c r="G17" s="2">
         <v>44</v>
@@ -17746,30 +17746,30 @@
         <v>2634890</v>
       </c>
       <c r="I17" s="4">
-        <v>1010706</v>
+        <v>1002698</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="4"/>
-        <v>3645596</v>
+        <v>3637588</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" ref="L17:L18" si="13">E17-J17</f>
-        <v>264406</v>
+        <v>257742</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" ref="M17:M18" si="14">L17-L16</f>
-        <v>44777</v>
+        <v>44671</v>
       </c>
       <c r="P17" s="2">
         <v>44</v>
       </c>
       <c r="Q17" s="4">
         <f t="shared" ref="Q17" si="15">C17+D17</f>
-        <v>3910002</v>
+        <v>3895330</v>
       </c>
       <c r="R17" s="4">
         <f t="shared" ref="R17" si="16">H17+I17</f>
-        <v>3645596</v>
+        <v>3637588</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17780,11 +17780,11 @@
         <v>283159</v>
       </c>
       <c r="D18" s="4">
-        <v>4082264</v>
+        <v>4065864</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>4365423</v>
+        <v>4349023</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
@@ -17793,30 +17793,30 @@
         <v>2634890</v>
       </c>
       <c r="I18" s="4">
-        <v>1207272</v>
+        <v>1198172</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" ref="J18:J23" si="17">H18+I18</f>
-        <v>3842162</v>
+        <v>3833062</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="13"/>
-        <v>523261</v>
+        <v>515961</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="14"/>
-        <v>258855</v>
+        <v>258219</v>
       </c>
       <c r="P18" s="2">
         <v>50</v>
       </c>
       <c r="Q18" s="4">
         <f t="shared" si="2"/>
-        <v>4365423</v>
+        <v>4349023</v>
       </c>
       <c r="R18" s="4">
         <f t="shared" si="3"/>
-        <v>3842162</v>
+        <v>3833062</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17827,11 +17827,11 @@
         <v>283159</v>
       </c>
       <c r="D19" s="4">
-        <v>4838979</v>
+        <v>4819699</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>5122138</v>
+        <v>5102858</v>
       </c>
       <c r="G19" s="2">
         <v>60</v>
@@ -17840,30 +17840,30 @@
         <v>2634890</v>
       </c>
       <c r="I19" s="4">
-        <v>1569922</v>
+        <v>1559002</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="17"/>
-        <v>4204812</v>
+        <v>4193892</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" si="1"/>
-        <v>917326</v>
+        <v>908966</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="5"/>
-        <v>394065</v>
+        <v>393005</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="2"/>
-        <v>5122138</v>
+        <v>5102858</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>4204812</v>
+        <v>4193892</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17874,11 +17874,11 @@
         <v>283159</v>
       </c>
       <c r="D20" s="4">
-        <v>5592794</v>
+        <v>5570634</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>5875953</v>
+        <v>5853793</v>
       </c>
       <c r="G20" s="2">
         <v>70</v>
@@ -17887,30 +17887,30 @@
         <v>2634890</v>
       </c>
       <c r="I20" s="4">
-        <v>1976372</v>
+        <v>1963632</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="17"/>
-        <v>4611262</v>
+        <v>4598522</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>1264691</v>
+        <v>1255271</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="5"/>
-        <v>347365</v>
+        <v>346305</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="2"/>
-        <v>5875953</v>
+        <v>5853793</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>4611262</v>
+        <v>4598522</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17921,11 +17921,11 @@
         <v>283159</v>
       </c>
       <c r="D21" s="4">
-        <v>6343709</v>
+        <v>6318669</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>6626868</v>
+        <v>6601828</v>
       </c>
       <c r="G21" s="2">
         <v>80</v>
@@ -17934,30 +17934,30 @@
         <v>2634890</v>
       </c>
       <c r="I21" s="4">
-        <v>2426622</v>
+        <v>2412062</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="17"/>
-        <v>5061512</v>
+        <v>5046952</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>1565356</v>
+        <v>1554876</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>300665</v>
+        <v>299605</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="2"/>
-        <v>6626868</v>
+        <v>6601828</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="3"/>
-        <v>5061512</v>
+        <v>5046952</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -17968,11 +17968,11 @@
         <v>283159</v>
       </c>
       <c r="D22" s="4">
-        <v>7091724</v>
+        <v>7063804</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>7374883</v>
+        <v>7346963</v>
       </c>
       <c r="G22" s="2">
         <v>90</v>
@@ -17981,30 +17981,30 @@
         <v>2634890</v>
       </c>
       <c r="I22" s="4">
-        <v>2920672</v>
+        <v>2904292</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="17"/>
-        <v>5555562</v>
+        <v>5539182</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>1819321</v>
+        <v>1807781</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="5"/>
-        <v>253965</v>
+        <v>252905</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="2"/>
-        <v>7374883</v>
+        <v>7346963</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>5555562</v>
+        <v>5539182</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18015,11 +18015,11 @@
         <v>283159</v>
       </c>
       <c r="D23" s="4">
-        <v>7819539</v>
+        <v>7788739</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>8102698</v>
+        <v>8071898</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
@@ -18028,30 +18028,30 @@
         <v>2634890</v>
       </c>
       <c r="I23" s="4">
-        <v>3453722</v>
+        <v>3435522</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="17"/>
-        <v>6088612</v>
+        <v>6070412</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>2014086</v>
+        <v>2001486</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="5"/>
-        <v>194765</v>
+        <v>193705</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="2"/>
-        <v>8102698</v>
+        <v>8071898</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>6088612</v>
+        <v>6070412</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 200 runs ascended data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{791F02CE-2878-4B62-8727-92DC6905A08C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C758965-E8BD-44A8-A264-ED4DB3B3B053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -4046,37 +4046,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>367760</c:v>
+                  <c:v>365654</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640631</c:v>
+                  <c:v>637571</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>979161</c:v>
+                  <c:v>975041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1354891</c:v>
+                  <c:v>1349711</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1767821</c:v>
+                  <c:v>1761581</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2217951</c:v>
+                  <c:v>2210651</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2705281</c:v>
+                  <c:v>2696921</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3229811</c:v>
+                  <c:v>3220391</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3791541</c:v>
+                  <c:v>3781061</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4390471</c:v>
+                  <c:v>4378931</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5006526</c:v>
+                  <c:v>4993926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8119,37 +8119,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>367760</c:v>
+                  <c:v>365654</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640631</c:v>
+                  <c:v>637571</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>979161</c:v>
+                  <c:v>975041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1354891</c:v>
+                  <c:v>1349711</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1767821</c:v>
+                  <c:v>1761581</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2217951</c:v>
+                  <c:v>2210651</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2705281</c:v>
+                  <c:v>2696921</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3229811</c:v>
+                  <c:v>3220391</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3791541</c:v>
+                  <c:v>3781061</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4390471</c:v>
+                  <c:v>4378931</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5006526</c:v>
+                  <c:v>4993926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -17024,7 +17024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1DA2FE-2DBA-48DD-9085-CD8066E7E300}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -18076,8 +18076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F68343B-F0B9-4DF5-8EBB-C222891744B9}">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18128,11 +18128,11 @@
         <v>281777</v>
       </c>
       <c r="D3" s="4">
-        <v>85983</v>
+        <v>83877</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>367760</v>
+        <v>365654</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -18149,14 +18149,14 @@
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2286339</v>
+        <v>-2288445</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>367760</v>
+        <v>365654</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
@@ -18171,11 +18171,11 @@
         <v>281777</v>
       </c>
       <c r="D4" s="4">
-        <v>358854</v>
+        <v>355794</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E13" si="0">C4+D4</f>
-        <v>640631</v>
+        <v>637571</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -18192,18 +18192,18 @@
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L13" si="1">E4-J4</f>
-        <v>-2131917</v>
+        <v>-2134977</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>154422</v>
+        <v>153468</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q13" si="2">C4+D4</f>
-        <v>640631</v>
+        <v>637571</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R13" si="3">H4+I4</f>
@@ -18218,11 +18218,11 @@
         <v>281777</v>
       </c>
       <c r="D5" s="4">
-        <v>697384</v>
+        <v>693264</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>979161</v>
+        <v>975041</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -18239,18 +18239,18 @@
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1955492</v>
+        <v>-1959612</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>176425</v>
+        <v>175365</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>979161</v>
+        <v>975041</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
@@ -18265,11 +18265,11 @@
         <v>281777</v>
       </c>
       <c r="D6" s="4">
-        <v>1073114</v>
+        <v>1067934</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1354891</v>
+        <v>1349711</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -18286,18 +18286,18 @@
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-1773967</v>
+        <v>-1779147</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>181525</v>
+        <v>180465</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>1354891</v>
+        <v>1349711</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
@@ -18312,11 +18312,11 @@
         <v>281777</v>
       </c>
       <c r="D7" s="4">
-        <v>1486044</v>
+        <v>1479804</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1767821</v>
+        <v>1761581</v>
       </c>
       <c r="G7" s="2">
         <v>40</v>
@@ -18333,18 +18333,18 @@
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>-1587342</v>
+        <v>-1593582</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>186625</v>
+        <v>185565</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>1767821</v>
+        <v>1761581</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
@@ -18359,11 +18359,11 @@
         <v>281777</v>
       </c>
       <c r="D8" s="4">
-        <v>1936174</v>
+        <v>1928874</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2217951</v>
+        <v>2210651</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
@@ -18380,18 +18380,18 @@
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-1395617</v>
+        <v>-1402917</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>191725</v>
+        <v>190665</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>2217951</v>
+        <v>2210651</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
@@ -18406,11 +18406,11 @@
         <v>281777</v>
       </c>
       <c r="D9" s="4">
-        <v>2423504</v>
+        <v>2415144</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2705281</v>
+        <v>2696921</v>
       </c>
       <c r="G9" s="2">
         <v>60</v>
@@ -18427,18 +18427,18 @@
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>-1198792</v>
+        <v>-1207152</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>196825</v>
+        <v>195765</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>2705281</v>
+        <v>2696921</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
@@ -18453,11 +18453,11 @@
         <v>281777</v>
       </c>
       <c r="D10" s="4">
-        <v>2948034</v>
+        <v>2938614</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3229811</v>
+        <v>3220391</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
@@ -18474,18 +18474,18 @@
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>-996867</v>
+        <v>-1006287</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>201925</v>
+        <v>200865</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3229811</v>
+        <v>3220391</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
@@ -18500,11 +18500,11 @@
         <v>281777</v>
       </c>
       <c r="D11" s="4">
-        <v>3509764</v>
+        <v>3499284</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3791541</v>
+        <v>3781061</v>
       </c>
       <c r="G11" s="2">
         <v>80</v>
@@ -18521,18 +18521,18 @@
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>-789842</v>
+        <v>-800322</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>207025</v>
+        <v>205965</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3791541</v>
+        <v>3781061</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
@@ -18547,11 +18547,11 @@
         <v>281777</v>
       </c>
       <c r="D12" s="4">
-        <v>4108694</v>
+        <v>4097154</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>4390471</v>
+        <v>4378931</v>
       </c>
       <c r="G12" s="2">
         <v>90</v>
@@ -18568,18 +18568,18 @@
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>-577717</v>
+        <v>-589257</v>
       </c>
       <c r="M12" s="5">
         <f>L12-L11</f>
-        <v>212125</v>
+        <v>211065</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>4390471</v>
+        <v>4378931</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
@@ -18594,11 +18594,11 @@
         <v>281777</v>
       </c>
       <c r="D13" s="4">
-        <v>4724749</v>
+        <v>4712149</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>5006526</v>
+        <v>4993926</v>
       </c>
       <c r="G13" s="2">
         <v>100</v>
@@ -18615,18 +18615,18 @@
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>-375767</v>
+        <v>-388367</v>
       </c>
       <c r="M13" s="5">
         <f>L13-L12</f>
-        <v>201950</v>
+        <v>200890</v>
       </c>
       <c r="P13" s="2">
         <v>100</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>5006526</v>
+        <v>4993926</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Update 200 runs descended data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C758965-E8BD-44A8-A264-ED4DB3B3B053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F98BC7-41A1-4830-9977-A77D68461AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -1215,67 +1215,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604286</c:v>
+                  <c:v>602117</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1209869</c:v>
+                  <c:v>1206179</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1876469</c:v>
+                  <c:v>1871089</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2536469</c:v>
+                  <c:v>2529399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3124826</c:v>
+                  <c:v>3116235</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3189869</c:v>
+                  <c:v>3181109</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3254846</c:v>
+                  <c:v>3245917</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3319757</c:v>
+                  <c:v>3310659</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3384602</c:v>
+                  <c:v>3375335</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3449381</c:v>
+                  <c:v>3439945</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3514094</c:v>
+                  <c:v>3504489</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3578741</c:v>
+                  <c:v>3568967</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3643322</c:v>
+                  <c:v>3633379</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3707837</c:v>
+                  <c:v>3697725</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3772286</c:v>
+                  <c:v>3762005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3836669</c:v>
+                  <c:v>3826219</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4476869</c:v>
+                  <c:v>4464729</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5110469</c:v>
+                  <c:v>5096639</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5737469</c:v>
+                  <c:v>5721949</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6357869</c:v>
+                  <c:v>6340659</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6954345</c:v>
+                  <c:v>6935445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1412,67 +1412,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2654148</c:v>
+                  <c:v>2654085</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2772030</c:v>
+                  <c:v>2771400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2931415</c:v>
+                  <c:v>2930155</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3120700</c:v>
+                  <c:v>3118810</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3316621</c:v>
+                  <c:v>3314164</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3339885</c:v>
+                  <c:v>3337365</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3363448</c:v>
+                  <c:v>3360865</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3387310</c:v>
+                  <c:v>3384664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3411471</c:v>
+                  <c:v>3408762</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3435931</c:v>
+                  <c:v>3433159</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3460690</c:v>
+                  <c:v>3457855</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3485748</c:v>
+                  <c:v>3482850</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3511105</c:v>
+                  <c:v>3508144</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3536761</c:v>
+                  <c:v>3533737</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3562716</c:v>
+                  <c:v>3559629</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3588970</c:v>
+                  <c:v>3585820</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3867955</c:v>
+                  <c:v>3864175</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4176840</c:v>
+                  <c:v>4172430</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4515625</c:v>
+                  <c:v>4510585</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4884310</c:v>
+                  <c:v>4878640</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5278095</c:v>
+                  <c:v>5271795</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4690,67 +4690,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604286</c:v>
+                  <c:v>602117</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1209869</c:v>
+                  <c:v>1206179</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1876469</c:v>
+                  <c:v>1871089</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2536469</c:v>
+                  <c:v>2529399</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3124826</c:v>
+                  <c:v>3116235</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3189869</c:v>
+                  <c:v>3181109</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3254846</c:v>
+                  <c:v>3245917</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3319757</c:v>
+                  <c:v>3310659</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3384602</c:v>
+                  <c:v>3375335</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3449381</c:v>
+                  <c:v>3439945</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3514094</c:v>
+                  <c:v>3504489</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3578741</c:v>
+                  <c:v>3568967</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3643322</c:v>
+                  <c:v>3633379</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3707837</c:v>
+                  <c:v>3697725</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3772286</c:v>
+                  <c:v>3762005</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3836669</c:v>
+                  <c:v>3826219</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4476869</c:v>
+                  <c:v>4464729</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5110469</c:v>
+                  <c:v>5096639</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5737469</c:v>
+                  <c:v>5721949</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6357869</c:v>
+                  <c:v>6340659</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6954345</c:v>
+                  <c:v>6935445</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4873,67 +4873,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2654148</c:v>
+                  <c:v>2654085</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2772030</c:v>
+                  <c:v>2771400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2931415</c:v>
+                  <c:v>2930155</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3120700</c:v>
+                  <c:v>3118810</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3316621</c:v>
+                  <c:v>3314164</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3339885</c:v>
+                  <c:v>3337365</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3363448</c:v>
+                  <c:v>3360865</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3387310</c:v>
+                  <c:v>3384664</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3411471</c:v>
+                  <c:v>3408762</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3435931</c:v>
+                  <c:v>3433159</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3460690</c:v>
+                  <c:v>3457855</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3485748</c:v>
+                  <c:v>3482850</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3511105</c:v>
+                  <c:v>3508144</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3536761</c:v>
+                  <c:v>3533737</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3562716</c:v>
+                  <c:v>3559629</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3588970</c:v>
+                  <c:v>3585820</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3867955</c:v>
+                  <c:v>3864175</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4176840</c:v>
+                  <c:v>4172430</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4515625</c:v>
+                  <c:v>4510585</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4884310</c:v>
+                  <c:v>4878640</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5278095</c:v>
+                  <c:v>5271795</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18076,7 +18076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F68343B-F0B9-4DF5-8EBB-C222891744B9}">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -18667,8 +18667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06EBE3-BB9C-4874-A95E-FF2651C40304}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18719,11 +18719,11 @@
         <v>281777</v>
       </c>
       <c r="D3" s="4">
-        <v>322509</v>
+        <v>320340</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>604286</v>
+        <v>602117</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -18732,26 +18732,26 @@
         <v>2591819</v>
       </c>
       <c r="I3" s="4">
-        <v>62329</v>
+        <v>62266</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2654148</v>
+        <v>2654085</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2049862</v>
+        <v>-2051968</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>604286</v>
+        <v>602117</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2654148</v>
+        <v>2654085</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18762,11 +18762,11 @@
         <v>281777</v>
       </c>
       <c r="D4" s="4">
-        <v>928092</v>
+        <v>924402</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E23" si="0">C4+D4</f>
-        <v>1209869</v>
+        <v>1206179</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -18775,30 +18775,30 @@
         <v>2591819</v>
       </c>
       <c r="I4" s="4">
-        <v>180211</v>
+        <v>179581</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2772030</v>
+        <v>2771400</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>-1562161</v>
+        <v>-1565221</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>487701</v>
+        <v>486747</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
-        <v>1209869</v>
+        <v>1206179</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>2772030</v>
+        <v>2771400</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18809,11 +18809,11 @@
         <v>281777</v>
       </c>
       <c r="D5" s="4">
-        <v>1594692</v>
+        <v>1589312</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1876469</v>
+        <v>1871089</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -18822,30 +18822,30 @@
         <v>2591819</v>
       </c>
       <c r="I5" s="4">
-        <v>339596</v>
+        <v>338336</v>
       </c>
       <c r="J5" s="4">
         <f>H5+I5</f>
-        <v>2931415</v>
+        <v>2930155</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1054946</v>
+        <v>-1059066</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="4">L5-L4</f>
-        <v>507215</v>
+        <v>506155</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>1876469</v>
+        <v>1871089</v>
       </c>
       <c r="R5" s="4">
         <f>H5+I5</f>
-        <v>2931415</v>
+        <v>2930155</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18856,11 +18856,11 @@
         <v>281777</v>
       </c>
       <c r="D6" s="4">
-        <v>2254692</v>
+        <v>2247622</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2536469</v>
+        <v>2529399</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -18869,30 +18869,30 @@
         <v>2591819</v>
       </c>
       <c r="I6" s="4">
-        <v>528881</v>
+        <v>526991</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" ref="J6:J23" si="5">H6+I6</f>
-        <v>3120700</v>
+        <v>3118810</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-584231</v>
+        <v>-589411</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>470715</v>
+        <v>469655</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>2536469</v>
+        <v>2529399</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3120700</v>
+        <v>3118810</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18903,11 +18903,11 @@
         <v>281777</v>
       </c>
       <c r="D7" s="4">
-        <v>2843049</v>
+        <v>2834458</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>3124826</v>
+        <v>3116235</v>
       </c>
       <c r="G7" s="2">
         <v>39</v>
@@ -18916,30 +18916,30 @@
         <v>2591819</v>
       </c>
       <c r="I7" s="4">
-        <v>724802</v>
+        <v>722345</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="5"/>
-        <v>3316621</v>
+        <v>3314164</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" ref="L7:L8" si="6">E7-J7</f>
-        <v>-191795</v>
+        <v>-197929</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" ref="M7:M8" si="7">L7-L6</f>
-        <v>392436</v>
+        <v>391482</v>
       </c>
       <c r="P7" s="2">
         <v>39</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" ref="Q7" si="8">C7+D7</f>
-        <v>3124826</v>
+        <v>3116235</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" ref="R7" si="9">H7+I7</f>
-        <v>3316621</v>
+        <v>3314164</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18950,11 +18950,11 @@
         <v>281777</v>
       </c>
       <c r="D8" s="4">
-        <v>2908092</v>
+        <v>2899332</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3189869</v>
+        <v>3181109</v>
       </c>
       <c r="G8" s="2">
         <v>40</v>
@@ -18963,30 +18963,30 @@
         <v>2591819</v>
       </c>
       <c r="I8" s="4">
-        <v>748066</v>
+        <v>745546</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="5"/>
-        <v>3339885</v>
+        <v>3337365</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="6"/>
-        <v>-150016</v>
+        <v>-156256</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="7"/>
-        <v>41779</v>
+        <v>41673</v>
       </c>
       <c r="P8" s="2">
         <v>40</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>3189869</v>
+        <v>3181109</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>3339885</v>
+        <v>3337365</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -18997,11 +18997,11 @@
         <v>281777</v>
       </c>
       <c r="D9" s="4">
-        <v>2973069</v>
+        <v>2964140</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3254846</v>
+        <v>3245917</v>
       </c>
       <c r="G9" s="2">
         <v>41</v>
@@ -19010,30 +19010,30 @@
         <v>2591819</v>
       </c>
       <c r="I9" s="4">
-        <v>771629</v>
+        <v>769046</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="5"/>
-        <v>3363448</v>
+        <v>3360865</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" ref="L9" si="10">E9-J9</f>
-        <v>-108602</v>
+        <v>-114948</v>
       </c>
       <c r="M9" s="5">
         <f>L9-L8</f>
-        <v>41414</v>
+        <v>41308</v>
       </c>
       <c r="P9" s="2">
         <v>41</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>3254846</v>
+        <v>3245917</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>3363448</v>
+        <v>3360865</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19044,11 +19044,11 @@
         <v>281777</v>
       </c>
       <c r="D10" s="4">
-        <v>3037980</v>
+        <v>3028882</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3319757</v>
+        <v>3310659</v>
       </c>
       <c r="G10" s="2">
         <v>42</v>
@@ -19057,30 +19057,30 @@
         <v>2591819</v>
       </c>
       <c r="I10" s="4">
-        <v>795491</v>
+        <v>792845</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="5"/>
-        <v>3387310</v>
+        <v>3384664</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" ref="L10:L16" si="11">E10-J10</f>
-        <v>-67553</v>
+        <v>-74005</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" ref="M10:M16" si="12">L10-L9</f>
-        <v>41049</v>
+        <v>40943</v>
       </c>
       <c r="P10" s="2">
         <v>42</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3319757</v>
+        <v>3310659</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>3387310</v>
+        <v>3384664</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19091,11 +19091,11 @@
         <v>281777</v>
       </c>
       <c r="D11" s="4">
-        <v>3102825</v>
+        <v>3093558</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3384602</v>
+        <v>3375335</v>
       </c>
       <c r="G11" s="2">
         <v>43</v>
@@ -19104,30 +19104,30 @@
         <v>2591819</v>
       </c>
       <c r="I11" s="4">
-        <v>819652</v>
+        <v>816943</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="5"/>
-        <v>3411471</v>
+        <v>3408762</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="11"/>
-        <v>-26869</v>
+        <v>-33427</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" si="12"/>
-        <v>40684</v>
+        <v>40578</v>
       </c>
       <c r="P11" s="2">
         <v>43</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3384602</v>
+        <v>3375335</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>3411471</v>
+        <v>3408762</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19139,11 +19139,11 @@
         <v>281777</v>
       </c>
       <c r="D12" s="4">
-        <v>3167604</v>
+        <v>3158168</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3449381</v>
+        <v>3439945</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2">
@@ -19153,31 +19153,31 @@
         <v>2591819</v>
       </c>
       <c r="I12" s="4">
-        <v>844112</v>
+        <v>841340</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="5"/>
-        <v>3435931</v>
+        <v>3433159</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="4">
         <f t="shared" si="11"/>
-        <v>13450</v>
+        <v>6786</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="12"/>
-        <v>40319</v>
+        <v>40213</v>
       </c>
       <c r="P12" s="2">
         <v>44</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>3449381</v>
+        <v>3439945</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>3435931</v>
+        <v>3433159</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19188,11 +19188,11 @@
         <v>281777</v>
       </c>
       <c r="D13" s="4">
-        <v>3232317</v>
+        <v>3222712</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>3514094</v>
+        <v>3504489</v>
       </c>
       <c r="G13" s="2">
         <v>45</v>
@@ -19201,30 +19201,30 @@
         <v>2591819</v>
       </c>
       <c r="I13" s="4">
-        <v>868871</v>
+        <v>866036</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="5"/>
-        <v>3460690</v>
+        <v>3457855</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="11"/>
-        <v>53404</v>
+        <v>46634</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="12"/>
-        <v>39954</v>
+        <v>39848</v>
       </c>
       <c r="P13" s="2">
         <v>45</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>3514094</v>
+        <v>3504489</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>3460690</v>
+        <v>3457855</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19235,11 +19235,11 @@
         <v>281777</v>
       </c>
       <c r="D14" s="4">
-        <v>3296964</v>
+        <v>3287190</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3578741</v>
+        <v>3568967</v>
       </c>
       <c r="G14" s="2">
         <v>46</v>
@@ -19248,30 +19248,30 @@
         <v>2591819</v>
       </c>
       <c r="I14" s="4">
-        <v>893929</v>
+        <v>891031</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="5"/>
-        <v>3485748</v>
+        <v>3482850</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" si="11"/>
-        <v>92993</v>
+        <v>86117</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="12"/>
-        <v>39589</v>
+        <v>39483</v>
       </c>
       <c r="P14" s="2">
         <v>46</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>3578741</v>
+        <v>3568967</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>3485748</v>
+        <v>3482850</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19282,11 +19282,11 @@
         <v>281777</v>
       </c>
       <c r="D15" s="4">
-        <v>3361545</v>
+        <v>3351602</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>3643322</v>
+        <v>3633379</v>
       </c>
       <c r="G15" s="2">
         <v>47</v>
@@ -19295,30 +19295,30 @@
         <v>2591819</v>
       </c>
       <c r="I15" s="4">
-        <v>919286</v>
+        <v>916325</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="5"/>
-        <v>3511105</v>
+        <v>3508144</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="11"/>
-        <v>132217</v>
+        <v>125235</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="12"/>
-        <v>39224</v>
+        <v>39118</v>
       </c>
       <c r="P15" s="2">
         <v>47</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>3643322</v>
+        <v>3633379</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>3511105</v>
+        <v>3508144</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19329,11 +19329,11 @@
         <v>281777</v>
       </c>
       <c r="D16" s="4">
-        <v>3426060</v>
+        <v>3415948</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>3707837</v>
+        <v>3697725</v>
       </c>
       <c r="G16" s="2">
         <v>48</v>
@@ -19342,30 +19342,30 @@
         <v>2591819</v>
       </c>
       <c r="I16" s="4">
-        <v>944942</v>
+        <v>941918</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="5"/>
-        <v>3536761</v>
+        <v>3533737</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="11"/>
-        <v>171076</v>
+        <v>163988</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" si="12"/>
-        <v>38859</v>
+        <v>38753</v>
       </c>
       <c r="P16" s="2">
         <v>48</v>
       </c>
       <c r="Q16" s="4">
         <f t="shared" si="2"/>
-        <v>3707837</v>
+        <v>3697725</v>
       </c>
       <c r="R16" s="4">
         <f t="shared" si="3"/>
-        <v>3536761</v>
+        <v>3533737</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19376,11 +19376,11 @@
         <v>281777</v>
       </c>
       <c r="D17" s="4">
-        <v>3490509</v>
+        <v>3480228</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>3772286</v>
+        <v>3762005</v>
       </c>
       <c r="G17" s="2">
         <v>49</v>
@@ -19389,30 +19389,30 @@
         <v>2591819</v>
       </c>
       <c r="I17" s="4">
-        <v>970897</v>
+        <v>967810</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="5"/>
-        <v>3562716</v>
+        <v>3559629</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" ref="L17:L18" si="13">E17-J17</f>
-        <v>209570</v>
+        <v>202376</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" ref="M17:M19" si="14">L17-L16</f>
-        <v>38494</v>
+        <v>38388</v>
       </c>
       <c r="P17" s="2">
         <v>49</v>
       </c>
       <c r="Q17" s="4">
         <f t="shared" ref="Q17" si="15">C17+D17</f>
-        <v>3772286</v>
+        <v>3762005</v>
       </c>
       <c r="R17" s="4">
         <f t="shared" ref="R17" si="16">H17+I17</f>
-        <v>3562716</v>
+        <v>3559629</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19423,11 +19423,11 @@
         <v>281777</v>
       </c>
       <c r="D18" s="4">
-        <v>3554892</v>
+        <v>3544442</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>3836669</v>
+        <v>3826219</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
@@ -19436,30 +19436,30 @@
         <v>2591819</v>
       </c>
       <c r="I18" s="4">
-        <v>997151</v>
+        <v>994001</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="5"/>
-        <v>3588970</v>
+        <v>3585820</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="13"/>
-        <v>247699</v>
+        <v>240399</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="14"/>
-        <v>38129</v>
+        <v>38023</v>
       </c>
       <c r="P18" s="2">
         <v>50</v>
       </c>
       <c r="Q18" s="4">
         <f t="shared" si="2"/>
-        <v>3836669</v>
+        <v>3826219</v>
       </c>
       <c r="R18" s="4">
         <f t="shared" si="3"/>
-        <v>3588970</v>
+        <v>3585820</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19470,11 +19470,11 @@
         <v>281777</v>
       </c>
       <c r="D19" s="4">
-        <v>4195092</v>
+        <v>4182952</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>4476869</v>
+        <v>4464729</v>
       </c>
       <c r="G19" s="2">
         <v>60</v>
@@ -19483,30 +19483,30 @@
         <v>2591819</v>
       </c>
       <c r="I19" s="4">
-        <v>1276136</v>
+        <v>1272356</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="5"/>
-        <v>3867955</v>
+        <v>3864175</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" ref="L19" si="17">E19-J19</f>
-        <v>608914</v>
+        <v>600554</v>
       </c>
       <c r="M19" s="5">
         <f t="shared" si="14"/>
-        <v>361215</v>
+        <v>360155</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="2"/>
-        <v>4476869</v>
+        <v>4464729</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>3867955</v>
+        <v>3864175</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19517,11 +19517,11 @@
         <v>281777</v>
       </c>
       <c r="D20" s="4">
-        <v>4828692</v>
+        <v>4814862</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>5110469</v>
+        <v>5096639</v>
       </c>
       <c r="G20" s="2">
         <v>70</v>
@@ -19530,30 +19530,30 @@
         <v>2591819</v>
       </c>
       <c r="I20" s="4">
-        <v>1585021</v>
+        <v>1580611</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="5"/>
-        <v>4176840</v>
+        <v>4172430</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>933629</v>
+        <v>924209</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="4"/>
-        <v>324715</v>
+        <v>323655</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="2"/>
-        <v>5110469</v>
+        <v>5096639</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>4176840</v>
+        <v>4172430</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19564,11 +19564,11 @@
         <v>281777</v>
       </c>
       <c r="D21" s="4">
-        <v>5455692</v>
+        <v>5440172</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>5737469</v>
+        <v>5721949</v>
       </c>
       <c r="G21" s="2">
         <v>80</v>
@@ -19577,30 +19577,30 @@
         <v>2591819</v>
       </c>
       <c r="I21" s="4">
-        <v>1923806</v>
+        <v>1918766</v>
       </c>
       <c r="J21" s="4">
         <f>H21+I21</f>
-        <v>4515625</v>
+        <v>4510585</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>1221844</v>
+        <v>1211364</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="4"/>
-        <v>288215</v>
+        <v>287155</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="2"/>
-        <v>5737469</v>
+        <v>5721949</v>
       </c>
       <c r="R21" s="4">
         <f>H21+I21</f>
-        <v>4515625</v>
+        <v>4510585</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19611,11 +19611,11 @@
         <v>281777</v>
       </c>
       <c r="D22" s="4">
-        <v>6076092</v>
+        <v>6058882</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>6357869</v>
+        <v>6340659</v>
       </c>
       <c r="G22" s="2">
         <v>90</v>
@@ -19624,30 +19624,30 @@
         <v>2591819</v>
       </c>
       <c r="I22" s="4">
-        <v>2292491</v>
+        <v>2286821</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="5"/>
-        <v>4884310</v>
+        <v>4878640</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>1473559</v>
+        <v>1462019</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="4"/>
-        <v>251715</v>
+        <v>250655</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="2"/>
-        <v>6357869</v>
+        <v>6340659</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>4884310</v>
+        <v>4878640</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -19658,11 +19658,11 @@
         <v>281777</v>
       </c>
       <c r="D23" s="4">
-        <v>6672568</v>
+        <v>6653668</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>6954345</v>
+        <v>6935445</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
@@ -19671,30 +19671,30 @@
         <v>2591819</v>
       </c>
       <c r="I23" s="4">
-        <v>2686276</v>
+        <v>2679976</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="5"/>
-        <v>5278095</v>
+        <v>5271795</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>1676250</v>
+        <v>1663650</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="4"/>
-        <v>202691</v>
+        <v>201631</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="2"/>
-        <v>6954345</v>
+        <v>6935445</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>5278095</v>
+        <v>5271795</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1000 runs ascended data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F98BC7-41A1-4830-9977-A77D68461AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EE6E73-17DD-4011-9824-01722272E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -1935,37 +1935,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>367760</c:v>
+                  <c:v>365610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640631</c:v>
+                  <c:v>637527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>979161</c:v>
+                  <c:v>974997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1354891</c:v>
+                  <c:v>1349667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1767821</c:v>
+                  <c:v>1761537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2217951</c:v>
+                  <c:v>2210607</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2705281</c:v>
+                  <c:v>2696877</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3229811</c:v>
+                  <c:v>3220347</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3791541</c:v>
+                  <c:v>3781017</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4390471</c:v>
+                  <c:v>4378887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5006526</c:v>
+                  <c:v>4993882</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5394,37 +5394,37 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>367760</c:v>
+                  <c:v>365610</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>640631</c:v>
+                  <c:v>637527</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>979161</c:v>
+                  <c:v>974997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1354891</c:v>
+                  <c:v>1349667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1767821</c:v>
+                  <c:v>1761537</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2217951</c:v>
+                  <c:v>2210607</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2705281</c:v>
+                  <c:v>2696877</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3229811</c:v>
+                  <c:v>3220347</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3791541</c:v>
+                  <c:v>3781017</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4390471</c:v>
+                  <c:v>4378887</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5006526</c:v>
+                  <c:v>4993882</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18667,7 +18667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06EBE3-BB9C-4874-A95E-FF2651C40304}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -19719,8 +19719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871ADF-8F0F-453C-9415-AC73938A5FD8}">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19768,14 +19768,14 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D3" s="4">
-        <v>85983</v>
+        <v>83877</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>367760</v>
+        <v>365610</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -19792,14 +19792,14 @@
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2285127</v>
+        <v>-2287277</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>367760</v>
+        <v>365610</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
@@ -19811,14 +19811,14 @@
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D4" s="4">
-        <v>358854</v>
+        <v>355794</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E13" si="0">C4+D4</f>
-        <v>640631</v>
+        <v>637527</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -19835,18 +19835,18 @@
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L13" si="1">E4-J4</f>
-        <v>-2130597</v>
+        <v>-2133701</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>154530</v>
+        <v>153576</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q13" si="2">C4+D4</f>
-        <v>640631</v>
+        <v>637527</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R13" si="3">H4+I4</f>
@@ -19858,14 +19858,14 @@
         <v>20</v>
       </c>
       <c r="C5" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D5" s="4">
-        <v>697384</v>
+        <v>693264</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>979161</v>
+        <v>974997</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -19882,18 +19882,18 @@
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1954052</v>
+        <v>-1958216</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>176545</v>
+        <v>175485</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>979161</v>
+        <v>974997</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
@@ -19905,14 +19905,14 @@
         <v>30</v>
       </c>
       <c r="C6" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D6" s="4">
-        <v>1073114</v>
+        <v>1067934</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1354891</v>
+        <v>1349667</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -19929,18 +19929,18 @@
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-1772407</v>
+        <v>-1777631</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>181645</v>
+        <v>180585</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>1354891</v>
+        <v>1349667</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
@@ -19952,14 +19952,14 @@
         <v>40</v>
       </c>
       <c r="C7" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D7" s="4">
-        <v>1486044</v>
+        <v>1479804</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1767821</v>
+        <v>1761537</v>
       </c>
       <c r="G7" s="2">
         <v>40</v>
@@ -19976,18 +19976,18 @@
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>-1585662</v>
+        <v>-1591946</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>186745</v>
+        <v>185685</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>1767821</v>
+        <v>1761537</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
@@ -19999,14 +19999,14 @@
         <v>50</v>
       </c>
       <c r="C8" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D8" s="4">
-        <v>1936174</v>
+        <v>1928874</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>2217951</v>
+        <v>2210607</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
@@ -20023,18 +20023,18 @@
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>-1393817</v>
+        <v>-1401161</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>191845</v>
+        <v>190785</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>2217951</v>
+        <v>2210607</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
@@ -20046,14 +20046,14 @@
         <v>60</v>
       </c>
       <c r="C9" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D9" s="4">
-        <v>2423504</v>
+        <v>2415144</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2705281</v>
+        <v>2696877</v>
       </c>
       <c r="G9" s="2">
         <v>60</v>
@@ -20070,18 +20070,18 @@
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>-1196872</v>
+        <v>-1205276</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>196945</v>
+        <v>195885</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>2705281</v>
+        <v>2696877</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
@@ -20093,14 +20093,14 @@
         <v>70</v>
       </c>
       <c r="C10" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D10" s="4">
-        <v>2948034</v>
+        <v>2938614</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3229811</v>
+        <v>3220347</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
@@ -20117,18 +20117,18 @@
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>-994827</v>
+        <v>-1004291</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>202045</v>
+        <v>200985</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3229811</v>
+        <v>3220347</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
@@ -20140,14 +20140,14 @@
         <v>80</v>
       </c>
       <c r="C11" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D11" s="4">
-        <v>3509764</v>
+        <v>3499284</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3791541</v>
+        <v>3781017</v>
       </c>
       <c r="G11" s="2">
         <v>80</v>
@@ -20164,18 +20164,18 @@
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>-787682</v>
+        <v>-798206</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>207145</v>
+        <v>206085</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3791541</v>
+        <v>3781017</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
@@ -20187,14 +20187,14 @@
         <v>90</v>
       </c>
       <c r="C12" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D12" s="4">
-        <v>4108694</v>
+        <v>4097154</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>4390471</v>
+        <v>4378887</v>
       </c>
       <c r="G12" s="2">
         <v>90</v>
@@ -20211,18 +20211,18 @@
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>-575437</v>
+        <v>-587021</v>
       </c>
       <c r="M12" s="5">
         <f>L12-L11</f>
-        <v>212245</v>
+        <v>211185</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>4390471</v>
+        <v>4378887</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
@@ -20234,14 +20234,14 @@
         <v>100</v>
       </c>
       <c r="C13" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D13" s="4">
-        <v>4724749</v>
+        <v>4712149</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>5006526</v>
+        <v>4993882</v>
       </c>
       <c r="G13" s="2">
         <v>100</v>
@@ -20258,18 +20258,18 @@
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>-373367</v>
+        <v>-386011</v>
       </c>
       <c r="M13" s="5">
         <f>L13-L12</f>
-        <v>202070</v>
+        <v>201010</v>
       </c>
       <c r="P13" s="2">
         <v>100</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>5006526</v>
+        <v>4993882</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Update 1000 runs descended data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EE6E73-17DD-4011-9824-01722272E69B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A90B06-B625-4E55-BABD-390E5A57DE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="4" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -2600,67 +2600,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604286</c:v>
+                  <c:v>602029</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1209869</c:v>
+                  <c:v>1206091</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1876469</c:v>
+                  <c:v>1871001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2536469</c:v>
+                  <c:v>2529311</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3124738</c:v>
+                  <c:v>3116147</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3189869</c:v>
+                  <c:v>3181021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3254846</c:v>
+                  <c:v>3245829</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3319757</c:v>
+                  <c:v>3310571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3384602</c:v>
+                  <c:v>3375247</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3449381</c:v>
+                  <c:v>3439857</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3514094</c:v>
+                  <c:v>3504401</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3578741</c:v>
+                  <c:v>3568879</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3643322</c:v>
+                  <c:v>3633291</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3707837</c:v>
+                  <c:v>3697637</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3772286</c:v>
+                  <c:v>3761917</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3836669</c:v>
+                  <c:v>3826131</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4476869</c:v>
+                  <c:v>4464641</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5110469</c:v>
+                  <c:v>5096551</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5737469</c:v>
+                  <c:v>5721861</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6357869</c:v>
+                  <c:v>6340571</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6954345</c:v>
+                  <c:v>6935357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2797,67 +2797,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2652936</c:v>
+                  <c:v>2652873</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2770710</c:v>
+                  <c:v>2770080</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2929975</c:v>
+                  <c:v>2928715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3119140</c:v>
+                  <c:v>3117250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3314953</c:v>
+                  <c:v>3312496</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3338205</c:v>
+                  <c:v>3335685</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3361756</c:v>
+                  <c:v>3359173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3385606</c:v>
+                  <c:v>3382960</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3409755</c:v>
+                  <c:v>3407046</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3434203</c:v>
+                  <c:v>3431431</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3458950</c:v>
+                  <c:v>3456115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3483996</c:v>
+                  <c:v>3481098</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3509341</c:v>
+                  <c:v>3506380</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3534985</c:v>
+                  <c:v>3531961</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3560928</c:v>
+                  <c:v>3557841</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3587170</c:v>
+                  <c:v>3584020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3866035</c:v>
+                  <c:v>3862255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4174800</c:v>
+                  <c:v>4170390</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4513465</c:v>
+                  <c:v>4508425</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4882030</c:v>
+                  <c:v>4876360</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5275695</c:v>
+                  <c:v>5269395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6043,67 +6043,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>604286</c:v>
+                  <c:v>602029</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1209869</c:v>
+                  <c:v>1206091</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1876469</c:v>
+                  <c:v>1871001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2536469</c:v>
+                  <c:v>2529311</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3124738</c:v>
+                  <c:v>3116147</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3189869</c:v>
+                  <c:v>3181021</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3254846</c:v>
+                  <c:v>3245829</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3319757</c:v>
+                  <c:v>3310571</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3384602</c:v>
+                  <c:v>3375247</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3449381</c:v>
+                  <c:v>3439857</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3514094</c:v>
+                  <c:v>3504401</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3578741</c:v>
+                  <c:v>3568879</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3643322</c:v>
+                  <c:v>3633291</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3707837</c:v>
+                  <c:v>3697637</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3772286</c:v>
+                  <c:v>3761917</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3836669</c:v>
+                  <c:v>3826131</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4476869</c:v>
+                  <c:v>4464641</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5110469</c:v>
+                  <c:v>5096551</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5737469</c:v>
+                  <c:v>5721861</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6357869</c:v>
+                  <c:v>6340571</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>6954345</c:v>
+                  <c:v>6935357</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6226,67 +6226,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2652936</c:v>
+                  <c:v>2652873</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2770710</c:v>
+                  <c:v>2770080</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2929975</c:v>
+                  <c:v>2928715</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3119140</c:v>
+                  <c:v>3117250</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3314953</c:v>
+                  <c:v>3312496</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3338205</c:v>
+                  <c:v>3335685</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3361756</c:v>
+                  <c:v>3359173</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3385606</c:v>
+                  <c:v>3382960</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3409755</c:v>
+                  <c:v>3407046</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3434203</c:v>
+                  <c:v>3431431</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3458950</c:v>
+                  <c:v>3456115</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3483996</c:v>
+                  <c:v>3481098</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3509341</c:v>
+                  <c:v>3506380</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3534985</c:v>
+                  <c:v>3531961</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3560928</c:v>
+                  <c:v>3557841</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3587170</c:v>
+                  <c:v>3584020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3866035</c:v>
+                  <c:v>3862255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4174800</c:v>
+                  <c:v>4170390</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4513465</c:v>
+                  <c:v>4508425</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4882030</c:v>
+                  <c:v>4876360</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5275695</c:v>
+                  <c:v>5269395</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19719,7 +19719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871ADF-8F0F-453C-9415-AC73938A5FD8}">
   <dimension ref="B2:R15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -20310,7 +20310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
@@ -20359,14 +20359,14 @@
         <v>1</v>
       </c>
       <c r="C3" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D3" s="4">
-        <v>322509</v>
+        <v>320296</v>
       </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>604286</v>
+        <v>602029</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -20375,26 +20375,26 @@
         <v>2590619</v>
       </c>
       <c r="I3" s="4">
-        <v>62317</v>
+        <v>62254</v>
       </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>2652936</v>
+        <v>2652873</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>-2048650</v>
+        <v>-2050844</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>604286</v>
+        <v>602029</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>2652936</v>
+        <v>2652873</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20402,14 +20402,14 @@
         <v>10</v>
       </c>
       <c r="C4" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D4" s="4">
-        <v>928092</v>
+        <v>924358</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E23" si="0">C4+D4</f>
-        <v>1209869</v>
+        <v>1206091</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
@@ -20418,30 +20418,30 @@
         <v>2590619</v>
       </c>
       <c r="I4" s="4">
-        <v>180091</v>
+        <v>179461</v>
       </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>2770710</v>
+        <v>2770080</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>-1560841</v>
+        <v>-1563989</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>487809</v>
+        <v>486855</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
-        <v>1209869</v>
+        <v>1206091</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>2770710</v>
+        <v>2770080</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20449,14 +20449,14 @@
         <v>20</v>
       </c>
       <c r="C5" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D5" s="4">
-        <v>1594692</v>
+        <v>1589268</v>
       </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>1876469</v>
+        <v>1871001</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
@@ -20465,30 +20465,30 @@
         <v>2590619</v>
       </c>
       <c r="I5" s="4">
-        <v>339356</v>
+        <v>338096</v>
       </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J23" si="4">H5+I5</f>
-        <v>2929975</v>
+        <v>2928715</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>-1053506</v>
+        <v>-1057714</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="5">L5-L4</f>
-        <v>507335</v>
+        <v>506275</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>1876469</v>
+        <v>1871001</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>2929975</v>
+        <v>2928715</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20496,14 +20496,14 @@
         <v>30</v>
       </c>
       <c r="C6" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D6" s="4">
-        <v>2254692</v>
+        <v>2247578</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>2536469</v>
+        <v>2529311</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
@@ -20512,30 +20512,30 @@
         <v>2590619</v>
       </c>
       <c r="I6" s="4">
-        <v>528521</v>
+        <v>526631</v>
       </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>3119140</v>
+        <v>3117250</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>-582671</v>
+        <v>-587939</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>470835</v>
+        <v>469775</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>2536469</v>
+        <v>2529311</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>3119140</v>
+        <v>3117250</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20546,11 +20546,11 @@
         <v>281733</v>
       </c>
       <c r="D7" s="4">
-        <v>2843005</v>
+        <v>2834414</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>3124738</v>
+        <v>3116147</v>
       </c>
       <c r="G7" s="2">
         <v>39</v>
@@ -20559,30 +20559,30 @@
         <v>2590619</v>
       </c>
       <c r="I7" s="4">
-        <v>724334</v>
+        <v>721877</v>
       </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>3314953</v>
+        <v>3312496</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" ref="L7:L8" si="6">E7-J7</f>
-        <v>-190215</v>
+        <v>-196349</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" ref="M7:M8" si="7">L7-L6</f>
-        <v>392456</v>
+        <v>391590</v>
       </c>
       <c r="P7" s="2">
         <v>31</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" ref="Q7" si="8">C7+D7</f>
-        <v>3124738</v>
+        <v>3116147</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" ref="R7" si="9">H7+I7</f>
-        <v>3314953</v>
+        <v>3312496</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20590,14 +20590,14 @@
         <v>40</v>
       </c>
       <c r="C8" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D8" s="4">
-        <v>2908092</v>
+        <v>2899288</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>3189869</v>
+        <v>3181021</v>
       </c>
       <c r="G8" s="2">
         <v>40</v>
@@ -20606,30 +20606,30 @@
         <v>2590619</v>
       </c>
       <c r="I8" s="4">
-        <v>747586</v>
+        <v>745066</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>3338205</v>
+        <v>3335685</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="6"/>
-        <v>-148336</v>
+        <v>-154664</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="7"/>
-        <v>41879</v>
+        <v>41685</v>
       </c>
       <c r="P8" s="2">
         <v>40</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>3189869</v>
+        <v>3181021</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>3338205</v>
+        <v>3335685</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20637,14 +20637,14 @@
         <v>41</v>
       </c>
       <c r="C9" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D9" s="4">
-        <v>2973069</v>
+        <v>2964096</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>3254846</v>
+        <v>3245829</v>
       </c>
       <c r="G9" s="2">
         <v>41</v>
@@ -20653,30 +20653,30 @@
         <v>2590619</v>
       </c>
       <c r="I9" s="4">
-        <v>771137</v>
+        <v>768554</v>
       </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>3361756</v>
+        <v>3359173</v>
       </c>
       <c r="L9" s="4">
         <f>E9-J9</f>
-        <v>-106910</v>
+        <v>-113344</v>
       </c>
       <c r="M9" s="5">
         <f>L9-L8</f>
-        <v>41426</v>
+        <v>41320</v>
       </c>
       <c r="P9" s="2">
         <v>41</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" ref="Q9" si="10">C9+D9</f>
-        <v>3254846</v>
+        <v>3245829</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" ref="R9" si="11">H9+I9</f>
-        <v>3361756</v>
+        <v>3359173</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20684,14 +20684,14 @@
         <v>42</v>
       </c>
       <c r="C10" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D10" s="4">
-        <v>3037980</v>
+        <v>3028838</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3319757</v>
+        <v>3310571</v>
       </c>
       <c r="G10" s="2">
         <v>42</v>
@@ -20700,30 +20700,30 @@
         <v>2590619</v>
       </c>
       <c r="I10" s="4">
-        <v>794987</v>
+        <v>792341</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>3385606</v>
+        <v>3382960</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" ref="L10" si="12">E10-J10</f>
-        <v>-65849</v>
+        <v>-72389</v>
       </c>
       <c r="M10" s="5">
         <f>L10-L9</f>
-        <v>41061</v>
+        <v>40955</v>
       </c>
       <c r="P10" s="2">
         <v>42</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>3319757</v>
+        <v>3310571</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>3385606</v>
+        <v>3382960</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20731,14 +20731,14 @@
         <v>43</v>
       </c>
       <c r="C11" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D11" s="4">
-        <v>3102825</v>
+        <v>3093514</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>3384602</v>
+        <v>3375247</v>
       </c>
       <c r="G11" s="2">
         <v>43</v>
@@ -20747,30 +20747,30 @@
         <v>2590619</v>
       </c>
       <c r="I11" s="4">
-        <v>819136</v>
+        <v>816427</v>
       </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>3409755</v>
+        <v>3407046</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" ref="L11" si="13">E11-J11</f>
-        <v>-25153</v>
+        <v>-31799</v>
       </c>
       <c r="M11" s="5">
         <f t="shared" ref="M11:M15" si="14">L11-L10</f>
-        <v>40696</v>
+        <v>40590</v>
       </c>
       <c r="P11" s="2">
         <v>43</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>3384602</v>
+        <v>3375247</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>3409755</v>
+        <v>3407046</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20779,14 +20779,14 @@
         <v>44</v>
       </c>
       <c r="C12" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D12" s="4">
-        <v>3167604</v>
+        <v>3158124</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>3449381</v>
+        <v>3439857</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2">
@@ -20796,31 +20796,31 @@
         <v>2590619</v>
       </c>
       <c r="I12" s="4">
-        <v>843584</v>
+        <v>840812</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>3434203</v>
+        <v>3431431</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="4">
         <f t="shared" ref="L12" si="15">E12-J12</f>
-        <v>15178</v>
+        <v>8426</v>
       </c>
       <c r="M12" s="5">
         <f t="shared" si="14"/>
-        <v>40331</v>
+        <v>40225</v>
       </c>
       <c r="P12" s="2">
         <v>44</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>3449381</v>
+        <v>3439857</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>3434203</v>
+        <v>3431431</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20828,14 +20828,14 @@
         <v>45</v>
       </c>
       <c r="C13" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D13" s="4">
-        <v>3232317</v>
+        <v>3222668</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>3514094</v>
+        <v>3504401</v>
       </c>
       <c r="G13" s="2">
         <v>45</v>
@@ -20844,30 +20844,30 @@
         <v>2590619</v>
       </c>
       <c r="I13" s="4">
-        <v>868331</v>
+        <v>865496</v>
       </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>3458950</v>
+        <v>3456115</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" ref="L13" si="16">E13-J13</f>
-        <v>55144</v>
+        <v>48286</v>
       </c>
       <c r="M13" s="5">
         <f t="shared" si="14"/>
-        <v>39966</v>
+        <v>39860</v>
       </c>
       <c r="P13" s="2">
         <v>45</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>3514094</v>
+        <v>3504401</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>3458950</v>
+        <v>3456115</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20875,14 +20875,14 @@
         <v>46</v>
       </c>
       <c r="C14" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D14" s="4">
-        <v>3296964</v>
+        <v>3287146</v>
       </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>3578741</v>
+        <v>3568879</v>
       </c>
       <c r="G14" s="2">
         <v>46</v>
@@ -20891,30 +20891,30 @@
         <v>2590619</v>
       </c>
       <c r="I14" s="4">
-        <v>893377</v>
+        <v>890479</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="4"/>
-        <v>3483996</v>
+        <v>3481098</v>
       </c>
       <c r="L14" s="4">
         <f t="shared" ref="L14:L16" si="17">E14-J14</f>
-        <v>94745</v>
+        <v>87781</v>
       </c>
       <c r="M14" s="5">
         <f t="shared" si="14"/>
-        <v>39601</v>
+        <v>39495</v>
       </c>
       <c r="P14" s="2">
         <v>46</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>3578741</v>
+        <v>3568879</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>3483996</v>
+        <v>3481098</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20922,14 +20922,14 @@
         <v>47</v>
       </c>
       <c r="C15" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D15" s="4">
-        <v>3361545</v>
+        <v>3351558</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>3643322</v>
+        <v>3633291</v>
       </c>
       <c r="G15" s="2">
         <v>47</v>
@@ -20938,30 +20938,30 @@
         <v>2590619</v>
       </c>
       <c r="I15" s="4">
-        <v>918722</v>
+        <v>915761</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="4"/>
-        <v>3509341</v>
+        <v>3506380</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" si="17"/>
-        <v>133981</v>
+        <v>126911</v>
       </c>
       <c r="M15" s="5">
         <f t="shared" si="14"/>
-        <v>39236</v>
+        <v>39130</v>
       </c>
       <c r="P15" s="2">
         <v>47</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>3643322</v>
+        <v>3633291</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>3509341</v>
+        <v>3506380</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -20969,14 +20969,14 @@
         <v>48</v>
       </c>
       <c r="C16" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D16" s="4">
-        <v>3426060</v>
+        <v>3415904</v>
       </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>3707837</v>
+        <v>3697637</v>
       </c>
       <c r="G16" s="2">
         <v>48</v>
@@ -20985,30 +20985,30 @@
         <v>2590619</v>
       </c>
       <c r="I16" s="4">
-        <v>944366</v>
+        <v>941342</v>
       </c>
       <c r="J16" s="4">
         <f t="shared" si="4"/>
-        <v>3534985</v>
+        <v>3531961</v>
       </c>
       <c r="L16" s="4">
         <f t="shared" si="17"/>
-        <v>172852</v>
+        <v>165676</v>
       </c>
       <c r="M16" s="5">
         <f t="shared" ref="M16" si="18">L16-L12</f>
-        <v>157674</v>
+        <v>157250</v>
       </c>
       <c r="P16" s="2">
         <v>48</v>
       </c>
       <c r="Q16" s="4">
         <f t="shared" si="2"/>
-        <v>3707837</v>
+        <v>3697637</v>
       </c>
       <c r="R16" s="4">
         <f t="shared" si="3"/>
-        <v>3534985</v>
+        <v>3531961</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21016,14 +21016,14 @@
         <v>49</v>
       </c>
       <c r="C17" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D17" s="4">
-        <v>3490509</v>
+        <v>3480184</v>
       </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>3772286</v>
+        <v>3761917</v>
       </c>
       <c r="G17" s="2">
         <v>49</v>
@@ -21032,30 +21032,30 @@
         <v>2590619</v>
       </c>
       <c r="I17" s="4">
-        <v>970309</v>
+        <v>967222</v>
       </c>
       <c r="J17" s="4">
         <f t="shared" si="4"/>
-        <v>3560928</v>
+        <v>3557841</v>
       </c>
       <c r="L17" s="4">
         <f t="shared" ref="L17:L18" si="19">E17-J17</f>
-        <v>211358</v>
+        <v>204076</v>
       </c>
       <c r="M17" s="5">
         <f t="shared" ref="M17:M18" si="20">L17-L13</f>
-        <v>156214</v>
+        <v>155790</v>
       </c>
       <c r="P17" s="2">
         <v>49</v>
       </c>
       <c r="Q17" s="4">
         <f t="shared" ref="Q17:Q18" si="21">C17+D17</f>
-        <v>3772286</v>
+        <v>3761917</v>
       </c>
       <c r="R17" s="4">
         <f t="shared" ref="R17:R18" si="22">H17+I17</f>
-        <v>3560928</v>
+        <v>3557841</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21063,14 +21063,14 @@
         <v>50</v>
       </c>
       <c r="C18" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D18" s="4">
-        <v>3554892</v>
+        <v>3544398</v>
       </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>3836669</v>
+        <v>3826131</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
@@ -21079,30 +21079,30 @@
         <v>2590619</v>
       </c>
       <c r="I18" s="4">
-        <v>996551</v>
+        <v>993401</v>
       </c>
       <c r="J18" s="4">
         <f t="shared" si="4"/>
-        <v>3587170</v>
+        <v>3584020</v>
       </c>
       <c r="L18" s="4">
         <f t="shared" si="19"/>
-        <v>249499</v>
+        <v>242111</v>
       </c>
       <c r="M18" s="5">
         <f t="shared" si="20"/>
-        <v>154754</v>
+        <v>154330</v>
       </c>
       <c r="P18" s="2">
         <v>50</v>
       </c>
       <c r="Q18" s="4">
         <f t="shared" si="21"/>
-        <v>3836669</v>
+        <v>3826131</v>
       </c>
       <c r="R18" s="4">
         <f t="shared" si="22"/>
-        <v>3587170</v>
+        <v>3584020</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21110,14 +21110,14 @@
         <v>60</v>
       </c>
       <c r="C19" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D19" s="4">
-        <v>4195092</v>
+        <v>4182908</v>
       </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>4476869</v>
+        <v>4464641</v>
       </c>
       <c r="G19" s="2">
         <v>60</v>
@@ -21126,30 +21126,30 @@
         <v>2590619</v>
       </c>
       <c r="I19" s="4">
-        <v>1275416</v>
+        <v>1271636</v>
       </c>
       <c r="J19" s="4">
         <f t="shared" si="4"/>
-        <v>3866035</v>
+        <v>3862255</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" ref="L19" si="23">E19-J19</f>
-        <v>610834</v>
+        <v>602386</v>
       </c>
       <c r="M19" s="5">
         <f>L19-L16</f>
-        <v>437982</v>
+        <v>436710</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="2"/>
-        <v>4476869</v>
+        <v>4464641</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>3866035</v>
+        <v>3862255</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21157,14 +21157,14 @@
         <v>70</v>
       </c>
       <c r="C20" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D20" s="4">
-        <v>4828692</v>
+        <v>4814818</v>
       </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>5110469</v>
+        <v>5096551</v>
       </c>
       <c r="G20" s="2">
         <v>70</v>
@@ -21173,30 +21173,30 @@
         <v>2590619</v>
       </c>
       <c r="I20" s="4">
-        <v>1584181</v>
+        <v>1579771</v>
       </c>
       <c r="J20" s="4">
         <f t="shared" si="4"/>
-        <v>4174800</v>
+        <v>4170390</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>935669</v>
+        <v>926161</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="5"/>
-        <v>324835</v>
+        <v>323775</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="2"/>
-        <v>5110469</v>
+        <v>5096551</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>4174800</v>
+        <v>4170390</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21204,14 +21204,14 @@
         <v>80</v>
       </c>
       <c r="C21" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D21" s="4">
-        <v>5455692</v>
+        <v>5440128</v>
       </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>5737469</v>
+        <v>5721861</v>
       </c>
       <c r="G21" s="2">
         <v>80</v>
@@ -21220,30 +21220,30 @@
         <v>2590619</v>
       </c>
       <c r="I21" s="4">
-        <v>1922846</v>
+        <v>1917806</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="4"/>
-        <v>4513465</v>
+        <v>4508425</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>1224004</v>
+        <v>1213436</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>288335</v>
+        <v>287275</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="2"/>
-        <v>5737469</v>
+        <v>5721861</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="3"/>
-        <v>4513465</v>
+        <v>4508425</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21251,14 +21251,14 @@
         <v>90</v>
       </c>
       <c r="C22" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D22" s="4">
-        <v>6076092</v>
+        <v>6058838</v>
       </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>6357869</v>
+        <v>6340571</v>
       </c>
       <c r="G22" s="2">
         <v>90</v>
@@ -21267,30 +21267,30 @@
         <v>2590619</v>
       </c>
       <c r="I22" s="4">
-        <v>2291411</v>
+        <v>2285741</v>
       </c>
       <c r="J22" s="4">
         <f t="shared" si="4"/>
-        <v>4882030</v>
+        <v>4876360</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>1475839</v>
+        <v>1464211</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="5"/>
-        <v>251835</v>
+        <v>250775</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="2"/>
-        <v>6357869</v>
+        <v>6340571</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>4882030</v>
+        <v>4876360</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -21298,14 +21298,14 @@
         <v>100</v>
       </c>
       <c r="C23" s="4">
-        <v>281777</v>
+        <v>281733</v>
       </c>
       <c r="D23" s="4">
-        <v>6672568</v>
+        <v>6653624</v>
       </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>6954345</v>
+        <v>6935357</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
@@ -21314,30 +21314,30 @@
         <v>2590619</v>
       </c>
       <c r="I23" s="4">
-        <v>2685076</v>
+        <v>2678776</v>
       </c>
       <c r="J23" s="4">
         <f t="shared" si="4"/>
-        <v>5275695</v>
+        <v>5269395</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>1678650</v>
+        <v>1665962</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="5"/>
-        <v>202811</v>
+        <v>201751</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="2"/>
-        <v>6954345</v>
+        <v>6935357</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>5275695</v>
+        <v>5269395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 200 runs data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1208A0F6-565B-4639-99A5-7DD4C2B7DC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB5DA96-755F-468B-87BD-0DC836D1D977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -1155,37 +1155,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -1215,67 +1215,58 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>548817</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1140513</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1794343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2444373</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3026151</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3090603</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3155017</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3219393</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3283731</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3348031</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3412293</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3476517</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3733033</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>4371663</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5006493</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>5637523</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>6264753</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>6868037</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,37 +1343,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -1412,67 +1403,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2599481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2673596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2784351</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2925006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3023751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3041255</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3059058</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3077160</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3095561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3114261</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3133260</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3152558</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3172155</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3192051</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3212246</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3296016</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>3526371</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>3786626</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>4076781</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>4396836</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>4726891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3999,10 +3990,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4034,6 +4025,33 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -4041,42 +4059,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$22</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>311116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>584005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>923695</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1301785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1718275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2173165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2666455</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3198145</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3768235</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4376725</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4439686</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4503031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4566760</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4630873</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4695370</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4760251</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4825516</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4891165</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4957198</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5003540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4122,10 +4167,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -4157,6 +4202,33 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -4164,42 +4236,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$22</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2599495</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2674744</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2788849</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2935054</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3113359</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3323764</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3566269</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3840874</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4147579</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4486384</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4522030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4557997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4594285</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4630894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4667824</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4705075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4742647</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4780540</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4818754</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4837389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4630,37 +4729,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -4690,67 +4789,58 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>548817</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1140513</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1794343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2444373</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3026151</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3090603</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3155017</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3219393</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3283731</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3348031</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3412293</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3476517</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3733033</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>4371663</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5006493</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>5637523</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>6264753</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>6868037</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4813,37 +4903,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>39</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -4873,67 +4963,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2599481</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2673596</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2784351</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2925006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3023751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3041255</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3059058</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3077160</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3095561</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3114261</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3133260</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3152558</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3172155</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3192051</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3212246</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3296016</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>3526371</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>3786626</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>4076781</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>4396836</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>4726891</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8072,10 +8162,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -8107,6 +8197,33 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -8114,42 +8231,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$Q$3:$Q$22</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>311116</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>584005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>923695</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1301785</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1718275</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2173165</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2666455</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3198145</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3768235</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4376725</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4439686</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4503031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4566760</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4630873</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4695370</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4760251</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4825516</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4891165</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4957198</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5003540</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8209,10 +8353,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$P$3:$P$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -8244,6 +8388,33 @@
                   <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -8251,42 +8422,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$13</c:f>
+              <c:f>'Optimizer | 200 run - Ascended'!$R$3:$R$22</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2599495</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2674744</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2788849</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2935054</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3113359</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3323764</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3566269</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3840874</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4147579</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4486384</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4522030</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4557997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4594285</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4630894</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4667824</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4705075</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4742647</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4780540</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4818754</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4837389</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15796,7 +15994,7 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>19500</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>431100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -17024,7 +17222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1DA2FE-2DBA-48DD-9085-CD8066E7E300}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -18074,10 +18272,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F68343B-F0B9-4DF5-8EBB-C222891744B9}">
-  <dimension ref="B2:R15"/>
+  <dimension ref="A2:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I13"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18124,441 +18322,955 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D3" s="4">
+        <v>50753</v>
+      </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>311116</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I3" s="4">
+        <v>29108</v>
+      </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2599495</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>0</v>
+        <v>-2288379</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>311116</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2599495</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D4" s="4">
+        <v>323642</v>
+      </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E13" si="0">C4+D4</f>
-        <v>0</v>
+        <f t="shared" ref="E4:E22" si="0">C4+D4</f>
+        <v>584005</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I4" s="4">
+        <v>104357</v>
+      </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>0</v>
+        <v>2674744</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L13" si="1">E4-J4</f>
-        <v>0</v>
+        <f t="shared" ref="L4:L12" si="1">E4-J4</f>
+        <v>-2090739</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>0</v>
+        <v>197640</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q13" si="2">C4+D4</f>
-        <v>0</v>
+        <f t="shared" ref="Q4:Q22" si="2">C4+D4</f>
+        <v>584005</v>
       </c>
       <c r="R4" s="4">
-        <f t="shared" ref="R4:R13" si="3">H4+I4</f>
-        <v>0</v>
+        <f t="shared" ref="R4:R22" si="3">H4+I4</f>
+        <v>2674744</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>20</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D5" s="4">
+        <v>663332</v>
+      </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>923695</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I5" s="4">
+        <v>218462</v>
+      </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J12" si="4">H5+I5</f>
-        <v>0</v>
+        <f t="shared" ref="J5:J21" si="4">H5+I5</f>
+        <v>2788849</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1865154</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>0</v>
+        <v>225585</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>923695</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2788849</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>30</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1041422</v>
+      </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1301785</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I6" s="4">
+        <v>364667</v>
+      </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2935054</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1633269</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>231885</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1301785</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2935054</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>40</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1457912</v>
+      </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1718275</v>
       </c>
       <c r="G7" s="2">
         <v>40</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="H7" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I7" s="4">
+        <v>542972</v>
+      </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3113359</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1395084</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>238185</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1718275</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3113359</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>50</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1912802</v>
+      </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2173165</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="H8" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I8" s="4">
+        <v>753377</v>
+      </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3323764</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1150599</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>244485</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2173165</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3323764</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>60</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2406092</v>
+      </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2666455</v>
       </c>
       <c r="G9" s="2">
         <v>60</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="H9" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I9" s="4">
+        <v>995882</v>
+      </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3566269</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-899814</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>250785</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2666455</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3566269</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>70</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2937782</v>
+      </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3198145</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="H10" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1270487</v>
+      </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3840874</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-642729</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>257085</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3198145</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3840874</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>80</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3507872</v>
+      </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3768235</v>
       </c>
       <c r="G11" s="2">
         <v>80</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="H11" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1577192</v>
+      </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4147579</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-379344</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>0</v>
+        <v>263385</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3768235</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4147579</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>90</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4116362</v>
+      </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4376725</v>
       </c>
       <c r="G12" s="2">
         <v>90</v>
       </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="H12" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1915997</v>
+      </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4486384</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-109659</v>
       </c>
       <c r="M12" s="5">
         <f>L12-L11</f>
-        <v>0</v>
+        <v>269685</v>
       </c>
       <c r="P12" s="2">
         <v>90</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4376725</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4486384</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>100</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="C13" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4179323</v>
+      </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4439686</v>
       </c>
       <c r="G13" s="2">
-        <v>100</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>91</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1951643</v>
+      </c>
       <c r="J13" s="4">
-        <f t="shared" ref="J13" si="6">H13+I13</f>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>4522030</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="L13:L15" si="6">E13-J13</f>
+        <v>-82344</v>
       </c>
       <c r="M13" s="5">
-        <f>L13-L12</f>
-        <v>0</v>
+        <f t="shared" ref="M13:M14" si="7">L13-L12</f>
+        <v>27315</v>
       </c>
       <c r="P13" s="2">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="Q13:Q22" si="8">C13+D13</f>
+        <v>4439686</v>
       </c>
       <c r="R13" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="R13:R22" si="9">H13+I13</f>
+        <v>4522030</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
+      <c r="B14" s="2">
+        <v>92</v>
+      </c>
+      <c r="C14" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4242668</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>4503031</v>
+      </c>
+      <c r="G14" s="2">
+        <v>92</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1987610</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="4"/>
+        <v>4557997</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="6"/>
+        <v>-54966</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="7"/>
+        <v>27378</v>
+      </c>
+      <c r="P14" s="2">
+        <v>92</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="8"/>
+        <v>4503031</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="9"/>
+        <v>4557997</v>
+      </c>
     </row>
     <row r="15" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
+      <c r="B15" s="2">
+        <v>93</v>
+      </c>
+      <c r="C15" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D15" s="4">
+        <v>4306397</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>4566760</v>
+      </c>
+      <c r="G15" s="2">
+        <v>93</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I15" s="4">
+        <v>2023898</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="4"/>
+        <v>4594285</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="6"/>
+        <v>-27525</v>
+      </c>
+      <c r="M15" s="5">
+        <f>L15-L14</f>
+        <v>27441</v>
+      </c>
+      <c r="P15" s="2">
+        <v>93</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="8"/>
+        <v>4566760</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" si="9"/>
+        <v>4594285</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>94</v>
+      </c>
+      <c r="C16" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D16" s="4">
+        <v>4370510</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>4630873</v>
+      </c>
+      <c r="G16" s="2">
+        <v>94</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2060507</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="4"/>
+        <v>4630894</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" ref="L15:L17" si="10">E16-J16</f>
+        <v>-21</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" ref="M16:M17" si="11">L16-L15</f>
+        <v>27504</v>
+      </c>
+      <c r="P16" s="2">
+        <v>94</v>
+      </c>
+      <c r="Q16" s="4">
+        <f t="shared" si="8"/>
+        <v>4630873</v>
+      </c>
+      <c r="R16" s="4">
+        <f t="shared" si="9"/>
+        <v>4630894</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="2">
+        <v>95</v>
+      </c>
+      <c r="C17" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4435007</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>4695370</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="2">
+        <v>95</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2097437</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="4"/>
+        <v>4667824</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4">
+        <f t="shared" si="10"/>
+        <v>27546</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="11"/>
+        <v>27567</v>
+      </c>
+      <c r="P17" s="2">
+        <v>95</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="8"/>
+        <v>4695370</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="9"/>
+        <v>4667824</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>96</v>
+      </c>
+      <c r="C18" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4499888</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>4760251</v>
+      </c>
+      <c r="G18" s="2">
+        <v>96</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I18" s="4">
+        <v>2134688</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="4"/>
+        <v>4705075</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" ref="L18:L19" si="12">E18-J18</f>
+        <v>55176</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" ref="M18:M19" si="13">L18-L17</f>
+        <v>27630</v>
+      </c>
+      <c r="P18" s="2">
+        <v>96</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" si="8"/>
+        <v>4760251</v>
+      </c>
+      <c r="R18" s="4">
+        <f t="shared" si="9"/>
+        <v>4705075</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>97</v>
+      </c>
+      <c r="C19" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4565153</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>4825516</v>
+      </c>
+      <c r="G19" s="2">
+        <v>97</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2172260</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="4"/>
+        <v>4742647</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="12"/>
+        <v>82869</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="13"/>
+        <v>27693</v>
+      </c>
+      <c r="P19" s="2">
+        <v>97</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="8"/>
+        <v>4825516</v>
+      </c>
+      <c r="R19" s="4">
+        <f t="shared" si="9"/>
+        <v>4742647</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>98</v>
+      </c>
+      <c r="C20" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4630802</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>4891165</v>
+      </c>
+      <c r="G20" s="2">
+        <v>98</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2210153</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="4"/>
+        <v>4780540</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" ref="L20:L22" si="14">E20-J20</f>
+        <v>110625</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" ref="M20:M22" si="15">L20-L19</f>
+        <v>27756</v>
+      </c>
+      <c r="P20" s="2">
+        <v>98</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" si="8"/>
+        <v>4891165</v>
+      </c>
+      <c r="R20" s="4">
+        <f t="shared" si="9"/>
+        <v>4780540</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>99</v>
+      </c>
+      <c r="C21" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D21" s="4">
+        <v>4696835</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>4957198</v>
+      </c>
+      <c r="G21" s="2">
+        <v>99</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I21" s="4">
+        <v>2248367</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="4"/>
+        <v>4818754</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="14"/>
+        <v>138444</v>
+      </c>
+      <c r="M21" s="5">
+        <f t="shared" si="15"/>
+        <v>27819</v>
+      </c>
+      <c r="P21" s="2">
+        <v>99</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="8"/>
+        <v>4957198</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="9"/>
+        <v>4818754</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>100</v>
+      </c>
+      <c r="C22" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4743177</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>5003540</v>
+      </c>
+      <c r="G22" s="2">
+        <v>100</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2267002</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" ref="J22" si="16">H22+I22</f>
+        <v>4837389</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="14"/>
+        <v>166151</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="15"/>
+        <v>27707</v>
+      </c>
+      <c r="P22" s="2">
+        <v>100</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="8"/>
+        <v>5003540</v>
+      </c>
+      <c r="R22" s="4">
+        <f t="shared" si="9"/>
+        <v>4837389</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+    </row>
+    <row r="24" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L3:L13">
+  <conditionalFormatting sqref="L3:L22">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -18579,8 +19291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06EBE3-BB9C-4874-A95E-FF2651C40304}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18627,818 +19339,977 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D3" s="4">
+        <v>288454</v>
+      </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>548817</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I3" s="4">
+        <v>29094</v>
+      </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2599481</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>0</v>
+        <v>-2050664</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>548817</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2599481</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D4" s="4">
+        <v>880150</v>
+      </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E23" si="0">C4+D4</f>
-        <v>0</v>
+        <v>1140513</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I4" s="4">
+        <v>103209</v>
+      </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>0</v>
+        <v>2673596</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>0</v>
+        <v>-1533083</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>0</v>
+        <v>517581</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
-        <v>0</v>
+        <v>1140513</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>0</v>
+        <v>2673596</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>20</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1533980</v>
+      </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1794343</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I5" s="4">
+        <v>213964</v>
+      </c>
       <c r="J5" s="4">
         <f>H5+I5</f>
-        <v>0</v>
+        <v>2784351</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-990008</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="4">L5-L4</f>
-        <v>0</v>
+        <v>543075</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1794343</v>
       </c>
       <c r="R5" s="4">
         <f>H5+I5</f>
-        <v>0</v>
+        <v>2784351</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>30</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2184010</v>
+      </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2444373</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I6" s="4">
+        <v>354619</v>
+      </c>
       <c r="J6" s="4">
         <f t="shared" ref="J6:J23" si="5">H6+I6</f>
-        <v>0</v>
+        <v>2925006</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-480633</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>0</v>
+        <v>509375</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2444373</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2925006</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>39</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="C7" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2572204</v>
+      </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2832567</v>
       </c>
       <c r="G7" s="2">
-        <v>39</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I7" s="4">
+        <v>453364</v>
+      </c>
       <c r="J7" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3023751</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7:L8" si="6">E7-J7</f>
-        <v>0</v>
+        <f t="shared" ref="L7:L9" si="6">E7-J7</f>
+        <v>-191184</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" ref="M7:M8" si="7">L7-L6</f>
-        <v>0</v>
+        <f t="shared" ref="M7:M18" si="7">L7-L6</f>
+        <v>289449</v>
       </c>
       <c r="P7" s="2">
-        <v>39</v>
-      </c>
-      <c r="Q7" s="4">
-        <f t="shared" ref="Q7" si="8">C7+D7</f>
-        <v>0</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="Q7" s="4"/>
       <c r="R7" s="4">
-        <f t="shared" ref="R7" si="9">H7+I7</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3023751</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>40</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="C8" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2636770</v>
+      </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2897133</v>
       </c>
       <c r="G8" s="2">
-        <v>40</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I8" s="4">
+        <v>470868</v>
+      </c>
       <c r="J8" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3041255</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-144122</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>47062</v>
       </c>
       <c r="P8" s="2">
-        <v>40</v>
-      </c>
-      <c r="Q8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="Q8" s="4"/>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3041255</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>41</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="C9" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2701298</v>
+      </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2961661</v>
       </c>
       <c r="G9" s="2">
-        <v>41</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I9" s="4">
+        <v>488671</v>
+      </c>
       <c r="J9" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3059058</v>
       </c>
       <c r="L9" s="4">
-        <f t="shared" ref="L9" si="10">E9-J9</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>-97397</v>
       </c>
       <c r="M9" s="5">
-        <f>L9-L8</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46725</v>
       </c>
       <c r="P9" s="2">
-        <v>41</v>
-      </c>
-      <c r="Q9" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="Q9" s="4"/>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3059058</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>42</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C10" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2765788</v>
+      </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3026151</v>
       </c>
       <c r="G10" s="2">
-        <v>42</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I10" s="4">
+        <v>506773</v>
+      </c>
       <c r="J10" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3077160</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" ref="L10:L16" si="11">E10-J10</f>
-        <v>0</v>
+        <f t="shared" ref="L10:L18" si="8">E10-J10</f>
+        <v>-51009</v>
       </c>
       <c r="M10" s="5">
-        <f t="shared" ref="M10:M16" si="12">L10-L9</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46388</v>
       </c>
       <c r="P10" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="Q10" si="9">C10+D10</f>
+        <v>3026151</v>
       </c>
       <c r="R10" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="R10" si="10">H10+I10</f>
+        <v>3077160</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>43</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C11" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2830240</v>
+      </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3090603</v>
       </c>
       <c r="G11" s="2">
-        <v>43</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I11" s="4">
+        <v>525174</v>
+      </c>
       <c r="J11" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3095561</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>-4958</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46051</v>
       </c>
       <c r="P11" s="2">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3090603</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3095561</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="2">
-        <v>44</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="C12" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2894654</v>
+      </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3155017</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2">
-        <v>44</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I12" s="4">
+        <v>543874</v>
+      </c>
       <c r="J12" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3114261</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>40756</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>45714</v>
       </c>
       <c r="P12" s="2">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3155017</v>
       </c>
       <c r="R12" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3114261</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>45</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="C13" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2959030</v>
+      </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3219393</v>
       </c>
       <c r="G13" s="2">
-        <v>45</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I13" s="4">
+        <v>562873</v>
+      </c>
       <c r="J13" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3133260</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>86133</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>45377</v>
       </c>
       <c r="P13" s="2">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3219393</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3133260</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>46</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C14" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3023368</v>
+      </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3283731</v>
       </c>
       <c r="G14" s="2">
-        <v>46</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I14" s="4">
+        <v>582171</v>
+      </c>
       <c r="J14" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3152558</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>131173</v>
       </c>
       <c r="M14" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>45040</v>
       </c>
       <c r="P14" s="2">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3283731</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3152558</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="C15" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3087668</v>
+      </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3348031</v>
       </c>
       <c r="G15" s="2">
-        <v>47</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I15" s="4">
+        <v>601768</v>
+      </c>
       <c r="J15" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3172155</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>175876</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>44703</v>
       </c>
       <c r="P15" s="2">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3348031</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3172155</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>48</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="C16" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3151930</v>
+      </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3412293</v>
       </c>
       <c r="G16" s="2">
-        <v>48</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I16" s="4">
+        <v>621664</v>
+      </c>
       <c r="J16" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3192051</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>220242</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>44366</v>
       </c>
       <c r="P16" s="2">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3412293</v>
       </c>
       <c r="R16" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3192051</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>49</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="C17" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3216154</v>
+      </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3476517</v>
       </c>
       <c r="G17" s="2">
-        <v>49</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I17" s="4">
+        <v>641859</v>
+      </c>
       <c r="J17" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3212246</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" ref="L17:L18" si="13">E17-J17</f>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>264271</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" ref="M17:M19" si="14">L17-L16</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>44029</v>
       </c>
       <c r="P17" s="2">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" ref="Q17" si="15">C17+D17</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3476517</v>
       </c>
       <c r="R17" s="4">
-        <f t="shared" ref="R17" si="16">H17+I17</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3212246</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>50</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3472670</v>
+      </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3733033</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="H18" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I18" s="4">
+        <v>725629</v>
+      </c>
       <c r="J18" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3296016</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>437017</v>
       </c>
       <c r="M18" s="5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>172746</v>
       </c>
       <c r="P18" s="2">
         <v>50</v>
       </c>
       <c r="Q18" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3733033</v>
       </c>
       <c r="R18" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3296016</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>60</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4111300</v>
+      </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4371663</v>
       </c>
       <c r="G19" s="2">
         <v>60</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="H19" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I19" s="4">
+        <v>955984</v>
+      </c>
       <c r="J19" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3526371</v>
       </c>
       <c r="L19" s="4">
-        <f t="shared" ref="L19" si="17">E19-J19</f>
-        <v>0</v>
+        <f t="shared" ref="L19" si="11">E19-J19</f>
+        <v>845292</v>
       </c>
       <c r="M19" s="5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" ref="M19" si="12">L19-L18</f>
+        <v>408275</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4371663</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3526371</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>70</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4746130</v>
+      </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5006493</v>
       </c>
       <c r="G20" s="2">
         <v>70</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1216239</v>
+      </c>
       <c r="J20" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3786626</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1219867</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>374575</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5006493</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3786626</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>80</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="C21" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5377160</v>
+      </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5637523</v>
       </c>
       <c r="G21" s="2">
         <v>80</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="H21" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1506394</v>
+      </c>
       <c r="J21" s="4">
         <f>H21+I21</f>
-        <v>0</v>
+        <v>4076781</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1560742</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>340875</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5637523</v>
       </c>
       <c r="R21" s="4">
         <f>H21+I21</f>
-        <v>0</v>
+        <v>4076781</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>90</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D22" s="4">
+        <v>6004390</v>
+      </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6264753</v>
       </c>
       <c r="G22" s="2">
         <v>90</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="H22" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1826449</v>
+      </c>
       <c r="J22" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4396836</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1867917</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>307175</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6264753</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4396836</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>100</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="4">
+        <v>260363</v>
+      </c>
+      <c r="D23" s="4">
+        <v>6607674</v>
+      </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6868037</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="H23" s="4">
+        <v>2570387</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2156504</v>
+      </c>
       <c r="J23" s="4">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4726891</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2141146</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>273229</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6868037</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4726891</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 1000 runs data
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB5DA96-755F-468B-87BD-0DC836D1D977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C4783-1835-457C-AB73-16A8329C7A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -1879,10 +1879,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1911,9 +1911,39 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -1921,42 +1951,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>311072</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>583961</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>923651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1301741</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1718231</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2173121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2666411</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3198101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3768191</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4314104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4376681</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4439642</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4502987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4566716</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4630829</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4695326</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4760207</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4825472</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4891121</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4957154</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5003496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2016,10 +2076,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -2048,9 +2108,39 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -2058,42 +2148,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2598283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2673424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2787409</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2933494</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3111679</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3321964</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3564349</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3838834</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4145419</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4448791</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4484104</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4519738</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4555693</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4591969</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4628566</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4665484</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4702723</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4740283</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4778164</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4816366</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4834989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2531,37 +2651,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -2591,67 +2711,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>548729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1140425</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1794255</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2444285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2832479</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2897045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2961573</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3026063</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3090515</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3154929</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3219305</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3283643</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3347943</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3412205</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3476429</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3732945</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>4371575</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5006405</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>5637435</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>6264665</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>6867949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2728,37 +2848,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -2788,67 +2908,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2598269</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2672276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2782911</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2923446</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3022119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3039611</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3057402</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3075492</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3093881</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3112569</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3131556</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3150842</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3170427</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3190311</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3210494</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3294216</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>3524451</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>3784586</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>4074621</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>4394556</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>4724491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5437,10 +5557,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5469,9 +5589,39 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -5479,42 +5629,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$Q$3:$Q$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>311072</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>583961</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>923651</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1301741</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1718231</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2173121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2666411</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3198101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3768191</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4314104</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4376681</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4439642</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4502987</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4566716</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4630829</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4695326</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4760207</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4825472</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4891121</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4957154</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5003496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5560,10 +5740,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$P$3:$P$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5592,9 +5772,39 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>90</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
@@ -5602,42 +5812,72 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$13</c:f>
+              <c:f>'Optimizer | 1000 run - Ascended'!$R$3:$R$23</c:f>
               <c:numCache>
                 <c:formatCode>#,##0</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2598283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2673424</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2787409</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2933494</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3111679</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3321964</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3564349</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3838834</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>4145419</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>4448791</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>4484104</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4519738</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4555693</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4591969</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4628566</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4665484</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4702723</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4740283</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4778164</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4816366</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4834989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6073,37 +6313,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -6133,67 +6373,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>548729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1140425</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1794255</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2444285</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2832479</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2897045</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2961573</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3026063</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3090515</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3154929</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3219305</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3283643</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3347943</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3412205</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3476429</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3732945</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>4371575</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>5006405</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>5637435</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>6264665</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>6867949</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6256,37 +6496,37 @@
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>31</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="9">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="10">
                   <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="11">
                   <c:v>43</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="12">
                   <c:v>44</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="13">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="14">
                   <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>50</c:v>
@@ -6316,67 +6556,67 @@
                 <c:formatCode>#,##0</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2598269</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2672276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2782911</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2923446</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3022119</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>3039611</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3057402</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>3075492</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>3093881</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3112569</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>3131556</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3150842</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>3170427</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>3190311</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>3210494</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>3294216</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>3524451</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>3784586</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>4074621</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>4394556</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>4724491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -19291,7 +19531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06EBE3-BB9C-4874-A95E-FF2651C40304}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -20332,10 +20572,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74871ADF-8F0F-453C-9415-AC73938A5FD8}">
-  <dimension ref="B2:R15"/>
+  <dimension ref="A2:R25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20382,441 +20622,1002 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D3" s="4">
+        <v>50753</v>
+      </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>311072</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I3" s="4">
+        <v>29096</v>
+      </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2598283</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>0</v>
+        <v>-2287211</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>311072</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2598283</v>
       </c>
     </row>
     <row r="4" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D4" s="4">
+        <v>323642</v>
+      </c>
       <c r="E4" s="4">
-        <f t="shared" ref="E4:E13" si="0">C4+D4</f>
-        <v>0</v>
+        <f t="shared" ref="E4:E23" si="0">C4+D4</f>
+        <v>583961</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I4" s="4">
+        <v>104237</v>
+      </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>0</v>
+        <v>2673424</v>
       </c>
       <c r="L4" s="4">
-        <f t="shared" ref="L4:L13" si="1">E4-J4</f>
-        <v>0</v>
+        <f t="shared" ref="L4:L23" si="1">E4-J4</f>
+        <v>-2089463</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>0</v>
+        <v>197748</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
-        <f t="shared" ref="Q4:Q13" si="2">C4+D4</f>
-        <v>0</v>
+        <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
+        <v>583961</v>
       </c>
       <c r="R4" s="4">
-        <f t="shared" ref="R4:R13" si="3">H4+I4</f>
-        <v>0</v>
+        <f t="shared" ref="R4:R23" si="3">H4+I4</f>
+        <v>2673424</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>20</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D5" s="4">
+        <v>663332</v>
+      </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>923651</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I5" s="4">
+        <v>218222</v>
+      </c>
       <c r="J5" s="4">
-        <f t="shared" ref="J5:J13" si="4">H5+I5</f>
-        <v>0</v>
+        <f t="shared" ref="J5:J23" si="4">H5+I5</f>
+        <v>2787409</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1863758</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M10" si="5">L5-L4</f>
-        <v>0</v>
+        <v>225705</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>923651</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2787409</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>30</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D6" s="4">
+        <v>1041422</v>
+      </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1301741</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I6" s="4">
+        <v>364307</v>
+      </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2933494</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1631753</v>
       </c>
       <c r="M6" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>232005</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1301741</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2933494</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>40</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1457912</v>
+      </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1718231</v>
       </c>
       <c r="G7" s="2">
         <v>40</v>
       </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="H7" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I7" s="4">
+        <v>542492</v>
+      </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3111679</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1393448</v>
       </c>
       <c r="M7" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>238305</v>
       </c>
       <c r="P7" s="2">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1718231</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3111679</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>50</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1912802</v>
+      </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2173121</v>
       </c>
       <c r="G8" s="2">
         <v>50</v>
       </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="H8" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I8" s="4">
+        <v>752777</v>
+      </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3321964</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-1148843</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>244605</v>
       </c>
       <c r="P8" s="2">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2173121</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3321964</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>60</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2406092</v>
+      </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2666411</v>
       </c>
       <c r="G9" s="2">
         <v>60</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="H9" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I9" s="4">
+        <v>995162</v>
+      </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3564349</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-897938</v>
       </c>
       <c r="M9" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>250905</v>
       </c>
       <c r="P9" s="2">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2666411</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3564349</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>70</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2937782</v>
+      </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3198101</v>
       </c>
       <c r="G10" s="2">
         <v>70</v>
       </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="H10" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I10" s="4">
+        <v>1269647</v>
+      </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3838834</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-640733</v>
       </c>
       <c r="M10" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>257205</v>
       </c>
       <c r="P10" s="2">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3198101</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3838834</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>80</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3507872</v>
+      </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3768191</v>
       </c>
       <c r="G11" s="2">
         <v>80</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="H11" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I11" s="4">
+        <v>1576232</v>
+      </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4145419</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-377228</v>
       </c>
       <c r="M11" s="5">
         <f>L11-L10</f>
-        <v>0</v>
+        <v>263505</v>
       </c>
       <c r="P11" s="2">
         <v>80</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3768191</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4145419</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
-        <v>90</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="C12" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D12" s="4">
+        <v>4053785</v>
+      </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4314104</v>
       </c>
       <c r="G12" s="2">
-        <v>90</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I12" s="4">
+        <v>1879604</v>
+      </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4448791</v>
       </c>
       <c r="L12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" ref="L12:L22" si="6">E12-J12</f>
+        <v>-134687</v>
       </c>
       <c r="M12" s="5">
-        <f>L12-L11</f>
-        <v>0</v>
+        <f t="shared" ref="M12:M22" si="7">L12-L11</f>
+        <v>242541</v>
       </c>
       <c r="P12" s="2">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="Q12:Q22" si="8">C12+D12</f>
+        <v>4314104</v>
       </c>
       <c r="R12" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="R12:R22" si="9">H12+I12</f>
+        <v>4448791</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>100</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="C13" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D13" s="4">
+        <v>4116362</v>
+      </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4376681</v>
       </c>
       <c r="G13" s="2">
-        <v>100</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I13" s="4">
+        <v>1914917</v>
+      </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4484104</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>-107423</v>
       </c>
       <c r="M13" s="5">
-        <f>L13-L12</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>27264</v>
       </c>
       <c r="P13" s="2">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="Q13" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>4376681</v>
       </c>
       <c r="R13" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>4484104</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-      <c r="R14"/>
+      <c r="B14" s="2">
+        <v>91</v>
+      </c>
+      <c r="C14" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4179323</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>4439642</v>
+      </c>
+      <c r="G14" s="2">
+        <v>91</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I14" s="4">
+        <v>1950551</v>
+      </c>
+      <c r="J14" s="4">
+        <f t="shared" si="4"/>
+        <v>4519738</v>
+      </c>
+      <c r="L14" s="4">
+        <f t="shared" si="6"/>
+        <v>-80096</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="7"/>
+        <v>27327</v>
+      </c>
+      <c r="P14" s="2">
+        <v>91</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="8"/>
+        <v>4439642</v>
+      </c>
+      <c r="R14" s="4">
+        <f t="shared" si="9"/>
+        <v>4519738</v>
+      </c>
     </row>
     <row r="15" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15"/>
-      <c r="E15"/>
-      <c r="F15"/>
-      <c r="G15"/>
+      <c r="B15" s="2">
+        <v>92</v>
+      </c>
+      <c r="C15" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D15" s="4">
+        <v>4242668</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>4502987</v>
+      </c>
+      <c r="G15" s="2">
+        <v>92</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I15" s="4">
+        <v>1986506</v>
+      </c>
+      <c r="J15" s="4">
+        <f t="shared" si="4"/>
+        <v>4555693</v>
+      </c>
+      <c r="L15" s="4">
+        <f t="shared" si="6"/>
+        <v>-52706</v>
+      </c>
+      <c r="M15" s="5">
+        <f t="shared" si="7"/>
+        <v>27390</v>
+      </c>
+      <c r="P15" s="2">
+        <v>92</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="8"/>
+        <v>4502987</v>
+      </c>
+      <c r="R15" s="4">
+        <f t="shared" si="9"/>
+        <v>4555693</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>93</v>
+      </c>
+      <c r="C16" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D16" s="4">
+        <v>4306397</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>4566716</v>
+      </c>
+      <c r="G16" s="2">
+        <v>93</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I16" s="4">
+        <v>2022782</v>
+      </c>
+      <c r="J16" s="4">
+        <f t="shared" si="4"/>
+        <v>4591969</v>
+      </c>
+      <c r="L16" s="4">
+        <f t="shared" si="6"/>
+        <v>-25253</v>
+      </c>
+      <c r="M16" s="5">
+        <f t="shared" si="7"/>
+        <v>27453</v>
+      </c>
+      <c r="P16" s="2">
+        <v>93</v>
+      </c>
+      <c r="Q16" s="4">
+        <f t="shared" si="8"/>
+        <v>4566716</v>
+      </c>
+      <c r="R16" s="4">
+        <f t="shared" si="9"/>
+        <v>4591969</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="2">
+        <v>94</v>
+      </c>
+      <c r="C17" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4370510</v>
+      </c>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>4630829</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="2">
+        <v>94</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I17" s="4">
+        <v>2059379</v>
+      </c>
+      <c r="J17" s="4">
+        <f t="shared" si="4"/>
+        <v>4628566</v>
+      </c>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4">
+        <f t="shared" si="6"/>
+        <v>2263</v>
+      </c>
+      <c r="M17" s="5">
+        <f t="shared" si="7"/>
+        <v>27516</v>
+      </c>
+      <c r="P17" s="2">
+        <v>94</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="8"/>
+        <v>4630829</v>
+      </c>
+      <c r="R17" s="4">
+        <f t="shared" si="9"/>
+        <v>4628566</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>95</v>
+      </c>
+      <c r="C18" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D18" s="4">
+        <v>4435007</v>
+      </c>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>4695326</v>
+      </c>
+      <c r="G18" s="2">
+        <v>95</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I18" s="4">
+        <v>2096297</v>
+      </c>
+      <c r="J18" s="4">
+        <f t="shared" si="4"/>
+        <v>4665484</v>
+      </c>
+      <c r="L18" s="4">
+        <f t="shared" si="6"/>
+        <v>29842</v>
+      </c>
+      <c r="M18" s="5">
+        <f t="shared" si="7"/>
+        <v>27579</v>
+      </c>
+      <c r="P18" s="2">
+        <v>95</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" si="8"/>
+        <v>4695326</v>
+      </c>
+      <c r="R18" s="4">
+        <f t="shared" si="9"/>
+        <v>4665484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>96</v>
+      </c>
+      <c r="C19" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4499888</v>
+      </c>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>4760207</v>
+      </c>
+      <c r="G19" s="2">
+        <v>96</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I19" s="4">
+        <v>2133536</v>
+      </c>
+      <c r="J19" s="4">
+        <f t="shared" si="4"/>
+        <v>4702723</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="6"/>
+        <v>57484</v>
+      </c>
+      <c r="M19" s="5">
+        <f t="shared" si="7"/>
+        <v>27642</v>
+      </c>
+      <c r="P19" s="2">
+        <v>96</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="8"/>
+        <v>4760207</v>
+      </c>
+      <c r="R19" s="4">
+        <f t="shared" si="9"/>
+        <v>4702723</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>97</v>
+      </c>
+      <c r="C20" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4565153</v>
+      </c>
+      <c r="E20" s="4">
+        <f t="shared" si="0"/>
+        <v>4825472</v>
+      </c>
+      <c r="G20" s="2">
+        <v>97</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I20" s="4">
+        <v>2171096</v>
+      </c>
+      <c r="J20" s="4">
+        <f t="shared" si="4"/>
+        <v>4740283</v>
+      </c>
+      <c r="L20" s="4">
+        <f t="shared" si="6"/>
+        <v>85189</v>
+      </c>
+      <c r="M20" s="5">
+        <f t="shared" si="7"/>
+        <v>27705</v>
+      </c>
+      <c r="P20" s="2">
+        <v>97</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" si="8"/>
+        <v>4825472</v>
+      </c>
+      <c r="R20" s="4">
+        <f t="shared" si="9"/>
+        <v>4740283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>98</v>
+      </c>
+      <c r="C21" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D21" s="4">
+        <v>4630802</v>
+      </c>
+      <c r="E21" s="4">
+        <f t="shared" si="0"/>
+        <v>4891121</v>
+      </c>
+      <c r="G21" s="2">
+        <v>98</v>
+      </c>
+      <c r="H21" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I21" s="4">
+        <v>2208977</v>
+      </c>
+      <c r="J21" s="4">
+        <f t="shared" si="4"/>
+        <v>4778164</v>
+      </c>
+      <c r="L21" s="4">
+        <f t="shared" si="6"/>
+        <v>112957</v>
+      </c>
+      <c r="M21" s="5">
+        <f t="shared" si="7"/>
+        <v>27768</v>
+      </c>
+      <c r="P21" s="2">
+        <v>98</v>
+      </c>
+      <c r="Q21" s="4">
+        <f t="shared" si="8"/>
+        <v>4891121</v>
+      </c>
+      <c r="R21" s="4">
+        <f t="shared" si="9"/>
+        <v>4778164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>99</v>
+      </c>
+      <c r="C22" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D22" s="4">
+        <v>4696835</v>
+      </c>
+      <c r="E22" s="4">
+        <f t="shared" si="0"/>
+        <v>4957154</v>
+      </c>
+      <c r="G22" s="2">
+        <v>99</v>
+      </c>
+      <c r="H22" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I22" s="4">
+        <v>2247179</v>
+      </c>
+      <c r="J22" s="4">
+        <f t="shared" si="4"/>
+        <v>4816366</v>
+      </c>
+      <c r="L22" s="4">
+        <f t="shared" si="6"/>
+        <v>140788</v>
+      </c>
+      <c r="M22" s="5">
+        <f t="shared" si="7"/>
+        <v>27831</v>
+      </c>
+      <c r="P22" s="2">
+        <v>99</v>
+      </c>
+      <c r="Q22" s="4">
+        <f t="shared" si="8"/>
+        <v>4957154</v>
+      </c>
+      <c r="R22" s="4">
+        <f t="shared" si="9"/>
+        <v>4816366</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>100</v>
+      </c>
+      <c r="C23" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D23" s="4">
+        <v>4743177</v>
+      </c>
+      <c r="E23" s="4">
+        <f t="shared" si="0"/>
+        <v>5003496</v>
+      </c>
+      <c r="G23" s="2">
+        <v>100</v>
+      </c>
+      <c r="H23" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2265802</v>
+      </c>
+      <c r="J23" s="4">
+        <f t="shared" si="4"/>
+        <v>4834989</v>
+      </c>
+      <c r="L23" s="4">
+        <f t="shared" si="1"/>
+        <v>168507</v>
+      </c>
+      <c r="M23" s="5">
+        <f>L23-L22</f>
+        <v>27719</v>
+      </c>
+      <c r="P23" s="2">
+        <v>100</v>
+      </c>
+      <c r="Q23" s="4">
+        <f t="shared" si="2"/>
+        <v>5003496</v>
+      </c>
+      <c r="R23" s="4">
+        <f t="shared" si="3"/>
+        <v>4834989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+    </row>
+    <row r="25" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L3:L13">
+  <conditionalFormatting sqref="L3:L23">
     <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -20837,8 +21638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20885,818 +21686,986 @@
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D3" s="4">
+        <v>288410</v>
+      </c>
       <c r="E3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>548729</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="H3" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I3" s="4">
+        <v>29082</v>
+      </c>
       <c r="J3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2598269</v>
       </c>
       <c r="L3" s="4">
         <f>E3-J3</f>
-        <v>0</v>
+        <v>-2049540</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
       </c>
       <c r="Q3" s="4">
         <f>C3+D3</f>
-        <v>0</v>
+        <v>548729</v>
       </c>
       <c r="R3" s="4">
         <f>H3+I3</f>
-        <v>0</v>
+        <v>2598269</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>10</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D4" s="4">
+        <v>880106</v>
+      </c>
       <c r="E4" s="4">
         <f t="shared" ref="E4:E23" si="0">C4+D4</f>
-        <v>0</v>
+        <v>1140425</v>
       </c>
       <c r="G4" s="2">
         <v>10</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="H4" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I4" s="4">
+        <v>103089</v>
+      </c>
       <c r="J4" s="4">
         <f>H4+I4</f>
-        <v>0</v>
+        <v>2672276</v>
       </c>
       <c r="L4" s="4">
         <f t="shared" ref="L4:L23" si="1">E4-J4</f>
-        <v>0</v>
+        <v>-1531851</v>
       </c>
       <c r="M4" s="5">
         <f>L4-L3</f>
-        <v>0</v>
+        <v>517689</v>
       </c>
       <c r="P4" s="2">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q23" si="2">C4+D4</f>
-        <v>0</v>
+        <v>1140425</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" ref="R4:R23" si="3">H4+I4</f>
-        <v>0</v>
+        <v>2672276</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>20</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1533936</v>
+      </c>
       <c r="E5" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1794255</v>
       </c>
       <c r="G5" s="2">
         <v>20</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="H5" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I5" s="4">
+        <v>213724</v>
+      </c>
       <c r="J5" s="4">
         <f t="shared" ref="J5:J23" si="4">H5+I5</f>
-        <v>0</v>
+        <v>2782911</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-988656</v>
       </c>
       <c r="M5" s="5">
         <f t="shared" ref="M5:M23" si="5">L5-L4</f>
-        <v>0</v>
+        <v>543195</v>
       </c>
       <c r="P5" s="2">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1794255</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2782911</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>30</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2183966</v>
+      </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2444285</v>
       </c>
       <c r="G6" s="2">
         <v>30</v>
       </c>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="H6" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I6" s="4">
+        <v>354259</v>
+      </c>
       <c r="J6" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2923446</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-479161</v>
       </c>
       <c r="M6" s="5">
         <f>L6-L5</f>
-        <v>0</v>
+        <v>509495</v>
       </c>
       <c r="P6" s="2">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2444285</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2923446</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
-        <v>39</v>
-      </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="C7" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2572160</v>
+      </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2832479</v>
       </c>
       <c r="G7" s="2">
-        <v>39</v>
-      </c>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+        <v>36</v>
+      </c>
+      <c r="H7" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I7" s="4">
+        <v>452932</v>
+      </c>
       <c r="J7" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3022119</v>
       </c>
       <c r="L7" s="4">
-        <f t="shared" ref="L7:L8" si="6">E7-J7</f>
-        <v>0</v>
+        <f t="shared" ref="L7:L10" si="6">E7-J7</f>
+        <v>-189640</v>
       </c>
       <c r="M7" s="5">
-        <f t="shared" ref="M7:M8" si="7">L7-L6</f>
-        <v>0</v>
+        <f t="shared" ref="M7:M10" si="7">L7-L6</f>
+        <v>289521</v>
       </c>
       <c r="P7" s="2">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="Q7" s="4">
-        <f t="shared" ref="Q7" si="8">C7+D7</f>
-        <v>0</v>
+        <f t="shared" ref="Q7:Q10" si="8">C7+D7</f>
+        <v>2832479</v>
       </c>
       <c r="R7" s="4">
-        <f t="shared" ref="R7" si="9">H7+I7</f>
-        <v>0</v>
+        <f t="shared" ref="R7:R10" si="9">H7+I7</f>
+        <v>3022119</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
-        <v>40</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="C8" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D8" s="4">
+        <v>2636726</v>
+      </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2897045</v>
       </c>
       <c r="G8" s="2">
-        <v>40</v>
-      </c>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+        <v>37</v>
+      </c>
+      <c r="H8" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I8" s="4">
+        <v>470424</v>
+      </c>
       <c r="J8" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3039611</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-142566</v>
       </c>
       <c r="M8" s="5">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>47074</v>
       </c>
       <c r="P8" s="2">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="Q8" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2897045</v>
       </c>
       <c r="R8" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>3039611</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
-        <v>41</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="C9" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2701254</v>
+      </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2961573</v>
       </c>
       <c r="G9" s="2">
-        <v>41</v>
-      </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+        <v>38</v>
+      </c>
+      <c r="H9" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I9" s="4">
+        <v>488215</v>
+      </c>
       <c r="J9" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3057402</v>
       </c>
       <c r="L9" s="4">
-        <f>E9-J9</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>-95829</v>
       </c>
       <c r="M9" s="5">
-        <f>L9-L8</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46737</v>
       </c>
       <c r="P9" s="2">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="Q9" s="4">
-        <f t="shared" ref="Q9" si="10">C9+D9</f>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>2961573</v>
       </c>
       <c r="R9" s="4">
-        <f t="shared" ref="R9" si="11">H9+I9</f>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>3057402</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
-        <v>42</v>
-      </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="C10" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2765744</v>
+      </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3026063</v>
       </c>
       <c r="G10" s="2">
-        <v>42</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="H10" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I10" s="4">
+        <v>506305</v>
+      </c>
       <c r="J10" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3075492</v>
       </c>
       <c r="L10" s="4">
-        <f t="shared" ref="L10" si="12">E10-J10</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>-49429</v>
       </c>
       <c r="M10" s="5">
-        <f>L10-L9</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>46400</v>
       </c>
       <c r="P10" s="2">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="Q10" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>3026063</v>
       </c>
       <c r="R10" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="9"/>
+        <v>3075492</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
-        <v>43</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C11" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2830196</v>
+      </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3090515</v>
       </c>
       <c r="G11" s="2">
-        <v>43</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="H11" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I11" s="4">
+        <v>524694</v>
+      </c>
       <c r="J11" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3093881</v>
       </c>
       <c r="L11" s="4">
-        <f t="shared" ref="L11" si="13">E11-J11</f>
-        <v>0</v>
+        <f t="shared" ref="L10:L11" si="10">E11-J11</f>
+        <v>-3366</v>
       </c>
       <c r="M11" s="5">
-        <f t="shared" ref="M11:M15" si="14">L11-L10</f>
-        <v>0</v>
+        <f t="shared" ref="M11" si="11">L11-L10</f>
+        <v>46063</v>
       </c>
       <c r="P11" s="2">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3090515</v>
       </c>
       <c r="R11" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3093881</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
       <c r="B12" s="2">
-        <v>44</v>
-      </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="C12" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D12" s="4">
+        <v>2894610</v>
+      </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3154929</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2">
-        <v>44</v>
-      </c>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+        <v>41</v>
+      </c>
+      <c r="H12" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I12" s="4">
+        <v>543382</v>
+      </c>
       <c r="J12" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3112569</v>
       </c>
       <c r="K12" s="6"/>
       <c r="L12" s="4">
-        <f t="shared" ref="L12" si="15">E12-J12</f>
-        <v>0</v>
+        <f>E12-J12</f>
+        <v>42360</v>
       </c>
       <c r="M12" s="5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>L12-L11</f>
+        <v>45726</v>
       </c>
       <c r="P12" s="2">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="Q12" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" ref="Q12" si="12">C12+D12</f>
+        <v>3154929</v>
       </c>
       <c r="R12" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" ref="R12" si="13">H12+I12</f>
+        <v>3112569</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
-        <v>45</v>
-      </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="C13" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D13" s="4">
+        <v>2958986</v>
+      </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3219305</v>
       </c>
       <c r="G13" s="2">
-        <v>45</v>
-      </c>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="H13" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I13" s="4">
+        <v>562369</v>
+      </c>
       <c r="J13" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3131556</v>
       </c>
       <c r="L13" s="4">
-        <f t="shared" ref="L13" si="16">E13-J13</f>
-        <v>0</v>
+        <f t="shared" ref="L13" si="14">E13-J13</f>
+        <v>87749</v>
       </c>
       <c r="M13" s="5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>L13-L12</f>
+        <v>45389</v>
       </c>
       <c r="P13" s="2">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q13" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3219305</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3131556</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
-        <v>46</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="C14" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3023324</v>
+      </c>
       <c r="E14" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3283643</v>
       </c>
       <c r="G14" s="2">
-        <v>46</v>
-      </c>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I14" s="4">
+        <v>581655</v>
+      </c>
       <c r="J14" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3150842</v>
       </c>
       <c r="L14" s="4">
-        <f t="shared" ref="L14:L16" si="17">E14-J14</f>
-        <v>0</v>
+        <f t="shared" ref="L14" si="15">E14-J14</f>
+        <v>132801</v>
       </c>
       <c r="M14" s="5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" ref="M14:M17" si="16">L14-L13</f>
+        <v>45052</v>
       </c>
       <c r="P14" s="2">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3283643</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3150842</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
-        <v>47</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="C15" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3087624</v>
+      </c>
       <c r="E15" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3347943</v>
       </c>
       <c r="G15" s="2">
-        <v>47</v>
-      </c>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+        <v>44</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I15" s="4">
+        <v>601240</v>
+      </c>
       <c r="J15" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3170427</v>
       </c>
       <c r="L15" s="4">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" ref="L15" si="17">E15-J15</f>
+        <v>177516</v>
       </c>
       <c r="M15" s="5">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>44715</v>
       </c>
       <c r="P15" s="2">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3347943</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3170427</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
-        <v>48</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="C16" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3151886</v>
+      </c>
       <c r="E16" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3412205</v>
       </c>
       <c r="G16" s="2">
-        <v>48</v>
-      </c>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I16" s="4">
+        <v>621124</v>
+      </c>
       <c r="J16" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3190311</v>
       </c>
       <c r="L16" s="4">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f t="shared" ref="L16" si="18">E16-J16</f>
+        <v>221894</v>
       </c>
       <c r="M16" s="5">
-        <f t="shared" ref="M16" si="18">L16-L12</f>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>44378</v>
       </c>
       <c r="P16" s="2">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="Q16" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3412205</v>
       </c>
       <c r="R16" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3190311</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
-        <v>49</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="C17" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3216110</v>
+      </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3476429</v>
       </c>
       <c r="G17" s="2">
-        <v>49</v>
-      </c>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
+        <v>46</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I17" s="4">
+        <v>641307</v>
+      </c>
       <c r="J17" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3210494</v>
       </c>
       <c r="L17" s="4">
-        <f t="shared" ref="L17:L18" si="19">E17-J17</f>
-        <v>0</v>
+        <f t="shared" ref="L17" si="19">E17-J17</f>
+        <v>265935</v>
       </c>
       <c r="M17" s="5">
-        <f t="shared" ref="M17:M18" si="20">L17-L13</f>
-        <v>0</v>
+        <f t="shared" si="16"/>
+        <v>44041</v>
       </c>
       <c r="P17" s="2">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q17" s="4">
-        <f t="shared" ref="Q17:Q18" si="21">C17+D17</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>3476429</v>
       </c>
       <c r="R17" s="4">
-        <f t="shared" ref="R17:R18" si="22">H17+I17</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>3210494</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>50</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="C18" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3472626</v>
+      </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3732945</v>
       </c>
       <c r="G18" s="2">
         <v>50</v>
       </c>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
+      <c r="H18" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I18" s="4">
+        <v>725029</v>
+      </c>
       <c r="J18" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3294216</v>
       </c>
       <c r="L18" s="4">
-        <f t="shared" si="19"/>
-        <v>0</v>
+        <f t="shared" ref="L18" si="20">E18-J18</f>
+        <v>438729</v>
       </c>
       <c r="M18" s="5">
-        <f t="shared" si="20"/>
-        <v>0</v>
+        <f>L18-L17</f>
+        <v>172794</v>
       </c>
       <c r="P18" s="2">
         <v>50</v>
       </c>
       <c r="Q18" s="4">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" ref="Q18" si="21">C18+D18</f>
+        <v>3732945</v>
       </c>
       <c r="R18" s="4">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" ref="R18" si="22">H18+I18</f>
+        <v>3294216</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>60</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D19" s="4">
+        <v>4111256</v>
+      </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4371575</v>
       </c>
       <c r="G19" s="2">
         <v>60</v>
       </c>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
+      <c r="H19" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I19" s="4">
+        <v>955264</v>
+      </c>
       <c r="J19" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3524451</v>
       </c>
       <c r="L19" s="4">
         <f t="shared" ref="L19" si="23">E19-J19</f>
-        <v>0</v>
+        <v>847124</v>
       </c>
       <c r="M19" s="5">
-        <f>L19-L16</f>
-        <v>0</v>
+        <f>L19-L18</f>
+        <v>408395</v>
       </c>
       <c r="P19" s="2">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4371575</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3524451</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>70</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D20" s="4">
+        <v>4746086</v>
+      </c>
       <c r="E20" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5006405</v>
       </c>
       <c r="G20" s="2">
         <v>70</v>
       </c>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
+      <c r="H20" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I20" s="4">
+        <v>1215399</v>
+      </c>
       <c r="J20" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3784586</v>
       </c>
       <c r="L20" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1221819</v>
       </c>
       <c r="M20" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>374695</v>
       </c>
       <c r="P20" s="2">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5006405</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3784586</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>80</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="C21" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D21" s="4">
+        <v>5377116</v>
+      </c>
       <c r="E21" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5637435</v>
       </c>
       <c r="G21" s="2">
         <v>80</v>
       </c>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
+      <c r="H21" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I21" s="4">
+        <v>1505434</v>
+      </c>
       <c r="J21" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4074621</v>
       </c>
       <c r="L21" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1562814</v>
       </c>
       <c r="M21" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>340995</v>
       </c>
       <c r="P21" s="2">
         <v>80</v>
       </c>
       <c r="Q21" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5637435</v>
       </c>
       <c r="R21" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4074621</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>90</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D22" s="4">
+        <v>6004346</v>
+      </c>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6264665</v>
       </c>
       <c r="G22" s="2">
         <v>90</v>
       </c>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="H22" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I22" s="4">
+        <v>1825369</v>
+      </c>
       <c r="J22" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4394556</v>
       </c>
       <c r="L22" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1870109</v>
       </c>
       <c r="M22" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>307295</v>
       </c>
       <c r="P22" s="2">
         <v>90</v>
       </c>
       <c r="Q22" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6264665</v>
       </c>
       <c r="R22" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4394556</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>100</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="4">
+        <v>260319</v>
+      </c>
+      <c r="D23" s="4">
+        <v>6607630</v>
+      </c>
       <c r="E23" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6867949</v>
       </c>
       <c r="G23" s="2">
         <v>100</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
+      <c r="H23" s="4">
+        <v>2569187</v>
+      </c>
+      <c r="I23" s="4">
+        <v>2155304</v>
+      </c>
       <c r="J23" s="4">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4724491</v>
       </c>
       <c r="L23" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2143458</v>
       </c>
       <c r="M23" s="5">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>273349</v>
       </c>
       <c r="P23" s="2">
         <v>100</v>
       </c>
       <c r="Q23" s="4">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6867949</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4724491</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add forgotten data of 200 runs descended
</commit_message>
<xml_diff>
--- a/docs/data/Break even ERC721A and ERC721F.xlsx
+++ b/docs/data/Break even ERC721A and ERC721F.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hans_\OneDrive\Bureaublad\School\2022-2023\Stage\Contracts\ERC721F\docs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910C4783-1835-457C-AB73-16A8329C7A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6131BDB8-EBC3-4F35-9744-80D8CD45CF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
+    <workbookView xWindow="28680" yWindow="-5520" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="6" xr2:uid="{BE095514-5817-46A1-BEFE-93A077CD51C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Optimizer Disabled - Ascended" sheetId="1" r:id="rId1"/>
@@ -1226,6 +1226,15 @@
                 <c:pt idx="3">
                   <c:v>2444373</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>2832567</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2897133</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2961661</c:v>
+                </c:pt>
                 <c:pt idx="7">
                   <c:v>3026151</c:v>
                 </c:pt>
@@ -4919,6 +4928,15 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2444373</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2832567</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2897133</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2961661</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3026151</c:v>
@@ -19531,8 +19549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA06EBE3-BB9C-4874-A95E-FF2651C40304}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -19797,7 +19815,10 @@
       <c r="P7" s="2">
         <v>36</v>
       </c>
-      <c r="Q7" s="4"/>
+      <c r="Q7" s="4">
+        <f t="shared" si="2"/>
+        <v>2832567</v>
+      </c>
       <c r="R7" s="4">
         <f t="shared" si="3"/>
         <v>3023751</v>
@@ -19841,7 +19862,10 @@
       <c r="P8" s="2">
         <v>37</v>
       </c>
-      <c r="Q8" s="4"/>
+      <c r="Q8" s="4">
+        <f t="shared" si="2"/>
+        <v>2897133</v>
+      </c>
       <c r="R8" s="4">
         <f t="shared" si="3"/>
         <v>3041255</v>
@@ -19885,7 +19909,10 @@
       <c r="P9" s="2">
         <v>38</v>
       </c>
-      <c r="Q9" s="4"/>
+      <c r="Q9" s="4">
+        <f t="shared" si="2"/>
+        <v>2961661</v>
+      </c>
       <c r="R9" s="4">
         <f t="shared" si="3"/>
         <v>3059058</v>
@@ -21638,7 +21665,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F48680-259D-4EBA-A24F-AE9EC86DE4E8}">
   <dimension ref="A2:R23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
@@ -22690,8 +22717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D91734A6-3CBC-46E0-AC2D-961E5CB62031}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="35.1" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>